<commit_message>
moving hard coded overview table to yaml
</commit_message>
<xml_diff>
--- a/Documentation/IEA-15-240-RWT_tabular.xlsx
+++ b/Documentation/IEA-15-240-RWT_tabular.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gbarter/systems/referenceTurbines/15mw/IEA-15-240-RWT/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B59F8CE8-DAAA-B34C-B360-8B373700D97B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA72126C-A6F6-104C-AEC4-42C7A87A6377}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11060" yWindow="500" windowWidth="39000" windowHeight="23620" firstSheet="4" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17500" yWindow="500" windowWidth="32560" windowHeight="23220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="200">
   <si>
     <t>Parameter</t>
   </si>
@@ -105,9 +105,6 @@
     <t>Hub Overhang [m]</t>
   </si>
   <si>
-    <t>TODO??</t>
-  </si>
-  <si>
     <t>Drive train</t>
   </si>
   <si>
@@ -133,12 +130,6 @@
   </si>
   <si>
     <t>Tower top to nacelle (yaw bearing height) [m]</t>
-  </si>
-  <si>
-    <t>Tower top to shaft distnace [m]</t>
-  </si>
-  <si>
-    <t>Overhang [m]</t>
   </si>
   <si>
     <t>Generator efficiency [%]</t>
@@ -184,9 +175,6 @@
   </si>
   <si>
     <t>Nacellem center of mass from tower top [m]</t>
-  </si>
-  <si>
-    <t>[-5.019, 0.0, 3.161]</t>
   </si>
   <si>
     <t>Tower mass [t]</t>
@@ -650,6 +638,12 @@
   <si>
     <t>Torque [MNm]</t>
   </si>
+  <si>
+    <t>Tower top to shaft distance [m]</t>
+  </si>
+  <si>
+    <t>[-1.06144039, 0.0, 0.8916053]</t>
+  </si>
 </sst>
 </file>
 
@@ -728,11 +722,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Heading 1" xfId="2" builtinId="16"/>
@@ -1038,10 +1033,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1166,21 +1161,21 @@
       <c r="A15" t="s">
         <v>19</v>
       </c>
-      <c r="B15" t="s">
-        <v>20</v>
+      <c r="B15">
+        <v>-10.454000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
         <v>21</v>
-      </c>
-      <c r="B16" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17">
         <v>9</v>
@@ -1188,7 +1183,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18">
         <v>5</v>
@@ -1196,7 +1191,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19">
         <v>7.6</v>
@@ -1204,7 +1199,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20">
         <v>95</v>
@@ -1212,7 +1207,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B21">
         <v>6</v>
@@ -1220,7 +1215,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B22">
         <v>-4</v>
@@ -1228,7 +1223,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B23">
         <v>0.38500000000000001</v>
@@ -1236,7 +1231,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>198</v>
       </c>
       <c r="B24">
         <v>2.927</v>
@@ -1244,178 +1239,170 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B25">
-        <v>-10.454000000000001</v>
+        <v>96.55</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B26">
-        <v>96.55</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B27">
-        <v>4</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B28">
-        <v>68</v>
+        <v>188</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B29">
-        <v>188</v>
+        <v>371.95</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>36</v>
-      </c>
-      <c r="B30">
-        <v>371.95</v>
+        <v>34</v>
+      </c>
+      <c r="B30" s="4">
+        <v>12.946999999999999</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>37</v>
-      </c>
-      <c r="B31">
-        <v>12.946999999999999</v>
+        <v>35</v>
+      </c>
+      <c r="B31" s="4">
+        <v>49.999000000000002</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>38</v>
-      </c>
-      <c r="B32">
-        <v>49.999000000000002</v>
+        <v>36</v>
+      </c>
+      <c r="B32" s="4">
+        <v>19.504000000000001</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>39</v>
-      </c>
-      <c r="B33">
-        <v>19.504000000000001</v>
+        <v>37</v>
+      </c>
+      <c r="B33" s="4">
+        <v>4.6989999999999998</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>40</v>
-      </c>
-      <c r="B34">
-        <v>4.6989999999999998</v>
+        <v>38</v>
+      </c>
+      <c r="B34" s="4">
+        <v>1.7390000000000001</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B35">
-        <v>1.7390000000000001</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B36">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>43</v>
-      </c>
-      <c r="B37">
-        <v>50</v>
+        <v>41</v>
+      </c>
+      <c r="B37" s="4">
+        <v>615.53700000000003</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>44</v>
-      </c>
-      <c r="B38">
-        <v>615.53700000000003</v>
+        <v>42</v>
+      </c>
+      <c r="B38" s="4">
+        <v>1007.537</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>45</v>
-      </c>
-      <c r="B39">
-        <v>1007.537</v>
+        <v>43</v>
+      </c>
+      <c r="B39" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>46</v>
-      </c>
-      <c r="B40" t="s">
-        <v>47</v>
+        <v>44</v>
+      </c>
+      <c r="B40" s="4">
+        <v>922.58745611328004</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>48</v>
-      </c>
-      <c r="B41" t="s">
-        <v>20</v>
+        <v>45</v>
+      </c>
+      <c r="B41">
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B42">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B43">
-        <v>20</v>
+        <v>45</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B44">
-        <v>45</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>52</v>
-      </c>
-      <c r="B45">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>53</v>
-      </c>
-      <c r="B46" t="s">
-        <v>20</v>
+        <v>49</v>
+      </c>
+      <c r="B45" s="4">
+        <v>2319.41429420043</v>
       </c>
     </row>
   </sheetData>
@@ -1454,55 +1441,55 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -3120,46 +3107,46 @@
   <sheetData>
     <row r="1" spans="1:6" ht="20" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="20" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -3176,10 +3163,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -3196,10 +3183,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B6" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C6">
         <v>0.50001289063000232</v>
@@ -3216,10 +3203,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B7" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -3236,10 +3223,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -3256,10 +3243,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B9" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C9">
         <v>0.23252544225630681</v>
@@ -3276,10 +3263,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B10" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C10">
         <v>0.50001289063000232</v>
@@ -3296,10 +3283,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B11" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C11">
         <v>0.73592131634778191</v>
@@ -3316,10 +3303,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B12" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -3336,10 +3323,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B13" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C13">
         <v>0.1773648601567597</v>
@@ -3356,10 +3343,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B14" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C14">
         <v>0.6807607342482348</v>
@@ -3376,46 +3363,46 @@
     </row>
     <row r="17" spans="1:6" ht="20" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="20" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B20" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -3432,10 +3419,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B21" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -3452,10 +3439,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B22" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C22">
         <v>0.50001289063000176</v>
@@ -3472,10 +3459,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B23" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -3492,10 +3479,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B24" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -3512,10 +3499,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B25" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C25">
         <v>0.2368455686217322</v>
@@ -3532,10 +3519,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B26" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C26">
         <v>0.50001289063000176</v>
@@ -3552,10 +3539,10 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B27" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C27">
         <v>0.73153319648678317</v>
@@ -3572,10 +3559,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B28" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -3592,10 +3579,10 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B29" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C29">
         <v>0.18177268004700201</v>
@@ -3612,10 +3599,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B30" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C30">
         <v>0.67646030791205281</v>
@@ -3632,46 +3619,46 @@
     </row>
     <row r="33" spans="1:6" ht="20" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B33" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="20" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="F35" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B36" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -3688,10 +3675,10 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B37" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -3708,10 +3695,10 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B38" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C38">
         <v>0.47095842037511282</v>
@@ -3728,10 +3715,10 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B39" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C39">
         <v>0.96312247015924091</v>
@@ -3748,10 +3735,10 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B40" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C40">
         <v>3.6877529840759128E-2</v>
@@ -3768,10 +3755,10 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B41" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C41">
         <v>0.30044648254180312</v>
@@ -3788,10 +3775,10 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B42" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C42">
         <v>0.52996246812032755</v>
@@ -3808,10 +3795,10 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B43" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C43">
         <v>0.72632761344713592</v>
@@ -3828,10 +3815,10 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B44" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -3848,10 +3835,10 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B45" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C45">
         <v>0.23406692882843649</v>
@@ -3868,10 +3855,10 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B46" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C46">
         <v>0.65994805973376935</v>
@@ -3888,46 +3875,46 @@
     </row>
     <row r="49" spans="1:6" ht="20" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B49" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="20" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E51" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="F51" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B52" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -3944,10 +3931,10 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B53" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -3964,10 +3951,10 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B54" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C54">
         <v>0.46840764019255909</v>
@@ -3984,10 +3971,10 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B55" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C55">
         <v>0.96120237793118535</v>
@@ -4004,10 +3991,10 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B56" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C56">
         <v>3.8797622068814652E-2</v>
@@ -4024,10 +4011,10 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B57" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C57">
         <v>0.33969780513475811</v>
@@ -4044,10 +4031,10 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B58" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C58">
         <v>0.53048383550266243</v>
@@ -4064,10 +4051,10 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B59" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C59">
         <v>0.70662405728543753</v>
@@ -4084,10 +4071,10 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B60" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C60">
         <v>0</v>
@@ -4104,10 +4091,10 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B61" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C61">
         <v>0.26986208541089179</v>
@@ -4124,10 +4111,10 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B62" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C62">
         <v>0.63678833756157127</v>
@@ -4144,46 +4131,46 @@
     </row>
     <row r="65" spans="1:6" ht="20" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B65" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="20" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E67" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="F67" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B68" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C68">
         <v>0</v>
@@ -4200,10 +4187,10 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B69" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C69">
         <v>0</v>
@@ -4220,10 +4207,10 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B70" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C70">
         <v>0.45911697376462302</v>
@@ -4240,10 +4227,10 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B71" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C71">
         <v>0.95094061457450352</v>
@@ -4260,10 +4247,10 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B72" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C72">
         <v>4.9059385425496593E-2</v>
@@ -4280,10 +4267,10 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B73" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C73">
         <v>0.37460892707854732</v>
@@ -4300,10 +4287,10 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B74" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C74">
         <v>0.53761199044541741</v>
@@ -4320,10 +4307,10 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B75" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C75">
         <v>0.70302297234198696</v>
@@ -4340,10 +4327,10 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B76" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C76">
         <v>0</v>
@@ -4360,10 +4347,10 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B77" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C77">
         <v>0.2863020333126533</v>
@@ -4380,10 +4367,10 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B78" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C78">
         <v>0.61471607857609312</v>
@@ -4400,46 +4387,46 @@
     </row>
     <row r="81" spans="1:6" ht="20" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B81" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="20" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E83" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="F83" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F83" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B84" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C84">
         <v>0</v>
@@ -4456,10 +4443,10 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B85" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C85">
         <v>0</v>
@@ -4476,10 +4463,10 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B86" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C86">
         <v>0.44732732883666698</v>
@@ -4496,10 +4483,10 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B87" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C87">
         <v>0.93287724567055574</v>
@@ -4516,10 +4503,10 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B88" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C88">
         <v>6.7122754329444367E-2</v>
@@ -4536,10 +4523,10 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B89" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C89">
         <v>0.40162736717333247</v>
@@ -4556,10 +4543,10 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B90" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C90">
         <v>0.55472373576377776</v>
@@ -4576,10 +4563,10 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B91" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C91">
         <v>0.71639013344777758</v>
@@ -4596,10 +4583,10 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B92" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C92">
         <v>0</v>
@@ -4616,10 +4603,10 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B93" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C93">
         <v>0.28080640938033269</v>
@@ -4636,10 +4623,10 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B94" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C94">
         <v>0.59556917565477796</v>
@@ -4656,46 +4643,46 @@
     </row>
     <row r="97" spans="1:6" ht="20" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B97" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="20" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="99" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E99" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="F99" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E99" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F99" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B100" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C100">
         <v>0</v>
@@ -4712,10 +4699,10 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B101" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C101">
         <v>0</v>
@@ -4732,10 +4719,10 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B102" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C102">
         <v>0.4380108749928659</v>
@@ -4752,10 +4739,10 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B103" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C103">
         <v>0.91154023768039605</v>
@@ -4772,10 +4759,10 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B104" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C104">
         <v>8.8459762319603952E-2</v>
@@ -4792,10 +4779,10 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B105" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C105">
         <v>0.41718194473734682</v>
@@ -4812,10 +4799,10 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B106" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C106">
         <v>0.56823460613765442</v>
@@ -4832,10 +4819,10 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B107" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C107">
         <v>0.7435825246439598</v>
@@ -4852,10 +4839,10 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B108" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C108">
         <v>0</v>
@@ -4872,10 +4859,10 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B109" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C109">
         <v>0.25795437256205972</v>
@@ -4892,10 +4879,10 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B110" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C110">
         <v>0.58435495246867275</v>
@@ -4912,46 +4899,46 @@
     </row>
     <row r="113" spans="1:6" ht="20" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B113" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="114" spans="1:6" ht="20" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="115" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E115" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B115" s="1" t="s">
+      <c r="F115" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E115" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F115" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B116" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C116">
         <v>0</v>
@@ -4968,10 +4955,10 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B117" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C117">
         <v>0</v>
@@ -4988,10 +4975,10 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B118" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C118">
         <v>0.50558293872451976</v>
@@ -5008,10 +4995,10 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B119" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C119">
         <v>1</v>
@@ -5028,10 +5015,10 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B120" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C120">
         <v>1</v>
@@ -5048,10 +5035,10 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B121" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C121">
         <v>0.4447325597001473</v>
@@ -5068,10 +5055,10 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B122" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C122">
         <v>0.50558293872451976</v>
@@ -5088,10 +5075,10 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B123" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C123">
         <v>0.82458688369620969</v>
@@ -5108,10 +5095,10 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B124" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C124">
         <v>0</v>
@@ -5128,10 +5115,10 @@
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B125" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C125">
         <v>0.18091424072331</v>
@@ -5148,10 +5135,10 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B126" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C126">
         <v>0.56076856471937242</v>
@@ -5190,112 +5177,112 @@
   <sheetData>
     <row r="1" spans="1:5" ht="20" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="20" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="20" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="20" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="20" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="20" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B14" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C14" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D14">
         <v>1.911764705882353</v>
@@ -5306,13 +5293,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B15" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C15" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D15">
         <v>1.911764705882353</v>
@@ -5323,13 +5310,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B16" t="s">
         <v>130</v>
       </c>
-      <c r="B16" t="s">
-        <v>134</v>
-      </c>
       <c r="C16" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D16">
         <v>40.764705882352942</v>
@@ -5340,13 +5327,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B17" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C17" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D17">
         <v>1.911764705882353</v>
@@ -5357,13 +5344,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B18" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C18" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D18">
         <v>1.911764705882353</v>
@@ -5374,13 +5361,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>126</v>
+      </c>
+      <c r="B19" t="s">
         <v>130</v>
       </c>
-      <c r="B19" t="s">
-        <v>134</v>
-      </c>
       <c r="C19" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D19">
         <v>40.764705882352942</v>
@@ -5391,13 +5378,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B20" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C20" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D20">
         <v>40.764705882352942</v>
@@ -5408,13 +5395,13 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B21" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C21" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D21">
         <v>1.911764705882353</v>
@@ -5425,13 +5412,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B22" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C22" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D22">
         <v>1.911764705882353</v>
@@ -5442,13 +5429,13 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B23" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C23" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D23">
         <v>40.764705882352942</v>
@@ -5459,13 +5446,13 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B24" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C24" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D24">
         <v>1.911764705882353</v>
@@ -5476,13 +5463,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B25" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C25" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D25">
         <v>1.911764705882353</v>
@@ -5493,46 +5480,46 @@
     </row>
     <row r="28" spans="1:5" ht="20" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B28" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="20" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B31" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C31" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D31">
         <v>1.743817088078246</v>
@@ -5543,13 +5530,13 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B32" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C32" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D32">
         <v>1.743817088078246</v>
@@ -5560,13 +5547,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>126</v>
+      </c>
+      <c r="B33" t="s">
         <v>130</v>
       </c>
-      <c r="B33" t="s">
-        <v>134</v>
-      </c>
       <c r="C33" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D33">
         <v>36.5100328979822</v>
@@ -5577,13 +5564,13 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B34" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C34" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D34">
         <v>1.743817088078246</v>
@@ -5594,13 +5581,13 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B35" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C35" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D35">
         <v>1.743817088078246</v>
@@ -5611,13 +5598,13 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>126</v>
+      </c>
+      <c r="B36" t="s">
         <v>130</v>
       </c>
-      <c r="B36" t="s">
-        <v>134</v>
-      </c>
       <c r="C36" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D36">
         <v>36.5100328979822</v>
@@ -5628,13 +5615,13 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B37" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C37" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D37">
         <v>36.5100328979822</v>
@@ -5645,13 +5632,13 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B38" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C38" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D38">
         <v>1.743817088078246</v>
@@ -5662,13 +5649,13 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B39" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C39" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D39">
         <v>1.743817088078246</v>
@@ -5679,13 +5666,13 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B40" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C40" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D40">
         <v>36.5100328979822</v>
@@ -5696,13 +5683,13 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B41" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C41" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D41">
         <v>1.743817088078246</v>
@@ -5713,13 +5700,13 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B42" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C42" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D42">
         <v>1.743817088078246</v>
@@ -5730,13 +5717,13 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B43" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C43" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D43">
         <v>1.887074208110848</v>
@@ -5747,13 +5734,13 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B44" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C44" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D44">
         <v>37.741484162216963</v>
@@ -5764,13 +5751,13 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B45" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C45" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D45">
         <v>1.887074208110848</v>
@@ -5781,13 +5768,13 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B46" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C46" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D46">
         <v>37.741484162216963</v>
@@ -5798,13 +5785,13 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B47" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C47" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D47">
         <v>1.887074208110848</v>
@@ -5815,13 +5802,13 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B48" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C48" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D48">
         <v>1.887074208110848</v>
@@ -5832,46 +5819,46 @@
     </row>
     <row r="51" spans="1:5" ht="20" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B51" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="20" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B53" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="E53" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B54" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C54" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D54">
         <v>1.401448212154266</v>
@@ -5882,13 +5869,13 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B55" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C55" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D55">
         <v>1.401448212154266</v>
@@ -5899,13 +5886,13 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
+        <v>126</v>
+      </c>
+      <c r="B56" t="s">
         <v>130</v>
       </c>
-      <c r="B56" t="s">
-        <v>134</v>
-      </c>
       <c r="C56" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D56">
         <v>27.836688041241398</v>
@@ -5916,13 +5903,13 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B57" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C57" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D57">
         <v>1.401448212154266</v>
@@ -5933,13 +5920,13 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B58" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C58" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D58">
         <v>1.401448212154266</v>
@@ -5950,13 +5937,13 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
+        <v>126</v>
+      </c>
+      <c r="B59" t="s">
         <v>130</v>
       </c>
-      <c r="B59" t="s">
-        <v>134</v>
-      </c>
       <c r="C59" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D59">
         <v>27.836688041241398</v>
@@ -5967,13 +5954,13 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B60" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C60" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D60">
         <v>27.836688041241398</v>
@@ -5984,13 +5971,13 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B61" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C61" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D61">
         <v>1.401448212154266</v>
@@ -6001,13 +5988,13 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B62" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C62" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D62">
         <v>1.401448212154266</v>
@@ -6018,13 +6005,13 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B63" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C63" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D63">
         <v>27.836688041241398</v>
@@ -6035,13 +6022,13 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B64" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C64" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D64">
         <v>1.401448212154266</v>
@@ -6052,13 +6039,13 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B65" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C65" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D65">
         <v>1.401448212154266</v>
@@ -6069,13 +6056,13 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B66" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C66" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D66">
         <v>1.40205163388521</v>
@@ -6086,13 +6073,13 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B67" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C67" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D67">
         <v>28.041032677704202</v>
@@ -6103,13 +6090,13 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B68" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C68" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D68">
         <v>1.40205163388521</v>
@@ -6120,13 +6107,13 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B69" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C69" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D69">
         <v>28.041032677704202</v>
@@ -6137,13 +6124,13 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B70" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C70" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D70">
         <v>1.40205163388521</v>
@@ -6154,13 +6141,13 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B71" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C71" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D71">
         <v>1.40205163388521</v>
@@ -6171,46 +6158,46 @@
     </row>
     <row r="74" spans="1:5" ht="20" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B74" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="20" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B76" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D76" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="E76" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B77" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C77" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D77">
         <v>1.050221781912281</v>
@@ -6221,13 +6208,13 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B78" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C78" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D78">
         <v>1.050221781912281</v>
@@ -6238,13 +6225,13 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
+        <v>126</v>
+      </c>
+      <c r="B79" t="s">
         <v>130</v>
       </c>
-      <c r="B79" t="s">
-        <v>134</v>
-      </c>
       <c r="C79" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D79">
         <v>18.938951808444461</v>
@@ -6255,13 +6242,13 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B80" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C80" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D80">
         <v>1.050221781912281</v>
@@ -6272,13 +6259,13 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B81" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C81" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D81">
         <v>1.050221781912281</v>
@@ -6289,13 +6276,13 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
+        <v>126</v>
+      </c>
+      <c r="B82" t="s">
         <v>130</v>
       </c>
-      <c r="B82" t="s">
-        <v>134</v>
-      </c>
       <c r="C82" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D82">
         <v>18.938951808444461</v>
@@ -6306,13 +6293,13 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B83" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C83" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D83">
         <v>18.938951808444461</v>
@@ -6323,13 +6310,13 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B84" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C84" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D84">
         <v>1.050221781912281</v>
@@ -6340,13 +6327,13 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B85" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C85" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D85">
         <v>1.050221781912281</v>
@@ -6357,13 +6344,13 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B86" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C86" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D86">
         <v>18.938951808444461</v>
@@ -6374,13 +6361,13 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B87" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C87" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D87">
         <v>1.050221781912281</v>
@@ -6391,13 +6378,13 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B88" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C88" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D88">
         <v>1.050221781912281</v>
@@ -6408,46 +6395,46 @@
     </row>
     <row r="91" spans="1:5" ht="20" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B91" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="20" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B93" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D93" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C93" s="1" t="s">
+      <c r="E93" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E93" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B94" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C94" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D94">
         <v>0.81456967246191447</v>
@@ -6458,13 +6445,13 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B95" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C95" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D95">
         <v>0.81456967246191447</v>
@@ -6475,13 +6462,13 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
+        <v>126</v>
+      </c>
+      <c r="B96" t="s">
         <v>130</v>
       </c>
-      <c r="B96" t="s">
-        <v>134</v>
-      </c>
       <c r="C96" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D96">
         <v>12.969098369035169</v>
@@ -6492,13 +6479,13 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B97" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C97" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D97">
         <v>0.81456967246191447</v>
@@ -6509,13 +6496,13 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B98" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C98" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D98">
         <v>0.81456967246191447</v>
@@ -6526,13 +6513,13 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
+        <v>126</v>
+      </c>
+      <c r="B99" t="s">
         <v>130</v>
       </c>
-      <c r="B99" t="s">
-        <v>134</v>
-      </c>
       <c r="C99" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D99">
         <v>12.969098369035169</v>
@@ -6543,13 +6530,13 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B100" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C100" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D100">
         <v>12.969098369035169</v>
@@ -6560,13 +6547,13 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B101" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C101" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D101">
         <v>0.81456967246191447</v>
@@ -6577,13 +6564,13 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B102" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C102" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D102">
         <v>0.81456967246191447</v>
@@ -6594,13 +6581,13 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B103" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C103" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D103">
         <v>12.969098369035169</v>
@@ -6611,13 +6598,13 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B104" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C104" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D104">
         <v>0.81456967246191447</v>
@@ -6628,13 +6615,13 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B105" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C105" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D105">
         <v>0.81456967246191447</v>
@@ -6645,35 +6632,35 @@
     </row>
     <row r="108" spans="1:5" ht="20" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B108" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="20" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B110" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D110" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C110" s="1" t="s">
+      <c r="E110" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E110" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -6685,7 +6672,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
@@ -6704,34 +6691,34 @@
   <sheetData>
     <row r="1" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -7724,42 +7711,42 @@
   <sheetData>
     <row r="1" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>161</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B2">
         <v>-75</v>
@@ -7794,7 +7781,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B3">
         <v>-30</v>
@@ -7989,7 +7976,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -8120,7 +8107,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B13">
         <v>20</v>
@@ -8763,7 +8750,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B33">
         <v>146.16800000000001</v>
@@ -8825,69 +8812,69 @@
   <sheetData>
     <row r="1" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B2">
         <v>1235</v>
@@ -8940,7 +8927,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B3">
         <v>7850</v>
@@ -8993,7 +8980,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B4">
         <v>1940</v>
@@ -9047,15 +9034,15 @@
         <v>197</v>
       </c>
       <c r="S4" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="T4" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B5">
         <v>1220</v>
@@ -9108,7 +9095,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B6">
         <v>1940</v>
@@ -9162,15 +9149,15 @@
         <v>197</v>
       </c>
       <c r="S6" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="T6" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B7">
         <v>1940</v>
@@ -9224,15 +9211,15 @@
         <v>197</v>
       </c>
       <c r="S7" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="T7" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B8">
         <v>110</v>
@@ -9283,15 +9270,15 @@
         <v>0</v>
       </c>
       <c r="S8" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="T8" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B9">
         <v>130</v>
@@ -9342,10 +9329,10 @@
         <v>3</v>
       </c>
       <c r="S9" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="T9" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -9373,25 +9360,25 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -9880,10 +9867,10 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -9896,7 +9883,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -9904,7 +9891,7 @@
         <v>0.02</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -9912,7 +9899,7 @@
         <v>0.15</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -9920,7 +9907,7 @@
         <v>0.24517031675566089</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -9928,7 +9915,7 @@
         <v>0.43917934644591611</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -9936,7 +9923,7 @@
         <v>0.63820765691637371</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -9944,7 +9931,7 @@
         <v>0.77174385227158171</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -9952,12 +9939,12 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -9968,25 +9955,25 @@
     </row>
     <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -10702,17 +10689,17 @@
   <sheetData>
     <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -10720,7 +10707,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B3">
         <v>0.5</v>
@@ -10728,10 +10715,10 @@
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -11546,7 +11533,7 @@
     </row>
     <row r="109" spans="1:4" ht="20" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B109" s="2">
         <v>3000000</v>
@@ -11556,16 +11543,16 @@
     </row>
     <row r="110" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
@@ -11619,17 +11606,17 @@
   <sheetData>
     <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B2">
         <v>0.5</v>
@@ -11637,7 +11624,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B3">
         <v>0.316</v>
@@ -11645,10 +11632,10 @@
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -14855,7 +14842,7 @@
     </row>
     <row r="408" spans="1:4" ht="20" x14ac:dyDescent="0.25">
       <c r="A408" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B408" s="2">
         <v>8100000</v>
@@ -14865,16 +14852,16 @@
     </row>
     <row r="409" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A409" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B409" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C409" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D409" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="410" spans="1:4" x14ac:dyDescent="0.2">
@@ -17686,17 +17673,17 @@
   <sheetData>
     <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B2">
         <v>0.36</v>
@@ -17704,7 +17691,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B3">
         <v>0.316</v>
@@ -17712,10 +17699,10 @@
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -19322,7 +19309,7 @@
     </row>
     <row r="208" spans="1:4" ht="20" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B208" s="2">
         <v>8100000</v>
@@ -19332,16 +19319,16 @@
     </row>
     <row r="209" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.2">
@@ -20459,17 +20446,17 @@
   <sheetData>
     <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B2">
         <v>0.30099999999999999</v>
@@ -20477,7 +20464,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B3">
         <v>0.28199999999999997</v>
@@ -20485,10 +20472,10 @@
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -22095,7 +22082,7 @@
     </row>
     <row r="208" spans="1:4" ht="20" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B208" s="2">
         <v>8100000</v>
@@ -22105,16 +22092,16 @@
     </row>
     <row r="209" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.2">
@@ -24968,17 +24955,17 @@
   <sheetData>
     <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B2">
         <v>0.24099999999999999</v>
@@ -24986,7 +24973,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B3">
         <v>0.26600000000000001</v>
@@ -24994,10 +24981,10 @@
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -26612,7 +26599,7 @@
     </row>
     <row r="209" spans="1:4" ht="20" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B209" s="2">
         <v>10300000</v>
@@ -26622,16 +26609,16 @@
     </row>
     <row r="210" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.2">
@@ -29624,17 +29611,17 @@
   <sheetData>
     <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B2">
         <v>0.21099999999999999</v>
@@ -29642,7 +29629,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B3">
         <v>0.26500000000000001</v>
@@ -29650,10 +29637,10 @@
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -31268,7 +31255,7 @@
     </row>
     <row r="209" spans="1:4" ht="20" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B209" s="2">
         <v>10400000</v>
@@ -31278,16 +31265,16 @@
     </row>
     <row r="210" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.2">
@@ -34253,17 +34240,17 @@
   <sheetData>
     <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B2">
         <v>0.18</v>
@@ -34271,7 +34258,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B3">
         <v>0.25</v>
@@ -34279,10 +34266,10 @@
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -37481,7 +37468,7 @@
     </row>
     <row r="407" spans="1:4" ht="20" x14ac:dyDescent="0.25">
       <c r="A407" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B407" s="2">
         <v>750000</v>
@@ -37491,16 +37478,16 @@
     </row>
     <row r="408" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A408" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B408" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C408" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D408" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="409" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fix rounding format error in spreadsheet
</commit_message>
<xml_diff>
--- a/Documentation/IEA-15-240-RWT_tabular.xlsx
+++ b/Documentation/IEA-15-240-RWT_tabular.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gbarter/systems/referenceTurbines/15mw/IEA-15-240-RWT/Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gbarter/systems/referenceTurbines/15mw/IEA-15-240-RWT/WISDEM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F51ABCA-E930-8C4F-8645-44968E8A69B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD35B43C-4BD2-0343-8E20-6DA2C337F482}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -776,7 +776,7 @@
     <t>Z_TT [m]</t>
   </si>
   <si>
-    <t>Mass [t]</t>
+    <t>Mass [kg]</t>
   </si>
   <si>
     <t>I_xx [kg.m^2]</t>
@@ -1226,7 +1226,7 @@
   <dimension ref="A1:B46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M57" sqref="M57"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1613,7 +1613,7 @@
   <dimension ref="A1:Q51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M57" sqref="M57"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4350,7 +4350,7 @@
   <dimension ref="A1:F126"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M57" sqref="M57"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6421,7 +6421,7 @@
   <dimension ref="A1:E74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M57" sqref="M57"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7319,7 +7319,7 @@
   <dimension ref="A1:AZ22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M57" sqref="M57"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9182,7 +9182,7 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M57" sqref="M57"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10284,7 +10284,7 @@
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M57" sqref="M57"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10836,7 +10836,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M57" sqref="M57"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11342,14 +11342,14 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M57" sqref="M57"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="13" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="18.6640625" bestFit="1" customWidth="1"/>
@@ -11399,10 +11399,10 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>-0.19</v>
       </c>
       <c r="D3">
-        <v>100</v>
+        <v>100000</v>
       </c>
       <c r="E3">
         <v>490266</v>
@@ -11428,13 +11428,13 @@
         <v>255</v>
       </c>
       <c r="B4">
-        <v>6</v>
+        <v>-6.0750000000000002</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>4.9859999999999998</v>
       </c>
       <c r="D4">
-        <v>13</v>
+        <v>13362</v>
       </c>
       <c r="E4">
         <v>14766</v>
@@ -11460,13 +11460,13 @@
         <v>256</v>
       </c>
       <c r="B5">
-        <v>6</v>
+        <v>-5.7350000000000003</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>4.9509999999999996</v>
       </c>
       <c r="D5">
-        <v>227</v>
+        <v>226700</v>
       </c>
       <c r="E5">
         <v>4691596</v>
@@ -11492,13 +11492,13 @@
         <v>257</v>
       </c>
       <c r="B6">
-        <v>6</v>
+        <v>-6.3390000000000004</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>5.0140000000000002</v>
       </c>
       <c r="D6">
-        <v>145</v>
+        <v>145250</v>
       </c>
       <c r="E6">
         <v>3275431</v>
@@ -11524,13 +11524,13 @@
         <v>258</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>-6.1390000000000002</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>4.9930000000000003</v>
       </c>
       <c r="D7">
-        <v>20</v>
+        <v>19504</v>
       </c>
       <c r="E7">
         <v>48263</v>
@@ -11556,13 +11556,13 @@
         <v>259</v>
       </c>
       <c r="B8">
-        <v>11</v>
+        <v>-10.685</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>5.4710000000000001</v>
       </c>
       <c r="D8">
-        <v>190</v>
+        <v>190000</v>
       </c>
       <c r="E8">
         <v>1382171</v>
@@ -11588,13 +11588,13 @@
         <v>260</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>-0.80900000000000005</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>2.7050000000000001</v>
       </c>
       <c r="D9">
-        <v>39</v>
+        <v>39434</v>
       </c>
       <c r="E9">
         <v>226120</v>
@@ -11620,13 +11620,13 @@
         <v>261</v>
       </c>
       <c r="B10">
-        <v>5</v>
+        <v>-4.6710000000000003</v>
       </c>
       <c r="C10">
-        <v>5</v>
+        <v>4.8390000000000004</v>
       </c>
       <c r="D10">
-        <v>4</v>
+        <v>3627</v>
       </c>
       <c r="E10">
         <v>5317</v>
@@ -11655,10 +11655,10 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D11">
-        <v>50</v>
+        <v>50000</v>
       </c>
       <c r="E11">
         <v>16667</v>
@@ -11684,13 +11684,13 @@
         <v>263</v>
       </c>
       <c r="B12">
-        <v>5</v>
+        <v>-5.3559999999999999</v>
       </c>
       <c r="C12">
-        <v>5</v>
+        <v>4.9109999999999996</v>
       </c>
       <c r="D12">
-        <v>5</v>
+        <v>4699</v>
       </c>
       <c r="E12">
         <v>8084</v>
@@ -11716,13 +11716,13 @@
         <v>264</v>
       </c>
       <c r="B13">
-        <v>7</v>
+        <v>-6.9480000000000004</v>
       </c>
       <c r="C13">
-        <v>5</v>
+        <v>5.0780000000000003</v>
       </c>
       <c r="D13">
-        <v>5</v>
+        <v>4699</v>
       </c>
       <c r="E13">
         <v>8084</v>
@@ -11748,13 +11748,13 @@
         <v>265</v>
       </c>
       <c r="B14">
-        <v>6</v>
+        <v>-5.718</v>
       </c>
       <c r="C14">
-        <v>4</v>
+        <v>4.048</v>
       </c>
       <c r="D14">
-        <v>797</v>
+        <v>797275</v>
       </c>
       <c r="E14">
         <v>13442266</v>
@@ -11785,7 +11785,7 @@
   <dimension ref="A1:G62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M57" sqref="M57"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13070,7 +13070,7 @@
   <dimension ref="A1:D112"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M57" sqref="M57"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13987,7 +13987,7 @@
   <dimension ref="A1:D608"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M57" sqref="M57"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20054,7 +20054,7 @@
   <dimension ref="A1:D287"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M57" sqref="M57"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -22827,7 +22827,7 @@
   <dimension ref="A1:D411"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M57" sqref="M57"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -27336,7 +27336,7 @@
   <dimension ref="A1:D422"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M57" sqref="M57"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -31993,7 +31993,7 @@
   <dimension ref="A1:D420"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M57" sqref="M57"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -36621,7 +36621,7 @@
   <dimension ref="A1:D535"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M57" sqref="M57"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
now with ORBIT and better tower/monopile calculations
</commit_message>
<xml_diff>
--- a/Documentation/IEA-15-240-RWT_tabular.xlsx
+++ b/Documentation/IEA-15-240-RWT_tabular.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gbarter/systems/referenceTurbines/15mw/IEA-15-240-RWT/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10323E3B-414E-E546-AD77-8B109BF8AD59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE252FC-4FCE-1B4D-83C9-ED415E7D8FE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,17 @@
     <sheet name="Rotor Performance" sheetId="17" r:id="rId17"/>
     <sheet name="Nacelle Mass Properties" sheetId="18" r:id="rId18"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -177,7 +187,7 @@
     <t>Nacelle center of mass from tower top [m]</t>
   </si>
   <si>
-    <t>[-6.853, 0.0, 4.351]</t>
+    <t>[-7.65265556, 0.0, 4.6022611]</t>
   </si>
   <si>
     <t>Tower mass [t]</t>
@@ -1217,8 +1227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1296,7 +1306,7 @@
         <v>12</v>
       </c>
       <c r="B9">
-        <v>10.84</v>
+        <v>10.88</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -1448,7 +1458,7 @@
         <v>33</v>
       </c>
       <c r="B28">
-        <v>65.253500000000003</v>
+        <v>65.8</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -1536,7 +1546,7 @@
         <v>44</v>
       </c>
       <c r="B39">
-        <v>993.03499999999997</v>
+        <v>994.72</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -1552,7 +1562,8 @@
         <v>47</v>
       </c>
       <c r="B41">
-        <v>803.49777196829643</v>
+        <f>859.8</f>
+        <v>859.8</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -1592,7 +1603,8 @@
         <v>52</v>
       </c>
       <c r="B46">
-        <v>1138.040855481752</v>
+        <f>1317.7</f>
+        <v>1317.7</v>
       </c>
     </row>
   </sheetData>
@@ -1605,7 +1617,7 @@
   <dimension ref="A1:D329"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4966,7 +4978,7 @@
   <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6455,7 +6467,7 @@
   <dimension ref="A1:F158"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9038,7 +9050,7 @@
   <dimension ref="A1:E90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10104,12 +10116,12 @@
   <dimension ref="A1:AZ14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8" customWidth="1"/>
+    <col min="1" max="1" width="8.33203125" customWidth="1"/>
     <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.5" bestFit="1" customWidth="1"/>
@@ -12054,7 +12066,7 @@
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13411,7 +13423,7 @@
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13963,7 +13975,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14469,7 +14481,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14912,7 +14924,7 @@
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15753,7 +15765,7 @@
   <dimension ref="A1:D112"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16670,7 +16682,7 @@
   <dimension ref="A1:D408"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -21137,7 +21149,7 @@
   <dimension ref="A1:D329"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -24498,7 +24510,7 @@
   <dimension ref="A1:D329"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -27859,7 +27871,7 @@
   <dimension ref="A1:D386"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -31676,7 +31688,7 @@
   <dimension ref="A1:D329"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -35037,7 +35049,7 @@
   <dimension ref="A1:D386"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
switching from WISDEM performance data to FAST rotor performance data
</commit_message>
<xml_diff>
--- a/Documentation/IEA-15-240-RWT_tabular.xlsx
+++ b/Documentation/IEA-15-240-RWT_tabular.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gbarter/systems/referenceTurbines/15mw/IEA-15-240-RWT/WISDEM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gbarter/systems/referenceTurbines/15mw/IEA-15-240-RWT/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D9D21B-6FD0-224B-84A1-7962EEC1AC3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCAE0324-7A7A-3A40-B49E-F7F754458FB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11440" yWindow="3120" windowWidth="21240" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="851" uniqueCount="267">
   <si>
     <t>Parameter</t>
   </si>
@@ -759,12 +759,6 @@
     <t>Tip Speed [m/s]</t>
   </si>
   <si>
-    <t>Thrust [MN]</t>
-  </si>
-  <si>
-    <t>Torque [MNm]</t>
-  </si>
-  <si>
     <t>X_TT [m]</t>
   </si>
   <si>
@@ -832,6 +826,18 @@
   </si>
   <si>
     <t>Nacelle total minus hub</t>
+  </si>
+  <si>
+    <t>Rotor Thrust [MN]</t>
+  </si>
+  <si>
+    <t>Rotor Torque [MNm]</t>
+  </si>
+  <si>
+    <t>Rotor Cp [-]</t>
+  </si>
+  <si>
+    <t>Rotor Ct [-]</t>
   </si>
 </sst>
 </file>
@@ -1224,7 +1230,7 @@
   <dimension ref="A1:B47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J44" sqref="J44"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14914,10 +14920,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:I60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AG65" sqref="AG65"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14926,11 +14932,12 @@
     <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>235</v>
       </c>
@@ -14947,474 +14954,1732 @@
         <v>239</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>240</v>
+        <v>263</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+        <v>264</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>3</v>
+        <v>2.99999983141003</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>3.9999996628200609</v>
       </c>
       <c r="C2">
-        <v>0.1844719104952009</v>
+        <v>7.0021376744199365E-2</v>
       </c>
       <c r="D2">
-        <v>2.1485917317405869</v>
+        <v>4.9941963096430326</v>
       </c>
       <c r="E2">
-        <v>27</v>
+        <v>62.758921747839231</v>
       </c>
       <c r="F2">
-        <v>0.18728161362772949</v>
+        <v>0.59396486062420217</v>
       </c>
       <c r="G2">
-        <v>1.524094189763328</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.13867685799238821</v>
+      </c>
+      <c r="H2">
+        <v>0.1003355524845071</v>
+      </c>
+      <c r="I2">
+        <v>0.81974894275916343</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>4.1578947368421053</v>
+        <v>3.4999999157050161</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>3.9812329486735951</v>
       </c>
       <c r="C3">
-        <v>0.73981580862965213</v>
+        <v>0.30199370032882411</v>
       </c>
       <c r="D3">
-        <v>2.977872751008884</v>
+        <v>4.9942923978859888</v>
       </c>
       <c r="E3">
-        <v>37.421052631578952</v>
+        <v>62.760129228311897</v>
       </c>
       <c r="F3">
-        <v>0.35974901528182812</v>
+        <v>0.659768435914592</v>
       </c>
       <c r="G3">
-        <v>2.9276306058211552</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.59806054561282329</v>
+      </c>
+      <c r="H3">
+        <v>0.27219720825803823</v>
+      </c>
+      <c r="I3">
+        <v>0.80111203080249627</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>5.3157894736842106</v>
+        <v>4</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>3.7084214920140628</v>
       </c>
       <c r="C4">
-        <v>1.7018581803432229</v>
+        <v>0.59508847508677354</v>
       </c>
       <c r="D4">
-        <v>3.8071537702771812</v>
+        <v>4.9956686846266134</v>
       </c>
       <c r="E4">
-        <v>47.842105263157897</v>
+        <v>62.777424157566209</v>
       </c>
       <c r="F4">
-        <v>0.58801469394166461</v>
+        <v>0.74401984439709157</v>
       </c>
       <c r="G4">
-        <v>4.785252332956512</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>1.178170168295547</v>
+      </c>
+      <c r="H4">
+        <v>0.35930511792501008</v>
+      </c>
+      <c r="I4">
+        <v>0.80826842414674971</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>6.4736842105263159</v>
+        <v>4.5000000842949834</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>3.2250206080948391</v>
       </c>
       <c r="C5">
-        <v>3.1711862194522991</v>
+        <v>0.96488739433662229</v>
       </c>
       <c r="D5">
-        <v>4.6364347895454774</v>
+        <v>4.9936653665395037</v>
       </c>
       <c r="E5">
-        <v>58.263157894736842</v>
+        <v>62.752249720025148</v>
       </c>
       <c r="F5">
-        <v>0.8720786496072388</v>
+        <v>0.84428388552215738</v>
       </c>
       <c r="G5">
-        <v>7.0969593711694028</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>1.9110699558656621</v>
+      </c>
+      <c r="H5">
+        <v>0.40915668516038528</v>
+      </c>
+      <c r="I5">
+        <v>0.82191091836349184</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>7.6315789473684212</v>
+        <v>4.7500001264424769</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>2.9866517187425869</v>
       </c>
       <c r="C6">
-        <v>5.234605978477525</v>
+        <v>1.185081978468336</v>
       </c>
       <c r="D6">
-        <v>5.4657158088137754</v>
+        <v>4.9958015364090258</v>
       </c>
       <c r="E6">
-        <v>68.684210526315795</v>
+        <v>62.779093622300778</v>
       </c>
       <c r="F6">
-        <v>1.2119408822785509</v>
+        <v>0.89621856689648738</v>
       </c>
       <c r="G6">
-        <v>9.8627517204598245</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>2.3461876505674599</v>
+      </c>
+      <c r="H6">
+        <v>0.42729002007563921</v>
+      </c>
+      <c r="I6">
+        <v>0.82287623672430499</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>8.7894736842105274</v>
+        <v>5.0000001685899704</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>2.7204954086472348</v>
       </c>
       <c r="C7">
-        <v>7.9585884910449414</v>
+        <v>1.4292168887018191</v>
       </c>
       <c r="D7">
-        <v>6.2949968280820716</v>
+        <v>4.9951685754869173</v>
       </c>
       <c r="E7">
-        <v>79.10526315789474</v>
+        <v>62.771139600769168</v>
       </c>
       <c r="F7">
-        <v>1.6076013919556009</v>
+        <v>0.95066646971876601</v>
       </c>
       <c r="G7">
-        <v>13.08262938082779</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+        <v>2.8298766225327561</v>
+      </c>
+      <c r="H7">
+        <v>0.44181961435671568</v>
+      </c>
+      <c r="I7">
+        <v>0.82326598050248223</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>9.9473684210526319</v>
+        <v>5.2499998735575231</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>2.328109733589848</v>
       </c>
       <c r="C8">
-        <v>11.381428525473019</v>
+        <v>1.6952452234643649</v>
       </c>
       <c r="D8">
-        <v>7.1242778473503678</v>
+        <v>4.9949383768649884</v>
       </c>
       <c r="E8">
-        <v>89.526315789473685</v>
+        <v>62.76824683957107</v>
       </c>
       <c r="F8">
-        <v>2.0590601786383891</v>
+        <v>1.013407272726035</v>
       </c>
       <c r="G8">
-        <v>16.75659235227327</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3.3567731971550119</v>
+      </c>
+      <c r="H8">
+        <v>0.45270804916851848</v>
+      </c>
+      <c r="I8">
+        <v>0.83098935755972225</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>10.945048247893951</v>
+        <v>5.99999966282006</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>1.191921933242176</v>
       </c>
       <c r="C9">
-        <v>15.000002576468271</v>
+        <v>2.656263808497588</v>
       </c>
       <c r="D9">
-        <v>7.5598597968650294</v>
+        <v>4.9977004862168499</v>
       </c>
       <c r="E9">
-        <v>95</v>
+        <v>62.802956529363982</v>
       </c>
       <c r="F9">
-        <v>2.4170609327134289</v>
+        <v>1.206649681077935</v>
       </c>
       <c r="G9">
-        <v>21.030669828777569</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+        <v>5.2568059710445398</v>
+      </c>
+      <c r="H9">
+        <v>0.47527029833498541</v>
+      </c>
+      <c r="I9">
+        <v>0.83493245619331591</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>12.263157894736841</v>
+        <v>6.1999999662820056</v>
       </c>
       <c r="B10">
-        <v>5.6506703658104627</v>
+        <v>0.87429063591711509</v>
       </c>
       <c r="C10">
-        <v>15</v>
+        <v>2.9572168306095361</v>
       </c>
       <c r="D10">
-        <v>7.5598597968650294</v>
+        <v>4.9949352185383349</v>
       </c>
       <c r="E10">
-        <v>95</v>
+        <v>62.768207150867838</v>
       </c>
       <c r="F10">
-        <v>1.7668821665604919</v>
+        <v>1.260317718471448</v>
       </c>
       <c r="G10">
-        <v>21.03066897283189</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+        <v>5.8556165115747731</v>
+      </c>
+      <c r="H10">
+        <v>0.47947864437491711</v>
+      </c>
+      <c r="I10">
+        <v>0.833618597964214</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>13.42105263157895</v>
+        <v>6.400000269743952</v>
       </c>
       <c r="B11">
-        <v>8.1685973058974231</v>
+        <v>0.5532216369251427</v>
       </c>
       <c r="C11">
-        <v>15</v>
+        <v>3.2757433730434462</v>
       </c>
       <c r="D11">
-        <v>7.5598597968650294</v>
+        <v>4.9948539733013213</v>
       </c>
       <c r="E11">
-        <v>95</v>
+        <v>62.767186193108877</v>
       </c>
       <c r="F11">
-        <v>1.539086584138363</v>
+        <v>1.3150606483917371</v>
       </c>
       <c r="G11">
-        <v>21.030665508385901</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+        <v>6.4864390605857798</v>
+      </c>
+      <c r="H11">
+        <v>0.48287126336212061</v>
+      </c>
+      <c r="I11">
+        <v>0.83180478021536552</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>14.57894736842105</v>
+        <v>6.4999997471150444</v>
       </c>
       <c r="B12">
-        <v>10.219284215372451</v>
+        <v>0.42371500520600691</v>
       </c>
       <c r="C12">
-        <v>15</v>
+        <v>3.4426695659181048</v>
       </c>
       <c r="D12">
-        <v>7.5598597968650294</v>
+        <v>4.9957082600410097</v>
       </c>
       <c r="E12">
-        <v>95</v>
+        <v>62.777921476890732</v>
       </c>
       <c r="F12">
-        <v>1.3802714605441271</v>
+        <v>1.3408580862535791</v>
       </c>
       <c r="G12">
-        <v>21.030663896953399</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+        <v>6.8158224430846968</v>
+      </c>
+      <c r="H12">
+        <v>0.4844476273592071</v>
+      </c>
+      <c r="I12">
+        <v>0.82901110345207962</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>15.736842105263159</v>
+        <v>6.5500001601604687</v>
       </c>
       <c r="B13">
-        <v>12.013386967131551</v>
+        <v>0.37114649328400628</v>
       </c>
       <c r="C13">
-        <v>15</v>
+        <v>3.5286546776674421</v>
       </c>
       <c r="D13">
-        <v>7.5598597968650294</v>
+        <v>4.9961682259056044</v>
       </c>
       <c r="E13">
-        <v>95</v>
+        <v>62.783701578415183</v>
       </c>
       <c r="F13">
-        <v>1.259549989705572</v>
+        <v>1.353034620129991</v>
       </c>
       <c r="G13">
-        <v>21.030661686997259</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+        <v>6.9853869625399954</v>
+      </c>
+      <c r="H13">
+        <v>0.48518633738712819</v>
+      </c>
+      <c r="I13">
+        <v>0.82690920148115699</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>16.89473684210526</v>
+        <v>6.599999898846022</v>
       </c>
       <c r="B14">
-        <v>13.63982936665364</v>
+        <v>0.31532898414606331</v>
       </c>
       <c r="C14">
-        <v>15</v>
+        <v>3.614989063764126</v>
       </c>
       <c r="D14">
-        <v>7.5598597968650294</v>
+        <v>4.9948172128327153</v>
       </c>
       <c r="E14">
-        <v>95</v>
+        <v>62.766724247436407</v>
       </c>
       <c r="F14">
-        <v>1.1635331803690789</v>
+        <v>1.365170434971128</v>
       </c>
       <c r="G14">
-        <v>21.030662429873399</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+        <v>7.158251633338665</v>
+      </c>
+      <c r="H14">
+        <v>0.48590584607885468</v>
+      </c>
+      <c r="I14">
+        <v>0.82474099701943604</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>18.05263157894737</v>
+        <v>6.700000050576989</v>
       </c>
       <c r="B15">
-        <v>15.14597164175149</v>
+        <v>0.20934994787572769</v>
       </c>
       <c r="C15">
-        <v>15</v>
+        <v>3.791164266922209</v>
       </c>
       <c r="D15">
-        <v>7.5598597968650294</v>
+        <v>4.9951228154571998</v>
       </c>
       <c r="E15">
-        <v>95</v>
+        <v>62.770564563276423</v>
       </c>
       <c r="F15">
-        <v>1.084946138233341</v>
+        <v>1.38957378092968</v>
       </c>
       <c r="G15">
-        <v>21.030666126174591</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+        <v>7.5066500940912428</v>
+      </c>
+      <c r="H15">
+        <v>0.48711415410475001</v>
+      </c>
+      <c r="I15">
+        <v>0.8204296750987693</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>19.210526315789469</v>
+        <v>6.8000002023079613</v>
       </c>
       <c r="B16">
-        <v>16.560400447823159</v>
+        <v>9.955812454622219E-2</v>
       </c>
       <c r="C16">
-        <v>15</v>
+        <v>3.9719678446624722</v>
       </c>
       <c r="D16">
-        <v>7.5598597968650294</v>
+        <v>4.995177735735858</v>
       </c>
       <c r="E16">
-        <v>95</v>
+        <v>62.771254711852272</v>
       </c>
       <c r="F16">
-        <v>1.019325811955724</v>
+        <v>1.414180748480736</v>
       </c>
       <c r="G16">
-        <v>21.030672397613181</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+        <v>7.8645349314738828</v>
+      </c>
+      <c r="H16">
+        <v>0.48809479266966332</v>
+      </c>
+      <c r="I16">
+        <v>0.81617625728053933</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>20.368421052631579</v>
+        <v>6.9000003540389354</v>
       </c>
       <c r="B17">
-        <v>17.901868349081031</v>
+        <v>7.5548250505280464E-3</v>
       </c>
       <c r="C17">
-        <v>15</v>
+        <v>4.1555890400977704</v>
       </c>
       <c r="D17">
-        <v>7.5598597968650294</v>
+        <v>4.997082176068333</v>
       </c>
       <c r="E17">
-        <v>95</v>
+        <v>62.795186614883093</v>
       </c>
       <c r="F17">
-        <v>0.96371332110189956</v>
+        <v>1.437989394704861</v>
       </c>
       <c r="G17">
-        <v>21.030676263167631</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+        <v>8.225013269255637</v>
+      </c>
+      <c r="H17">
+        <v>0.48886648794033949</v>
+      </c>
+      <c r="I17">
+        <v>0.81120023292779286</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>21.526315789473681</v>
+        <v>6.9199998448972302</v>
       </c>
       <c r="B18">
-        <v>19.183439924377261</v>
+        <v>6.0363435104773822E-4</v>
       </c>
       <c r="C18">
-        <v>15</v>
+        <v>4.1923870512712869</v>
       </c>
       <c r="D18">
-        <v>7.5598597968650294</v>
+        <v>4.9982720098404361</v>
       </c>
       <c r="E18">
-        <v>95</v>
+        <v>62.810138507032818</v>
       </c>
       <c r="F18">
-        <v>0.91603802722512417</v>
+        <v>1.442160462715987</v>
       </c>
       <c r="G18">
-        <v>21.03066984284899</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+        <v>8.2959073907682921</v>
+      </c>
+      <c r="H18">
+        <v>0.48898805785557892</v>
+      </c>
+      <c r="I18">
+        <v>0.80974090334607529</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>22.684210526315791</v>
+        <v>6.9299999275063158</v>
       </c>
       <c r="B19">
-        <v>20.414597979230681</v>
+        <v>6.9759262380658747E-7</v>
       </c>
       <c r="C19">
-        <v>15</v>
+        <v>4.2107735494853218</v>
       </c>
       <c r="D19">
-        <v>7.5598597968650294</v>
+        <v>4.9981817964778399</v>
       </c>
       <c r="E19">
-        <v>95</v>
+        <v>62.809004852484073</v>
       </c>
       <c r="F19">
-        <v>0.87479145148922444</v>
+        <v>1.443944251321386</v>
       </c>
       <c r="G19">
-        <v>21.030664869517452</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+        <v>8.3324673733358825</v>
+      </c>
+      <c r="H19">
+        <v>0.48905015163814608</v>
+      </c>
+      <c r="I19">
+        <v>0.80878076478266125</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>23.842105263157901</v>
+        <v>6.9400000101153978</v>
       </c>
       <c r="B20">
-        <v>21.602432657681199</v>
+        <v>0</v>
       </c>
       <c r="C20">
-        <v>15</v>
+        <v>4.2288413766865682</v>
       </c>
       <c r="D20">
-        <v>7.5598597968650294</v>
+        <v>5.0004031306649006</v>
       </c>
       <c r="E20">
-        <v>95</v>
+        <v>62.836918961137009</v>
       </c>
       <c r="F20">
-        <v>0.83883946692129818</v>
+        <v>1.4460954761386791</v>
       </c>
       <c r="G20">
-        <v>21.030672481716021</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+        <v>8.3645492487878954</v>
+      </c>
+      <c r="H20">
+        <v>0.48908885760684129</v>
+      </c>
+      <c r="I20">
+        <v>0.80810230579183462</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>25</v>
+        <v>6.9500000927244807</v>
       </c>
       <c r="B21">
-        <v>22.752399824772219</v>
+        <v>0</v>
       </c>
       <c r="C21">
-        <v>15</v>
+        <v>4.2471864347291133</v>
       </c>
       <c r="D21">
-        <v>7.5598597968650294</v>
+        <v>5.0036851538949696</v>
       </c>
       <c r="E21">
-        <v>95</v>
+        <v>62.878162081411013</v>
       </c>
       <c r="F21">
-        <v>0.80730667518187127</v>
+        <v>1.4484338168473381</v>
       </c>
       <c r="G21">
-        <v>21.030658235729739</v>
+        <v>8.3953629851285179</v>
+      </c>
+      <c r="H21">
+        <v>0.48911453137404559</v>
+      </c>
+      <c r="I21">
+        <v>0.80756662607065333</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>6.9600001753335663</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>4.2654581052991372</v>
+      </c>
+      <c r="D22">
+        <v>5.0085864686395016</v>
+      </c>
+      <c r="E22">
+        <v>62.939753818988407</v>
+      </c>
+      <c r="F22">
+        <v>1.451063716287663</v>
+      </c>
+      <c r="G22">
+        <v>8.4232664637323715</v>
+      </c>
+      <c r="H22">
+        <v>0.48912776385443502</v>
+      </c>
+      <c r="I22">
+        <v>0.80725197739638843</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>6.9699995835827746</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>4.2838983916599824</v>
+      </c>
+      <c r="D23">
+        <v>5.0111700884403234</v>
+      </c>
+      <c r="E23">
+        <v>62.972220542932128</v>
+      </c>
+      <c r="F23">
+        <v>1.453280930706631</v>
+      </c>
+      <c r="G23">
+        <v>8.4553694968687783</v>
+      </c>
+      <c r="H23">
+        <v>0.48915575977465747</v>
+      </c>
+      <c r="I23">
+        <v>0.80662441966212617</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>6.9800003405517392</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>4.3019484942843773</v>
+      </c>
+      <c r="D24">
+        <v>5.0173999660494566</v>
+      </c>
+      <c r="E24">
+        <v>63.05050749385061</v>
+      </c>
+      <c r="F24">
+        <v>1.456152591917846</v>
+      </c>
+      <c r="G24">
+        <v>8.4804751525688946</v>
+      </c>
+      <c r="H24">
+        <v>0.48916504716561621</v>
+      </c>
+      <c r="I24">
+        <v>0.80649551197257474</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>6.989999748800944</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>4.3202899111755348</v>
+      </c>
+      <c r="D25">
+        <v>5.0268070601074326</v>
+      </c>
+      <c r="E25">
+        <v>63.168720524187258</v>
+      </c>
+      <c r="F25">
+        <v>1.459581324345367</v>
+      </c>
+      <c r="G25">
+        <v>8.5006944222069496</v>
+      </c>
+      <c r="H25">
+        <v>0.48915446647173039</v>
+      </c>
+      <c r="I25">
+        <v>0.80680617316531367</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>6.9999998314100322</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>4.339296325727684</v>
+      </c>
+      <c r="D26">
+        <v>5.0328150196655193</v>
+      </c>
+      <c r="E26">
+        <v>63.244218770630262</v>
+      </c>
+      <c r="F26">
+        <v>1.4624085735374259</v>
+      </c>
+      <c r="G26">
+        <v>8.5278632412515272</v>
+      </c>
+      <c r="H26">
+        <v>0.48916386684904151</v>
+      </c>
+      <c r="I26">
+        <v>0.80665115789407715</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>7.4999999157050166</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>5.338823240491906</v>
+      </c>
+      <c r="D27">
+        <v>5.3829146199067637</v>
+      </c>
+      <c r="E27">
+        <v>67.643700099200743</v>
+      </c>
+      <c r="F27">
+        <v>1.61859861635883</v>
+      </c>
+      <c r="G27">
+        <v>9.8096774433373231</v>
+      </c>
+      <c r="H27">
+        <v>0.48922416074732672</v>
+      </c>
+      <c r="I27">
+        <v>0.80546965776526436</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>8</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>6.4811169945734166</v>
+      </c>
+      <c r="D28">
+        <v>5.7342028927818376</v>
+      </c>
+      <c r="E28">
+        <v>72.058118728627051</v>
+      </c>
+      <c r="F28">
+        <v>1.7856883247299129</v>
+      </c>
+      <c r="G28">
+        <v>11.17890909443933</v>
+      </c>
+      <c r="H28">
+        <v>0.48926304835543022</v>
+      </c>
+      <c r="I28">
+        <v>0.80457156746402092</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>8.5000000842949834</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>7.7745709836422199</v>
+      </c>
+      <c r="D29">
+        <v>6.0870247145305552</v>
+      </c>
+      <c r="E29">
+        <v>76.491808501554786</v>
+      </c>
+      <c r="F29">
+        <v>1.963797766389662</v>
+      </c>
+      <c r="G29">
+        <v>12.632607514238581</v>
+      </c>
+      <c r="H29">
+        <v>0.48928801999506211</v>
+      </c>
+      <c r="I29">
+        <v>0.80394912145493247</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>9.0000001685899669</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>9.2292270240913279</v>
+      </c>
+      <c r="D30">
+        <v>6.4446659060181632</v>
+      </c>
+      <c r="E30">
+        <v>80.986060260749085</v>
+      </c>
+      <c r="F30">
+        <v>2.1537662096573742</v>
+      </c>
+      <c r="G30">
+        <v>14.16401500573317</v>
+      </c>
+      <c r="H30">
+        <v>0.48929311562292183</v>
+      </c>
+      <c r="I30">
+        <v>0.80390489506621887</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>9.5000002528849539</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>10.85504374139297</v>
+      </c>
+      <c r="D31">
+        <v>6.8006806713811976</v>
+      </c>
+      <c r="E31">
+        <v>85.459873746485087</v>
+      </c>
+      <c r="F31">
+        <v>2.3541539570861771</v>
+      </c>
+      <c r="G31">
+        <v>15.787013884251371</v>
+      </c>
+      <c r="H31">
+        <v>0.48930430388906893</v>
+      </c>
+      <c r="I31">
+        <v>0.80370873431504297</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>10.000000337179941</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>12.66125447833948</v>
+      </c>
+      <c r="D32">
+        <v>7.1558534642157596</v>
+      </c>
+      <c r="E32">
+        <v>89.9231066933812</v>
+      </c>
+      <c r="F32">
+        <v>2.5651566947137989</v>
+      </c>
+      <c r="G32">
+        <v>17.499915246737469</v>
+      </c>
+      <c r="H32">
+        <v>0.48931914336180821</v>
+      </c>
+      <c r="I32">
+        <v>0.8034521100129528</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>10.24999970496755</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>13.638148000824231</v>
+      </c>
+      <c r="D33">
+        <v>7.3157570149505178</v>
+      </c>
+      <c r="E33">
+        <v>91.932513974466161</v>
+      </c>
+      <c r="F33">
+        <v>2.6700361587237058</v>
+      </c>
+      <c r="G33">
+        <v>18.43804958034011</v>
+      </c>
+      <c r="H33">
+        <v>0.48938292000222777</v>
+      </c>
+      <c r="I33">
+        <v>0.80170615434402726</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>10.49999974711505</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>14.660657272899151</v>
+      </c>
+      <c r="D34">
+        <v>7.4950527388934463</v>
+      </c>
+      <c r="E34">
+        <v>94.185610491102835</v>
+      </c>
+      <c r="F34">
+        <v>2.7826381588645481</v>
+      </c>
+      <c r="G34">
+        <v>19.34629471828212</v>
+      </c>
+      <c r="H34">
+        <v>0.48937805901974663</v>
+      </c>
+      <c r="I34">
+        <v>0.80177739279103899</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>10.60000057320589</v>
+      </c>
+      <c r="B35">
+        <v>0.6451004751540339</v>
+      </c>
+      <c r="C35">
+        <v>14.994846345015389</v>
+      </c>
+      <c r="D35">
+        <v>7.5574023057856241</v>
+      </c>
+      <c r="E35">
+        <v>94.969118256314715</v>
+      </c>
+      <c r="F35">
+        <v>2.7278304307801409</v>
+      </c>
+      <c r="G35">
+        <v>19.624049730854001</v>
+      </c>
+      <c r="H35">
+        <v>0.48650717675929978</v>
+      </c>
+      <c r="I35">
+        <v>0.76865755354022625</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>10.700000050576991</v>
+      </c>
+      <c r="B36">
+        <v>1.70652840144081</v>
+      </c>
+      <c r="C36">
+        <v>14.994649789088241</v>
+      </c>
+      <c r="D36">
+        <v>7.5573032426077216</v>
+      </c>
+      <c r="E36">
+        <v>94.967873391706974</v>
+      </c>
+      <c r="F36">
+        <v>2.5823259934055192</v>
+      </c>
+      <c r="G36">
+        <v>19.624047630528771</v>
+      </c>
+      <c r="H36">
+        <v>0.47299155755768502</v>
+      </c>
+      <c r="I36">
+        <v>0.70731524973583515</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>10.72000021579516</v>
+      </c>
+      <c r="B37">
+        <v>1.851434903322418</v>
+      </c>
+      <c r="C37">
+        <v>14.994611951802129</v>
+      </c>
+      <c r="D37">
+        <v>7.5572841720810517</v>
+      </c>
+      <c r="E37">
+        <v>94.967633744401013</v>
+      </c>
+      <c r="F37">
+        <v>2.5631670698209659</v>
+      </c>
+      <c r="G37">
+        <v>19.624047914206731</v>
+      </c>
+      <c r="H37">
+        <v>0.47034931558669402</v>
+      </c>
+      <c r="I37">
+        <v>0.69850774281490779</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>10.73999970665345</v>
+      </c>
+      <c r="B38">
+        <v>1.986782432530775</v>
+      </c>
+      <c r="C38">
+        <v>14.994553742196119</v>
+      </c>
+      <c r="D38">
+        <v>7.5572548326887183</v>
+      </c>
+      <c r="E38">
+        <v>94.967265054723356</v>
+      </c>
+      <c r="F38">
+        <v>2.5454141419453591</v>
+      </c>
+      <c r="G38">
+        <v>19.624047131924911</v>
+      </c>
+      <c r="H38">
+        <v>0.46772494147603022</v>
+      </c>
+      <c r="I38">
+        <v>0.69021196256090511</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>10.760000546231501</v>
+      </c>
+      <c r="B39">
+        <v>2.1143351494340221</v>
+      </c>
+      <c r="C39">
+        <v>14.994520824095391</v>
+      </c>
+      <c r="D39">
+        <v>7.5572382444185093</v>
+      </c>
+      <c r="E39">
+        <v>94.967056600372047</v>
+      </c>
+      <c r="F39">
+        <v>2.5287954044261269</v>
+      </c>
+      <c r="G39">
+        <v>19.624044566295879</v>
+      </c>
+      <c r="H39">
+        <v>0.46511914271936722</v>
+      </c>
+      <c r="I39">
+        <v>0.68233559119860587</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>10.78000003708979</v>
+      </c>
+      <c r="B40">
+        <v>2.2351114085194088</v>
+      </c>
+      <c r="C40">
+        <v>14.99455423628878</v>
+      </c>
+      <c r="D40">
+        <v>7.5572550824853311</v>
+      </c>
+      <c r="E40">
+        <v>94.967268193760177</v>
+      </c>
+      <c r="F40">
+        <v>2.5131908067130868</v>
+      </c>
+      <c r="G40">
+        <v>19.624044522807321</v>
+      </c>
+      <c r="H40">
+        <v>0.46253704356607039</v>
+      </c>
+      <c r="I40">
+        <v>0.67483593877483583</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>10.78400033987737</v>
+      </c>
+      <c r="B41">
+        <v>2.2586111365600341</v>
+      </c>
+      <c r="C41">
+        <v>14.99452964561466</v>
+      </c>
+      <c r="D41">
+        <v>7.5572426915616422</v>
+      </c>
+      <c r="E41">
+        <v>94.967112484820831</v>
+      </c>
+      <c r="F41">
+        <v>2.510161326258717</v>
+      </c>
+      <c r="G41">
+        <v>19.624044479306871</v>
+      </c>
+      <c r="H41">
+        <v>0.46202188233062569</v>
+      </c>
+      <c r="I41">
+        <v>0.67337118330027557</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>10.786000491271171</v>
+      </c>
+      <c r="B42">
+        <v>2.270237050223832</v>
+      </c>
+      <c r="C42">
+        <v>14.99453210864859</v>
+      </c>
+      <c r="D42">
+        <v>7.5572439315658766</v>
+      </c>
+      <c r="E42">
+        <v>94.967128067173618</v>
+      </c>
+      <c r="F42">
+        <v>2.508666998264526</v>
+      </c>
+      <c r="G42">
+        <v>19.62404463005041</v>
+      </c>
+      <c r="H42">
+        <v>0.46176528394372302</v>
+      </c>
+      <c r="I42">
+        <v>0.67264611050824108</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>10.78699989260819</v>
+      </c>
+      <c r="B43">
+        <v>2.276057578844537</v>
+      </c>
+      <c r="C43">
+        <v>14.994531409155369</v>
+      </c>
+      <c r="D43">
+        <v>7.5572435742219266</v>
+      </c>
+      <c r="E43">
+        <v>94.967123576657102</v>
+      </c>
+      <c r="F43">
+        <v>2.5079178126675372</v>
+      </c>
+      <c r="G43">
+        <v>19.624044171637429</v>
+      </c>
+      <c r="H43">
+        <v>0.46163655700244749</v>
+      </c>
+      <c r="I43">
+        <v>0.67228318485026184</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>10.78799996830509</v>
+      </c>
+      <c r="B44">
+        <v>2.2818460933955769</v>
+      </c>
+      <c r="C44">
+        <v>14.994515427678611</v>
+      </c>
+      <c r="D44">
+        <v>7.557235531856235</v>
+      </c>
+      <c r="E44">
+        <v>94.967022513309203</v>
+      </c>
+      <c r="F44">
+        <v>2.5071727500876362</v>
+      </c>
+      <c r="G44">
+        <v>19.624044979574251</v>
+      </c>
+      <c r="H44">
+        <v>0.46150845984941807</v>
+      </c>
+      <c r="I44">
+        <v>0.67192156924844904</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>10.788999369642109</v>
+      </c>
+      <c r="B45">
+        <v>2.2875719706819111</v>
+      </c>
+      <c r="C45">
+        <v>14.994524657631329</v>
+      </c>
+      <c r="D45">
+        <v>7.5572401745562194</v>
+      </c>
+      <c r="E45">
+        <v>94.967080855197864</v>
+      </c>
+      <c r="F45">
+        <v>2.506439830473643</v>
+      </c>
+      <c r="G45">
+        <v>19.624045426500381</v>
+      </c>
+      <c r="H45">
+        <v>0.4613809405217727</v>
+      </c>
+      <c r="I45">
+        <v>0.67156403315504276</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>10.789500419030359</v>
+      </c>
+      <c r="B46">
+        <v>2.2904449258786581</v>
+      </c>
+      <c r="C46">
+        <v>14.99459141750974</v>
+      </c>
+      <c r="D46">
+        <v>7.5572738237854136</v>
+      </c>
+      <c r="E46">
+        <v>94.967503703882798</v>
+      </c>
+      <c r="F46">
+        <v>2.5060789319752201</v>
+      </c>
+      <c r="G46">
+        <v>19.62404426469384</v>
+      </c>
+      <c r="H46">
+        <v>0.461317766316996</v>
+      </c>
+      <c r="I46">
+        <v>0.67138699405703517</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>10.80000020230796</v>
+      </c>
+      <c r="B47">
+        <v>2.350461945050077</v>
+      </c>
+      <c r="C47">
+        <v>14.99453984264248</v>
+      </c>
+      <c r="D47">
+        <v>7.5572478273202952</v>
+      </c>
+      <c r="E47">
+        <v>94.967177022667471</v>
+      </c>
+      <c r="F47">
+        <v>2.498382010974856</v>
+      </c>
+      <c r="G47">
+        <v>19.62404422578701</v>
+      </c>
+      <c r="H47">
+        <v>0.45997238191320972</v>
+      </c>
+      <c r="I47">
+        <v>0.66763969726393779</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>10.899999679679061</v>
+      </c>
+      <c r="B48">
+        <v>2.8636854087499559</v>
+      </c>
+      <c r="C48">
+        <v>14.99442650237954</v>
+      </c>
+      <c r="D48">
+        <v>7.5571907019880609</v>
+      </c>
+      <c r="E48">
+        <v>94.966459164571134</v>
+      </c>
+      <c r="F48">
+        <v>2.433693660257148</v>
+      </c>
+      <c r="G48">
+        <v>19.624040185661201</v>
+      </c>
+      <c r="H48">
+        <v>0.44742418361966868</v>
+      </c>
+      <c r="I48">
+        <v>0.63529230433049011</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>10.99999983141003</v>
+      </c>
+      <c r="B49">
+        <v>3.3045866679701401</v>
+      </c>
+      <c r="C49">
+        <v>14.9942662929165</v>
+      </c>
+      <c r="D49">
+        <v>7.5571099664750054</v>
+      </c>
+      <c r="E49">
+        <v>94.965444612192329</v>
+      </c>
+      <c r="F49">
+        <v>2.3797098645823231</v>
+      </c>
+      <c r="G49">
+        <v>19.624036603869381</v>
+      </c>
+      <c r="H49">
+        <v>0.43532429899766661</v>
+      </c>
+      <c r="I49">
+        <v>0.6072776984914261</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>11.249999873557529</v>
+      </c>
+      <c r="B50">
+        <v>4.2263915332770612</v>
+      </c>
+      <c r="C50">
+        <v>14.99402191610918</v>
+      </c>
+      <c r="D50">
+        <v>7.5569867983577712</v>
+      </c>
+      <c r="E50">
+        <v>94.963896835983306</v>
+      </c>
+      <c r="F50">
+        <v>2.271612585831408</v>
+      </c>
+      <c r="G50">
+        <v>19.624039161449559</v>
+      </c>
+      <c r="H50">
+        <v>0.40693483145203257</v>
+      </c>
+      <c r="I50">
+        <v>0.54896586649471968</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>11.500000590064889</v>
+      </c>
+      <c r="B51">
+        <v>4.998413158336918</v>
+      </c>
+      <c r="C51">
+        <v>14.994107621270899</v>
+      </c>
+      <c r="D51">
+        <v>7.557029989999636</v>
+      </c>
+      <c r="E51">
+        <v>94.964439598162429</v>
+      </c>
+      <c r="F51">
+        <v>2.1859620635970418</v>
+      </c>
+      <c r="G51">
+        <v>19.624036611571579</v>
+      </c>
+      <c r="H51">
+        <v>0.38096521614444928</v>
+      </c>
+      <c r="I51">
+        <v>0.50137910450446677</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>11.750000632212391</v>
+      </c>
+      <c r="B52">
+        <v>5.6787285204069518</v>
+      </c>
+      <c r="C52">
+        <v>14.99417513840767</v>
+      </c>
+      <c r="D52">
+        <v>7.55706401873522</v>
+      </c>
+      <c r="E52">
+        <v>94.964867215865311</v>
+      </c>
+      <c r="F52">
+        <v>2.114041428475443</v>
+      </c>
+      <c r="G52">
+        <v>19.62403342649651</v>
+      </c>
+      <c r="H52">
+        <v>0.35715716801480241</v>
+      </c>
+      <c r="I52">
+        <v>0.46098297722977882</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>11.99999932564012</v>
+      </c>
+      <c r="B53">
+        <v>6.2952273823116656</v>
+      </c>
+      <c r="C53">
+        <v>14.99417331436236</v>
+      </c>
+      <c r="D53">
+        <v>7.5570631011953946</v>
+      </c>
+      <c r="E53">
+        <v>94.964855685719812</v>
+      </c>
+      <c r="F53">
+        <v>2.0517839785016641</v>
+      </c>
+      <c r="G53">
+        <v>19.624040403528209</v>
+      </c>
+      <c r="H53">
+        <v>0.33529552497480519</v>
+      </c>
+      <c r="I53">
+        <v>0.42596565374114909</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>12.99999949423009</v>
+      </c>
+      <c r="B54">
+        <v>8.37744749154351</v>
+      </c>
+      <c r="C54">
+        <v>14.994762555493629</v>
+      </c>
+      <c r="D54">
+        <v>7.5573600776778038</v>
+      </c>
+      <c r="E54">
+        <v>94.968587602261508</v>
+      </c>
+      <c r="F54">
+        <v>1.861059797211517</v>
+      </c>
+      <c r="G54">
+        <v>19.624042539967569</v>
+      </c>
+      <c r="H54">
+        <v>0.26371868286139633</v>
+      </c>
+      <c r="I54">
+        <v>0.321166310070716</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>13.999999662820059</v>
+      </c>
+      <c r="B55">
+        <v>10.108851903142259</v>
+      </c>
+      <c r="C55">
+        <v>14.99476120800035</v>
+      </c>
+      <c r="D55">
+        <v>7.5573593998954864</v>
+      </c>
+      <c r="E55">
+        <v>94.968579084997685</v>
+      </c>
+      <c r="F55">
+        <v>1.7243821262135071</v>
+      </c>
+      <c r="G55">
+        <v>19.624039626901109</v>
+      </c>
+      <c r="H55">
+        <v>0.21113657854771339</v>
+      </c>
+      <c r="I55">
+        <v>0.25110229971449538</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>14.99999983141003</v>
+      </c>
+      <c r="B56">
+        <v>11.638304625059771</v>
+      </c>
+      <c r="C56">
+        <v>14.99475771471363</v>
+      </c>
+      <c r="D56">
+        <v>7.5573576391530377</v>
+      </c>
+      <c r="E56">
+        <v>94.968556958855544</v>
+      </c>
+      <c r="F56">
+        <v>1.61913070934842</v>
+      </c>
+      <c r="G56">
+        <v>19.62403671087197</v>
+      </c>
+      <c r="H56">
+        <v>0.1716519561494029</v>
+      </c>
+      <c r="I56">
+        <v>0.20141518199116029</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>17.500000252884949</v>
+      </c>
+      <c r="B57">
+        <v>14.95496777992313</v>
+      </c>
+      <c r="C57">
+        <v>14.994826649894099</v>
+      </c>
+      <c r="D57">
+        <v>7.5573923837793187</v>
+      </c>
+      <c r="E57">
+        <v>94.968993572706253</v>
+      </c>
+      <c r="F57">
+        <v>1.4345349522650841</v>
+      </c>
+      <c r="G57">
+        <v>19.624041136819571</v>
+      </c>
+      <c r="H57">
+        <v>0.10808074365648369</v>
+      </c>
+      <c r="I57">
+        <v>0.12565394385216869</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>20.000000674359882</v>
+      </c>
+      <c r="B58">
+        <v>17.842113867554652</v>
+      </c>
+      <c r="C58">
+        <v>14.994827536447771</v>
+      </c>
+      <c r="D58">
+        <v>7.5573928277101352</v>
+      </c>
+      <c r="E58">
+        <v>94.968999151305425</v>
+      </c>
+      <c r="F58">
+        <v>1.314275978544539</v>
+      </c>
+      <c r="G58">
+        <v>19.624047047788959</v>
+      </c>
+      <c r="H58">
+        <v>7.2394936526666065E-2</v>
+      </c>
+      <c r="I58">
+        <v>8.5066970289615726E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>22.499999747115051</v>
+      </c>
+      <c r="B59">
+        <v>20.46627919572235</v>
+      </c>
+      <c r="C59">
+        <v>14.996270082378739</v>
+      </c>
+      <c r="D59">
+        <v>7.5581198675607322</v>
+      </c>
+      <c r="E59">
+        <v>94.978135403519431</v>
+      </c>
+      <c r="F59">
+        <v>1.2297349402320481</v>
+      </c>
+      <c r="G59">
+        <v>19.624053644749921</v>
+      </c>
+      <c r="H59">
+        <v>5.0842442613076078E-2</v>
+      </c>
+      <c r="I59">
+        <v>6.1026445991146802E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>24.999998819870211</v>
+      </c>
+      <c r="B60">
+        <v>22.90524739476103</v>
+      </c>
+      <c r="C60">
+        <v>14.99762687359522</v>
+      </c>
+      <c r="D60">
+        <v>7.558803692002444</v>
+      </c>
+      <c r="E60">
+        <v>94.986728594889144</v>
+      </c>
+      <c r="F60">
+        <v>1.1687398959872559</v>
+      </c>
+      <c r="G60">
+        <v>19.62406335583357</v>
+      </c>
+      <c r="H60">
+        <v>3.7062292017191939E-2</v>
+      </c>
+      <c r="I60">
+        <v>4.5814967351370188E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -15440,41 +16705,41 @@
     <row r="1" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>248</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -15506,7 +16771,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B4">
         <v>5.7859999999999996</v>
@@ -15538,7 +16803,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B5">
         <v>5.5449999999999999</v>
@@ -15570,7 +16835,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B6">
         <v>6.5439999999999996</v>
@@ -15602,7 +16867,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B7">
         <v>6.2080000000000002</v>
@@ -15634,7 +16899,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B8">
         <v>10.603999999999999</v>
@@ -15666,7 +16931,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B9">
         <v>0.81200000000000006</v>
@@ -15698,7 +16963,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B10">
         <v>4.593</v>
@@ -15730,7 +16995,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -15762,7 +17027,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B12">
         <v>6.5819999999999999</v>
@@ -15794,7 +17059,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B13">
         <v>5.3879999999999999</v>
@@ -15826,7 +17091,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B14">
         <v>5.4859999999999998</v>
@@ -15858,7 +17123,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B15">
         <v>3.9449999999999998</v>

</xml_diff>

<commit_message>
fix a couple tests
</commit_message>
<xml_diff>
--- a/Documentation/IEA-15-240-RWT_tabular.xlsx
+++ b/Documentation/IEA-15-240-RWT_tabular.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gbarter/devel/IEA-15-240-RWT/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BBDEF3D-93F5-A54C-A4B7-5E6C11810AA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F42082-12A9-E94B-B12B-38A54CC5D1BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3580" yWindow="460" windowWidth="14200" windowHeight="17600" firstSheet="16" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -1262,7 +1262,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
@@ -21702,8 +21702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -22629,7 +22629,7 @@
         <v>272</v>
       </c>
       <c r="B19">
-        <v>646895.52796092397</v>
+        <v>646895</v>
       </c>
       <c r="C19">
         <v>-4.7257053985649007</v>
@@ -22853,7 +22853,7 @@
         <v>5.5497643096623923</v>
       </c>
       <c r="F23">
-        <v>973519.39936530218</v>
+        <v>973520</v>
       </c>
       <c r="G23">
         <v>619970.06166056427</v>

</xml_diff>

<commit_message>
including the floating tabs
</commit_message>
<xml_diff>
--- a/Documentation/IEA-15-240-RWT_tabular.xlsx
+++ b/Documentation/IEA-15-240-RWT_tabular.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gbarter/devel/IEA-15-240-RWT/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F42082-12A9-E94B-B12B-38A54CC5D1BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B095AE18-6201-DD4B-AE2C-CFE444B2CC76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3580" yWindow="460" windowWidth="14200" windowHeight="17600" firstSheet="16" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3580" yWindow="500" windowWidth="25940" windowHeight="21300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -28,16 +28,17 @@
     <sheet name="Shear Web Layup" sheetId="13" r:id="rId13"/>
     <sheet name="Blade Structural Properties" sheetId="14" r:id="rId14"/>
     <sheet name="Tower Properties" sheetId="15" r:id="rId15"/>
-    <sheet name="Material Properties" sheetId="16" r:id="rId16"/>
-    <sheet name="Rotor Performance" sheetId="17" r:id="rId17"/>
-    <sheet name="Nacelle Mass Properties" sheetId="18" r:id="rId18"/>
+    <sheet name="Floating Tower Properties" sheetId="19" r:id="rId16"/>
+    <sheet name="Material Properties" sheetId="16" r:id="rId17"/>
+    <sheet name="Rotor Performance" sheetId="17" r:id="rId18"/>
+    <sheet name="Nacelle Mass Properties" sheetId="18" r:id="rId19"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="287">
   <si>
     <t>Parameter</t>
   </si>
@@ -872,6 +873,33 @@
   <si>
     <t>RNA</t>
   </si>
+  <si>
+    <t>Floating tower mass [t]</t>
+  </si>
+  <si>
+    <t>Floating tower base diameter [m]</t>
+  </si>
+  <si>
+    <t>Floating transition piece height [m]</t>
+  </si>
+  <si>
+    <t>Volturn-S hull mass [t]</t>
+  </si>
+  <si>
+    <t>Volturn-S fixed ballast mass [t]</t>
+  </si>
+  <si>
+    <t>Volturn-S fluid ballast mass [t]</t>
+  </si>
+  <si>
+    <t>Volturn-S displacement [m^3]</t>
+  </si>
+  <si>
+    <t>Volturn-S freeboard [m]</t>
+  </si>
+  <si>
+    <t>Volturn-S draft [m]</t>
+  </si>
 </sst>
 </file>
 
@@ -1260,10 +1288,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1558,6 +1586,78 @@
       </c>
       <c r="B36">
         <v>1319.239060348589</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>278</v>
+      </c>
+      <c r="B37">
+        <v>1483.073634074095</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>279</v>
+      </c>
+      <c r="B38">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>280</v>
+      </c>
+      <c r="B39">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>281</v>
+      </c>
+      <c r="B40">
+        <v>4014.227616744387</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>282</v>
+      </c>
+      <c r="B41">
+        <v>2539.9999950000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>283</v>
+      </c>
+      <c r="B42">
+        <v>8444.6854659379842</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>284</v>
+      </c>
+      <c r="B43">
+        <v>17755.490038649681</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>285</v>
+      </c>
+      <c r="B44">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>286</v>
+      </c>
+      <c r="B45">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -18846,6 +18946,714 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F89D003-FE31-0044-B181-C017FE48CC05}">
+  <dimension ref="A1:K21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B2">
+        <v>15</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>88.528000000000006</v>
+      </c>
+      <c r="E2">
+        <v>21501.229098279051</v>
+      </c>
+      <c r="F2">
+        <v>264048.83909909509</v>
+      </c>
+      <c r="G2">
+        <v>264048.83909909509</v>
+      </c>
+      <c r="H2">
+        <v>6770483053822.9512</v>
+      </c>
+      <c r="I2">
+        <v>6770483053822.9512</v>
+      </c>
+      <c r="J2">
+        <v>5368993061681.6006</v>
+      </c>
+      <c r="K2">
+        <v>551313566622.53979</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>28</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>88.528000000000006</v>
+      </c>
+      <c r="E3">
+        <v>21501.229098279051</v>
+      </c>
+      <c r="F3">
+        <v>264048.83909909509</v>
+      </c>
+      <c r="G3">
+        <v>264048.83909909509</v>
+      </c>
+      <c r="H3">
+        <v>6770483053822.9512</v>
+      </c>
+      <c r="I3">
+        <v>6770483053822.9512</v>
+      </c>
+      <c r="J3">
+        <v>5368993061681.6006</v>
+      </c>
+      <c r="K3">
+        <v>551313566622.53979</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>28.001000000000001</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>78.376999999999995</v>
+      </c>
+      <c r="E4">
+        <v>19055.301833420239</v>
+      </c>
+      <c r="F4">
+        <v>234486.7933995277</v>
+      </c>
+      <c r="G4">
+        <v>234486.7933995277</v>
+      </c>
+      <c r="H4">
+        <v>6012481882039.1729</v>
+      </c>
+      <c r="I4">
+        <v>6012481882039.1729</v>
+      </c>
+      <c r="J4">
+        <v>4767898132457.0635</v>
+      </c>
+      <c r="K4">
+        <v>488597482908.21118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>41</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>78.376999999999995</v>
+      </c>
+      <c r="E5">
+        <v>19055.301833420239</v>
+      </c>
+      <c r="F5">
+        <v>234486.7933995277</v>
+      </c>
+      <c r="G5">
+        <v>234486.7933995277</v>
+      </c>
+      <c r="H5">
+        <v>6012481882039.1729</v>
+      </c>
+      <c r="I5">
+        <v>6012481882039.1729</v>
+      </c>
+      <c r="J5">
+        <v>4767898132457.0635</v>
+      </c>
+      <c r="K5">
+        <v>488597482908.21118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>41.000999999999998</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>68.146000000000001</v>
+      </c>
+      <c r="E6">
+        <v>16584.988359070299</v>
+      </c>
+      <c r="F6">
+        <v>204506.10760939261</v>
+      </c>
+      <c r="G6">
+        <v>204506.10760939261</v>
+      </c>
+      <c r="H6">
+        <v>5243746348958.7842</v>
+      </c>
+      <c r="I6">
+        <v>5243746348958.7842</v>
+      </c>
+      <c r="J6">
+        <v>4158290854724.3159</v>
+      </c>
+      <c r="K6">
+        <v>425256111771.03339</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>54</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="D7">
+        <v>68.146000000000001</v>
+      </c>
+      <c r="E7">
+        <v>16584.988359070299</v>
+      </c>
+      <c r="F7">
+        <v>204506.10760939261</v>
+      </c>
+      <c r="G7">
+        <v>204506.10760939261</v>
+      </c>
+      <c r="H7">
+        <v>5243746348958.7842</v>
+      </c>
+      <c r="I7">
+        <v>5243746348958.7842</v>
+      </c>
+      <c r="J7">
+        <v>4158290854724.3159</v>
+      </c>
+      <c r="K7">
+        <v>425256111771.03339</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>54.000999999999998</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>57.781999999999996</v>
+      </c>
+      <c r="E8">
+        <v>14077.331148695441</v>
+      </c>
+      <c r="F8">
+        <v>173944.84869346919</v>
+      </c>
+      <c r="G8">
+        <v>173944.84869346919</v>
+      </c>
+      <c r="H8">
+        <v>4460124325473.5674</v>
+      </c>
+      <c r="I8">
+        <v>4460124325473.5674</v>
+      </c>
+      <c r="J8">
+        <v>3536878590100.5391</v>
+      </c>
+      <c r="K8">
+        <v>360957208940.90863</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <v>67</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>57.781999999999996</v>
+      </c>
+      <c r="E9">
+        <v>14077.331148695441</v>
+      </c>
+      <c r="F9">
+        <v>173944.84869346919</v>
+      </c>
+      <c r="G9">
+        <v>173944.84869346919</v>
+      </c>
+      <c r="H9">
+        <v>4460124325473.5674</v>
+      </c>
+      <c r="I9">
+        <v>4460124325473.5674</v>
+      </c>
+      <c r="J9">
+        <v>3536878590100.5391</v>
+      </c>
+      <c r="K9">
+        <v>360957208940.90863</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>67.001000000000005</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <v>47.296999999999997</v>
+      </c>
+      <c r="E10">
+        <v>11535.04025774993</v>
+      </c>
+      <c r="F10">
+        <v>142830.52221336699</v>
+      </c>
+      <c r="G10">
+        <v>142830.52221336699</v>
+      </c>
+      <c r="H10">
+        <v>3662321082394.0249</v>
+      </c>
+      <c r="I10">
+        <v>3662321082394.0249</v>
+      </c>
+      <c r="J10">
+        <v>2904220618338.4619</v>
+      </c>
+      <c r="K10">
+        <v>295770263019.22913</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <v>80</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>47.296999999999997</v>
+      </c>
+      <c r="E11">
+        <v>11535.04025774993</v>
+      </c>
+      <c r="F11">
+        <v>142830.52221336699</v>
+      </c>
+      <c r="G11">
+        <v>142830.52221336699</v>
+      </c>
+      <c r="H11">
+        <v>3662321082394.0249</v>
+      </c>
+      <c r="I11">
+        <v>3662321082394.0249</v>
+      </c>
+      <c r="J11">
+        <v>2904220618338.4619</v>
+      </c>
+      <c r="K11">
+        <v>295770263019.22913</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <v>80.001000000000005</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <v>36.875999999999998</v>
+      </c>
+      <c r="E12">
+        <v>9002.9288352438489</v>
+      </c>
+      <c r="F12">
+        <v>111709.691065509</v>
+      </c>
+      <c r="G12">
+        <v>111709.691065509</v>
+      </c>
+      <c r="H12">
+        <v>2864351052961.77</v>
+      </c>
+      <c r="I12">
+        <v>2864351052961.77</v>
+      </c>
+      <c r="J12">
+        <v>2271430384998.6831</v>
+      </c>
+      <c r="K12">
+        <v>230844329108.81671</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <v>93</v>
+      </c>
+      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="D13">
+        <v>36.875999999999998</v>
+      </c>
+      <c r="E13">
+        <v>9002.9288352438489</v>
+      </c>
+      <c r="F13">
+        <v>111709.691065509</v>
+      </c>
+      <c r="G13">
+        <v>111709.691065509</v>
+      </c>
+      <c r="H13">
+        <v>2864351052961.77</v>
+      </c>
+      <c r="I13">
+        <v>2864351052961.77</v>
+      </c>
+      <c r="J13">
+        <v>2271430384998.6831</v>
+      </c>
+      <c r="K13">
+        <v>230844329108.81671</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <v>93.001000000000005</v>
+      </c>
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <v>26.873000000000001</v>
+      </c>
+      <c r="E14">
+        <v>6567.3774435858404</v>
+      </c>
+      <c r="F14">
+        <v>81652.190880971466</v>
+      </c>
+      <c r="G14">
+        <v>81652.190880971466</v>
+      </c>
+      <c r="H14">
+        <v>2093645920024.9089</v>
+      </c>
+      <c r="I14">
+        <v>2093645920024.9089</v>
+      </c>
+      <c r="J14">
+        <v>1660261214579.7529</v>
+      </c>
+      <c r="K14">
+        <v>168394293425.27802</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <v>106</v>
+      </c>
+      <c r="C15">
+        <v>10</v>
+      </c>
+      <c r="D15">
+        <v>26.873000000000001</v>
+      </c>
+      <c r="E15">
+        <v>6567.3774435858404</v>
+      </c>
+      <c r="F15">
+        <v>81652.190880971466</v>
+      </c>
+      <c r="G15">
+        <v>81652.190880971466</v>
+      </c>
+      <c r="H15">
+        <v>2093645920024.9089</v>
+      </c>
+      <c r="I15">
+        <v>2093645920024.9089</v>
+      </c>
+      <c r="J15">
+        <v>1660261214579.7529</v>
+      </c>
+      <c r="K15">
+        <v>168394293425.27802</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>106.001</v>
+      </c>
+      <c r="C16">
+        <v>10</v>
+      </c>
+      <c r="D16">
+        <v>17.748999999999999</v>
+      </c>
+      <c r="E16">
+        <v>4341.5704298743331</v>
+      </c>
+      <c r="F16">
+        <v>54077.325967507757</v>
+      </c>
+      <c r="G16">
+        <v>54077.325967507757</v>
+      </c>
+      <c r="H16">
+        <v>1386598101730.969</v>
+      </c>
+      <c r="I16">
+        <v>1386598101730.969</v>
+      </c>
+      <c r="J16">
+        <v>1099572294672.658</v>
+      </c>
+      <c r="K16">
+        <v>111322318714.7265</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>119</v>
+      </c>
+      <c r="C17">
+        <v>10</v>
+      </c>
+      <c r="D17">
+        <v>17.748999999999999</v>
+      </c>
+      <c r="E17">
+        <v>4341.5704298743331</v>
+      </c>
+      <c r="F17">
+        <v>54077.325967507757</v>
+      </c>
+      <c r="G17">
+        <v>54077.325967507757</v>
+      </c>
+      <c r="H17">
+        <v>1386598101730.969</v>
+      </c>
+      <c r="I17">
+        <v>1386598101730.969</v>
+      </c>
+      <c r="J17">
+        <v>1099572294672.658</v>
+      </c>
+      <c r="K17">
+        <v>111322318714.7265</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>119.001</v>
+      </c>
+      <c r="C18">
+        <v>10</v>
+      </c>
+      <c r="D18">
+        <v>9.9109999999999996</v>
+      </c>
+      <c r="E18">
+        <v>2426.2263151018619</v>
+      </c>
+      <c r="F18">
+        <v>30267.772697042441</v>
+      </c>
+      <c r="G18">
+        <v>30267.772697042441</v>
+      </c>
+      <c r="H18">
+        <v>776096735821.6012</v>
+      </c>
+      <c r="I18">
+        <v>776096735821.6012</v>
+      </c>
+      <c r="J18">
+        <v>615444711506.52966</v>
+      </c>
+      <c r="K18">
+        <v>62210931156.457993</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <v>132</v>
+      </c>
+      <c r="C19">
+        <v>10</v>
+      </c>
+      <c r="D19">
+        <v>9.9109999999999996</v>
+      </c>
+      <c r="E19">
+        <v>2426.2263151018619</v>
+      </c>
+      <c r="F19">
+        <v>30267.772697042441</v>
+      </c>
+      <c r="G19">
+        <v>30267.772697042441</v>
+      </c>
+      <c r="H19">
+        <v>776096735821.6012</v>
+      </c>
+      <c r="I19">
+        <v>776096735821.6012</v>
+      </c>
+      <c r="J19">
+        <v>615444711506.52966</v>
+      </c>
+      <c r="K19">
+        <v>62210931156.457993</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <v>132.001</v>
+      </c>
+      <c r="C20">
+        <v>10</v>
+      </c>
+      <c r="D20">
+        <v>7.9359999999999999</v>
+      </c>
+      <c r="E20">
+        <v>1943.127694419381</v>
+      </c>
+      <c r="F20">
+        <v>24250.575121376562</v>
+      </c>
+      <c r="G20">
+        <v>24250.575121376562</v>
+      </c>
+      <c r="H20">
+        <v>621809618496.83496</v>
+      </c>
+      <c r="I20">
+        <v>621809618496.83496</v>
+      </c>
+      <c r="J20">
+        <v>493095027467.99011</v>
+      </c>
+      <c r="K20">
+        <v>49823787036.394386</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>188</v>
+      </c>
+      <c r="B21">
+        <v>144.386</v>
+      </c>
+      <c r="C21">
+        <v>6.5</v>
+      </c>
+      <c r="D21">
+        <v>7.9359999999999999</v>
+      </c>
+      <c r="E21">
+        <v>1262.4928495596951</v>
+      </c>
+      <c r="F21">
+        <v>6651.2791319294456</v>
+      </c>
+      <c r="G21">
+        <v>6651.2791319294456</v>
+      </c>
+      <c r="H21">
+        <v>170545618767.42169</v>
+      </c>
+      <c r="I21">
+        <v>170545618767.42169</v>
+      </c>
+      <c r="J21">
+        <v>135242675682.5654</v>
+      </c>
+      <c r="K21">
+        <v>32371611527.171661</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:T12"/>
   <sheetViews>
@@ -19577,7 +20385,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:M51"/>
   <sheetViews>
@@ -21698,11 +22506,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
ensure that rated efficiency is what gets put in tabular data and matches servodyn
</commit_message>
<xml_diff>
--- a/Documentation/IEA-15-240-RWT_tabular.xlsx
+++ b/Documentation/IEA-15-240-RWT_tabular.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gbarter/devel/IEA-15-240-RWT/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B095AE18-6201-DD4B-AE2C-CFE444B2CC76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AB4B38D-8E6A-FA4B-BE06-6DC956873FC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3580" yWindow="500" windowWidth="25940" windowHeight="21300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8380" yWindow="500" windowWidth="25940" windowHeight="19960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -1291,7 +1291,7 @@
   <dimension ref="A1:B45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1489,7 +1489,7 @@
         <v>29</v>
       </c>
       <c r="B24">
-        <v>0.95897999191906358</v>
+        <v>0.95755999999999997</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fix bug in doc excel for fiber misalignment
</commit_message>
<xml_diff>
--- a/Documentation/IEA-15-240-RWT_tabular.xlsx
+++ b/Documentation/IEA-15-240-RWT_tabular.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gbarter/devel/IEA-15-240-RWT/Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pbortolo/work/3_projects/5_IEAtask37/IEA-15-240-RWT/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AB4B38D-8E6A-FA4B-BE06-6DC956873FC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39087379-4F21-784A-ACDD-7599C6D1F435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8380" yWindow="500" windowWidth="25940" windowHeight="19960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2860" yWindow="500" windowWidth="25940" windowHeight="16240" firstSheet="7" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -1290,7 +1290,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -10311,8 +10311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:F168"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="F158" sqref="F158:F163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10418,7 +10418,7 @@
         <v>0.1</v>
       </c>
       <c r="F6">
-        <v>-15.59455301971172</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -10438,7 +10438,7 @@
         <v>0.1</v>
       </c>
       <c r="F7">
-        <v>-15.59455301971172</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -10694,7 +10694,7 @@
         <v>2.0328788083942309</v>
       </c>
       <c r="F23">
-        <v>-15.577952430536181</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -10714,7 +10714,7 @@
         <v>2.0328788083942309</v>
       </c>
       <c r="F24">
-        <v>-15.577952430536181</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -10970,7 +10970,7 @@
         <v>53.226487468284041</v>
       </c>
       <c r="F40">
-        <v>-11.036007844744111</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -10990,7 +10990,7 @@
         <v>53.226487468284041</v>
       </c>
       <c r="F41">
-        <v>-11.036007844744111</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -11246,7 +11246,7 @@
         <v>83.864320039968234</v>
       </c>
       <c r="F57">
-        <v>-7.1822029308274153</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
@@ -11266,7 +11266,7 @@
         <v>83.864320039968234</v>
       </c>
       <c r="F58">
-        <v>-7.1822029308274153</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
@@ -11522,7 +11522,7 @@
         <v>96.371996364289288</v>
       </c>
       <c r="F74">
-        <v>-4.7423286989687901</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
@@ -11542,7 +11542,7 @@
         <v>96.371996364289288</v>
       </c>
       <c r="F75">
-        <v>-4.7423286989687901</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
@@ -11798,7 +11798,7 @@
         <v>95.742119882570222</v>
       </c>
       <c r="F91">
-        <v>-2.5664323958895001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
@@ -11818,7 +11818,7 @@
         <v>95.742119882570222</v>
       </c>
       <c r="F92">
-        <v>-2.5664323958895001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
@@ -12074,7 +12074,7 @@
         <v>87.535859940328749</v>
       </c>
       <c r="F108">
-        <v>-1.220206673847805</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
@@ -12094,7 +12094,7 @@
         <v>87.535859940328749</v>
       </c>
       <c r="F109">
-        <v>-1.220206673847805</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
@@ -12350,7 +12350,7 @@
         <v>77.610646044532388</v>
       </c>
       <c r="F125">
-        <v>-0.1853598799103659</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.2">
@@ -12370,7 +12370,7 @@
         <v>77.610646044532388</v>
       </c>
       <c r="F126">
-        <v>-0.1853598799103659</v>
+        <v>0</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.2">
@@ -12626,7 +12626,7 @@
         <v>43.575027988046173</v>
       </c>
       <c r="F142">
-        <v>1.5657693415317231</v>
+        <v>0</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.2">
@@ -12646,7 +12646,7 @@
         <v>43.575027988046173</v>
       </c>
       <c r="F143">
-        <v>1.5657693415317231</v>
+        <v>0</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.2">
@@ -12902,7 +12902,7 @@
         <v>1.0000000000001239</v>
       </c>
       <c r="F159">
-        <v>1.24238770627297</v>
+        <v>0</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.2">
@@ -12922,7 +12922,7 @@
         <v>1.0000000000001239</v>
       </c>
       <c r="F160">
-        <v>1.24238770627297</v>
+        <v>0</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
change orcina contact email
</commit_message>
<xml_diff>
--- a/Documentation/IEA-15-240-RWT_tabular.xlsx
+++ b/Documentation/IEA-15-240-RWT_tabular.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pbortolo/work/3_projects/5_IEAtask37/IEA-15-240-RWT/Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gbarter/devel/IEA-15-240-RWT/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39087379-4F21-784A-ACDD-7599C6D1F435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7027EE-4502-A140-9E5A-79D6ADDBDF4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2860" yWindow="500" windowWidth="25940" windowHeight="16240" firstSheet="7" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2860" yWindow="500" windowWidth="25940" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -1290,7 +1290,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -10311,7 +10311,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:F168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F158" sqref="F158:F163"/>
     </sheetView>
   </sheetViews>
@@ -14263,7 +14263,7 @@
   <dimension ref="A1:AQ29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16136,134 +16136,134 @@
         <v>461211585.49078351</v>
       </c>
     </row>
-    <row r="17" spans="1:43" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
+    <row r="17" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A17">
         <v>0.4</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17">
         <v>433.87160170581552</v>
       </c>
-      <c r="C17" s="1">
-        <v>0</v>
-      </c>
-      <c r="D17" s="1">
-        <v>0</v>
-      </c>
-      <c r="E17" s="1">
-        <v>0</v>
-      </c>
-      <c r="F17" s="1">
-        <v>0</v>
-      </c>
-      <c r="G17" s="1">
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
         <v>-345.88920172511263</v>
       </c>
-      <c r="H17" s="1">
+      <c r="H17">
         <v>433.87160170581552</v>
       </c>
-      <c r="I17" s="1">
-        <v>0</v>
-      </c>
-      <c r="J17" s="1">
-        <v>0</v>
-      </c>
-      <c r="K17" s="1">
-        <v>0</v>
-      </c>
-      <c r="L17" s="1">
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
         <v>9.3851006664052647</v>
       </c>
-      <c r="M17" s="1">
+      <c r="M17">
         <v>433.87160170581552</v>
       </c>
-      <c r="N17" s="1">
+      <c r="N17">
         <v>345.88920172511263</v>
       </c>
-      <c r="O17" s="1">
+      <c r="O17">
         <v>-9.3851006664052647</v>
       </c>
-      <c r="P17" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="1">
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
         <v>1076.1432859614899</v>
       </c>
-      <c r="R17" s="1">
+      <c r="R17">
         <v>-18.75152324183863</v>
       </c>
-      <c r="S17" s="1">
-        <v>0</v>
-      </c>
-      <c r="T17" s="1">
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17">
         <v>120.1630106896849</v>
       </c>
-      <c r="U17" s="1">
-        <v>0</v>
-      </c>
-      <c r="V17" s="1">
+      <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17">
         <v>1196.306296651172</v>
       </c>
-      <c r="W17" s="1">
+      <c r="W17">
         <v>161609316.90177181</v>
       </c>
-      <c r="X17" s="1">
+      <c r="X17">
         <v>-3309906.622644328</v>
       </c>
-      <c r="Y17" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z17" s="1">
-        <v>0</v>
-      </c>
-      <c r="AA17" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB17" s="1">
+      <c r="Y17">
+        <v>0</v>
+      </c>
+      <c r="Z17">
+        <v>0</v>
+      </c>
+      <c r="AA17">
+        <v>0</v>
+      </c>
+      <c r="AB17">
         <v>14196051.94594522</v>
       </c>
-      <c r="AC17" s="1">
+      <c r="AC17">
         <v>317531903.30316031</v>
       </c>
-      <c r="AD17" s="1">
-        <v>0</v>
-      </c>
-      <c r="AE17" s="1">
-        <v>0</v>
-      </c>
-      <c r="AF17" s="1">
-        <v>0</v>
-      </c>
-      <c r="AG17" s="1">
+      <c r="AD17">
+        <v>0</v>
+      </c>
+      <c r="AE17">
+        <v>0</v>
+      </c>
+      <c r="AF17">
+        <v>0</v>
+      </c>
+      <c r="AG17">
         <v>19104038.486917809</v>
       </c>
-      <c r="AH17" s="1">
+      <c r="AH17">
         <v>21621041012.042068</v>
       </c>
-      <c r="AI17" s="1">
+      <c r="AI17">
         <v>6912268845.2773895</v>
       </c>
-      <c r="AJ17" s="1">
+      <c r="AJ17">
         <v>-151464382.08732221</v>
       </c>
-      <c r="AK17" s="1">
-        <v>0</v>
-      </c>
-      <c r="AL17" s="1">
+      <c r="AK17">
+        <v>0</v>
+      </c>
+      <c r="AL17">
         <v>22217425410.95908</v>
       </c>
-      <c r="AM17" s="1">
+      <c r="AM17">
         <v>-10375272.85350344</v>
       </c>
-      <c r="AN17" s="1">
-        <v>0</v>
-      </c>
-      <c r="AO17" s="1">
+      <c r="AN17">
+        <v>0</v>
+      </c>
+      <c r="AO17">
         <v>8537806429.681531</v>
       </c>
-      <c r="AP17" s="1">
-        <v>0</v>
-      </c>
-      <c r="AQ17" s="1">
+      <c r="AP17">
+        <v>0</v>
+      </c>
+      <c r="AQ17">
         <v>364794590.15720928</v>
       </c>
     </row>

</xml_diff>

<commit_message>
restore some prior values for precision and consistency
</commit_message>
<xml_diff>
--- a/Documentation/IEA-15-240-RWT_tabular.xlsx
+++ b/Documentation/IEA-15-240-RWT_tabular.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gbarter/devel/IEA-15-240-RWT/WISDEM/outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37146820-2700-0444-B4DE-5978EFE10311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14C52078-2913-C746-95F6-C7D54E2C97EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19960" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12980" yWindow="1100" windowWidth="19640" windowHeight="18280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="287">
   <si>
     <t>Parameter</t>
   </si>
@@ -904,6 +904,15 @@
   <si>
     <t>Volturn-S draft [m]</t>
   </si>
+  <si>
+    <t>Floating tower mass [t]</t>
+  </si>
+  <si>
+    <t>Floating tower base diameter [m]</t>
+  </si>
+  <si>
+    <t>Floating transition piece height [m]</t>
+  </si>
 </sst>
 </file>
 
@@ -1292,10 +1301,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1509,7 +1518,7 @@
         <v>31</v>
       </c>
       <c r="B26">
-        <v>68.320470554533344</v>
+        <v>68.41529320106045</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -1517,7 +1526,7 @@
         <v>32</v>
       </c>
       <c r="B27">
-        <v>21.404868284427309</v>
+        <v>21.411423639666431</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -1533,7 +1542,7 @@
         <v>34</v>
       </c>
       <c r="B29">
-        <v>673.65021319469906</v>
+        <v>675.17545401594111</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -1541,7 +1550,7 @@
         <v>35</v>
       </c>
       <c r="B30">
-        <v>947.7243153458943</v>
+        <v>949.78129410589611</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -1594,49 +1603,73 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="B37">
-        <v>4014.227616744387</v>
+        <v>1483.073634074095</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="B38">
-        <v>2539.9999950000001</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="B39">
-        <v>8445.0161490074279</v>
+        <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B40">
-        <v>17755.490038649681</v>
+        <v>4014.227616744387</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B41">
-        <v>15</v>
+        <v>2539.9999950000001</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>280</v>
+      </c>
+      <c r="B42">
+        <v>8445.0161490074279</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>281</v>
+      </c>
+      <c r="B43">
+        <v>17755.490038649681</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>282</v>
+      </c>
+      <c r="B44">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>283</v>
       </c>
-      <c r="B42">
+      <c r="B45">
         <v>20</v>
       </c>
     </row>
@@ -17797,7 +17830,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
@@ -22460,7 +22493,7 @@
   <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -22750,7 +22783,7 @@
         <v>260</v>
       </c>
       <c r="B7">
-        <v>24335.34381095778</v>
+        <v>25860.584632199851</v>
       </c>
       <c r="C7">
         <v>-7.0885261800196817</v>
@@ -22762,13 +22795,13 @@
         <v>5.094493537559762</v>
       </c>
       <c r="F7">
-        <v>17849.710236176819</v>
+        <v>18968.457803955189</v>
       </c>
       <c r="G7">
-        <v>8924.8551180884078</v>
+        <v>9484.2289019775926</v>
       </c>
       <c r="H7">
-        <v>8924.8551180884078</v>
+        <v>9484.2289019775926</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -22780,19 +22813,19 @@
         <v>0</v>
       </c>
       <c r="L7">
-        <v>649348.40898757498</v>
+        <v>690046.93818404677</v>
       </c>
       <c r="M7">
-        <v>1863304.0390137341</v>
+        <v>1980088.3920422411</v>
       </c>
       <c r="N7">
-        <v>1231805.340262336</v>
+        <v>1309009.911662149</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="P7">
-        <v>877881.11557875539</v>
+        <v>932903.14954218478</v>
       </c>
       <c r="Q7">
         <v>0</v>
@@ -23386,52 +23419,52 @@
         <v>272</v>
       </c>
       <c r="B19">
-        <v>645370.28713968187</v>
+        <v>646895</v>
       </c>
       <c r="C19">
-        <v>-4.7201212079367174</v>
+        <v>-4.7257053985649007</v>
       </c>
       <c r="D19">
-        <v>-0.14642963096880149</v>
+        <v>-0.146084381325019</v>
       </c>
       <c r="E19">
-        <v>4.2751235383490496</v>
+        <v>4.277055436957836</v>
       </c>
       <c r="F19">
-        <v>9435311.1636606753</v>
+        <v>9437478.0082388092</v>
       </c>
       <c r="G19">
-        <v>9798039.6062639356</v>
+        <v>9808155.9876425676</v>
       </c>
       <c r="H19">
-        <v>9771315.646363128</v>
+        <v>9780449.1838345043</v>
       </c>
       <c r="I19">
-        <v>446057.7459965077</v>
+        <v>446585.45945450838</v>
       </c>
       <c r="J19">
-        <v>1957666.8663827041</v>
+        <v>1960561.6197482159</v>
       </c>
       <c r="K19">
-        <v>-232316.44141864989</v>
+        <v>-232499.0084123702</v>
       </c>
       <c r="L19">
-        <v>21244375.996959489</v>
+        <v>21285074.52615596</v>
       </c>
       <c r="M19">
-        <v>35971822.493310601</v>
+        <v>36088606.846339099</v>
       </c>
       <c r="N19">
-        <v>24163709.290740822</v>
+        <v>24240913.862140629</v>
       </c>
       <c r="O19">
-        <v>1.746229827404022E-10</v>
+        <v>2.9103830456733698E-10</v>
       </c>
       <c r="P19">
-        <v>14980659.25361947</v>
+        <v>15035681.2875829</v>
       </c>
       <c r="Q19">
-        <v>171688.43162700799</v>
+        <v>171688.4316270081</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
@@ -23492,52 +23525,52 @@
         <v>274</v>
       </c>
       <c r="B21">
-        <v>673650.21319469903</v>
+        <v>675175.45401594113</v>
       </c>
       <c r="C21">
-        <v>-4.5219698882805792</v>
+        <v>-4.5277678129576264</v>
       </c>
       <c r="D21">
-        <v>-0.14028249547481439</v>
+        <v>-0.1399655932720888</v>
       </c>
       <c r="E21">
-        <v>4.095653280383539</v>
+        <v>4.0979096893289224</v>
       </c>
       <c r="F21">
-        <v>9910245.7964229193</v>
+        <v>9912932.9695126321</v>
       </c>
       <c r="G21">
-        <v>10850691.62731188</v>
+        <v>10862814.68794382</v>
       </c>
       <c r="H21">
-        <v>10350146.086076509</v>
+        <v>10360760.95113921</v>
       </c>
       <c r="I21">
-        <v>428118.28383111738</v>
+        <v>428663.57360962109</v>
       </c>
       <c r="J21">
-        <v>2481422.9973048852</v>
+        <v>2485278.2157193492</v>
       </c>
       <c r="K21">
-        <v>-216068.25337643921</v>
+        <v>-216278.59414010291</v>
       </c>
       <c r="L21">
-        <v>21223564.508480519</v>
+        <v>21264289.35982516</v>
       </c>
       <c r="M21">
-        <v>35925695.607846387</v>
+        <v>36042500.993432969</v>
       </c>
       <c r="N21">
-        <v>24138345.120186839</v>
+        <v>24215544.736588061</v>
       </c>
       <c r="O21">
-        <v>786.10167467198335</v>
+        <v>783.47984265355626</v>
       </c>
       <c r="P21">
-        <v>14957708.4222154</v>
+        <v>15012742.581265541</v>
       </c>
       <c r="Q21">
-        <v>170976.4410604788</v>
+        <v>170979.33394991109</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
@@ -23545,25 +23578,25 @@
         <v>275</v>
       </c>
       <c r="B22">
-        <v>204961.41166360001</v>
+        <v>205245.8796031813</v>
       </c>
       <c r="C22">
-        <v>-11.420233625480851</v>
+        <v>-11.42013823115942</v>
       </c>
       <c r="D22">
         <v>0</v>
       </c>
       <c r="E22">
-        <v>5.5497743360095946</v>
+        <v>5.5497643096623923</v>
       </c>
       <c r="F22">
-        <v>349224644.64323473</v>
+        <v>349331591.28845012</v>
       </c>
       <c r="G22">
-        <v>174612322.32161731</v>
+        <v>174665795.64422509</v>
       </c>
       <c r="H22">
-        <v>174612322.32161731</v>
+        <v>174665795.64422509</v>
       </c>
       <c r="I22">
         <v>0</v>
@@ -23575,19 +23608,19 @@
         <v>0</v>
       </c>
       <c r="L22">
-        <v>353629606.04260409</v>
+        <v>353744707.19742173</v>
       </c>
       <c r="M22">
-        <v>207656555.947662</v>
+        <v>207755421.6443069</v>
       </c>
       <c r="N22">
-        <v>203251594.54829261</v>
+        <v>203342305.73533541</v>
       </c>
       <c r="O22">
         <v>0</v>
       </c>
       <c r="P22">
-        <v>-5161574.8090728521</v>
+        <v>-5149236.3370862883</v>
       </c>
       <c r="Q22">
         <v>0</v>
@@ -23598,25 +23631,25 @@
         <v>276</v>
       </c>
       <c r="B23">
-        <v>69112.69048759526</v>
+        <v>69359.960486773678</v>
       </c>
       <c r="C23">
-        <v>-11.420233625480851</v>
+        <v>-11.42013823115942</v>
       </c>
       <c r="D23">
         <v>0</v>
       </c>
       <c r="E23">
-        <v>5.5497743360095946</v>
+        <v>5.5497643096623923</v>
       </c>
       <c r="F23">
-        <v>969656.64106804691</v>
+        <v>973520</v>
       </c>
       <c r="G23">
-        <v>618004.06474673655</v>
+        <v>619970.06166056427</v>
       </c>
       <c r="H23">
-        <v>618004.06474673655</v>
+        <v>619970.06166056427</v>
       </c>
       <c r="I23">
         <v>0</v>
@@ -23628,19 +23661,19 @@
         <v>0</v>
       </c>
       <c r="L23">
-        <v>3094484.9487560252</v>
+        <v>3105935.1785233882</v>
       </c>
       <c r="M23">
-        <v>11760471.675893661</v>
+        <v>11802144.12686028</v>
       </c>
       <c r="N23">
-        <v>9635643.3682056814</v>
+        <v>9669728.347702194</v>
       </c>
       <c r="O23">
         <v>0</v>
       </c>
       <c r="P23">
-        <v>4343786.5951598212</v>
+        <v>4359216.6566996779</v>
       </c>
       <c r="Q23">
         <v>0</v>
@@ -23651,52 +23684,52 @@
         <v>277</v>
       </c>
       <c r="B24">
-        <v>947724.31534589431</v>
+        <v>949781.29410589614</v>
       </c>
       <c r="C24">
-        <v>-6.5168912061801638</v>
+        <v>-6.5205267571977208</v>
       </c>
       <c r="D24">
-        <v>-9.9713947879033385E-2</v>
+        <v>-9.9497993454434844E-2</v>
       </c>
       <c r="E24">
-        <v>4.5161731681679989</v>
+        <v>4.5176776508368102</v>
       </c>
       <c r="F24">
-        <v>477786152.0463897</v>
+        <v>478273025.46803188</v>
       </c>
       <c r="G24">
-        <v>314940913.46909481</v>
+        <v>315385456.23548102</v>
       </c>
       <c r="H24">
-        <v>315943964.79924762</v>
+        <v>316388042.72796369</v>
       </c>
       <c r="I24">
-        <v>616641.00757101178</v>
+        <v>616981.95015628426</v>
       </c>
       <c r="J24">
-        <v>-13752941.93038041</v>
+        <v>-13755590.64260529</v>
       </c>
       <c r="K24">
-        <v>-255807.94331839189</v>
+        <v>-255947.2260466138</v>
       </c>
       <c r="L24">
-        <v>377947655.49984068</v>
+        <v>378114931.73577023</v>
       </c>
       <c r="M24">
-        <v>255342723.2314021</v>
+        <v>255600066.76460019</v>
       </c>
       <c r="N24">
-        <v>237025583.03668511</v>
+        <v>237227578.81962559</v>
       </c>
       <c r="O24">
-        <v>786.10167467198335</v>
+        <v>783.47984265355626</v>
       </c>
       <c r="P24">
-        <v>14139920.20830236</v>
+        <v>14222722.90087894</v>
       </c>
       <c r="Q24">
-        <v>170976.4410604788</v>
+        <v>170979.33394991109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated OF files per changes to drivetrain props
</commit_message>
<xml_diff>
--- a/Documentation/IEA-15-240-RWT_tabular.xlsx
+++ b/Documentation/IEA-15-240-RWT_tabular.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gbarter/devel/IEA-15-240-RWT/WISDEM/outputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gbarter/devel/IEA-15-240-RWT/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB42E668-8BC8-7049-8FA5-527AEF27E6C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81D91865-4193-F240-A7A5-E6E76AB74416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20340" yWindow="500" windowWidth="30720" windowHeight="25140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,20 @@
     <sheet name="Rotor Performance" sheetId="17" r:id="rId18"/>
     <sheet name="Nacelle Mass Properties" sheetId="18" r:id="rId19"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -905,6 +918,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -978,11 +994,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Heading 1" xfId="2" builtinId="16"/>
@@ -1291,7 +1311,7 @@
   <dimension ref="A1:B45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -24078,71 +24098,72 @@
   <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="12.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="12.6640625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="4" t="s">
         <v>254</v>
       </c>
     </row>
@@ -24155,52 +24176,52 @@
       <c r="A3" t="s">
         <v>256</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="5">
         <v>48092.001786537301</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="7">
         <v>-7.0885261800196808</v>
       </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
+      <c r="D3" s="7">
+        <v>0</v>
+      </c>
+      <c r="E3" s="7">
         <v>5.094493537559762</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="5">
         <v>59002.874691857964</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="5">
         <v>29771.954855978249</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="5">
         <v>29771.954855978249</v>
       </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
+      <c r="I3" s="5">
+        <v>0</v>
+      </c>
+      <c r="J3" s="5">
+        <v>0</v>
+      </c>
+      <c r="K3" s="5">
+        <v>0</v>
+      </c>
+      <c r="L3" s="5">
         <v>1306856.7851224421</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="5">
         <v>3694433.844065466</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="5">
         <v>2446579.9336348828</v>
       </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3">
+      <c r="O3" s="5">
+        <v>0</v>
+      </c>
+      <c r="P3" s="5">
         <v>1733681.3241244019</v>
       </c>
-      <c r="Q3">
+      <c r="Q3" s="5">
         <v>0</v>
       </c>
     </row>
@@ -24208,52 +24229,52 @@
       <c r="A4" t="s">
         <v>257</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="5">
         <v>13479.28387693245</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="7">
         <v>-5.8950999055777533</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
+      <c r="D4" s="7">
+        <v>0</v>
+      </c>
+      <c r="E4" s="7">
         <v>4.9690593816385773</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="5">
         <v>16537.3964065115</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="5">
         <v>8344.5191750634949</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="5">
         <v>8344.5191750634949</v>
       </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
+      <c r="I4" s="5">
+        <v>0</v>
+      </c>
+      <c r="J4" s="5">
+        <v>0</v>
+      </c>
+      <c r="K4" s="5">
+        <v>0</v>
+      </c>
+      <c r="L4" s="5">
         <v>349272.30654858239</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="5">
         <v>809603.75452328555</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="5">
         <v>476868.84438121459</v>
       </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4">
+      <c r="O4" s="5">
+        <v>0</v>
+      </c>
+      <c r="P4" s="5">
         <v>393998.33316090098</v>
       </c>
-      <c r="Q4">
+      <c r="Q4" s="5">
         <v>0</v>
       </c>
     </row>
@@ -24261,52 +24282,52 @@
       <c r="A5" t="s">
         <v>258</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="5">
         <v>15734.038486973781</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="7">
         <v>-6.9890739904828534</v>
       </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
+      <c r="D5" s="7">
+        <v>0</v>
+      </c>
+      <c r="E5" s="7">
         <v>5.0840406912329961</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="5">
         <v>33120.151015079799</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="5">
         <v>22906.137697285991</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="5">
         <v>22906.137697285991</v>
       </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
+      <c r="I5" s="5">
+        <v>0</v>
+      </c>
+      <c r="J5" s="5">
+        <v>0</v>
+      </c>
+      <c r="K5" s="5">
+        <v>0</v>
+      </c>
+      <c r="L5" s="5">
         <v>439693.63450568088</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="5">
         <v>1198154.2421317161</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="5">
         <v>791580.75864111481</v>
       </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5">
+      <c r="O5" s="5">
+        <v>0</v>
+      </c>
+      <c r="P5" s="5">
         <v>558011.63821907982</v>
       </c>
-      <c r="Q5">
+      <c r="Q5" s="5">
         <v>0</v>
       </c>
     </row>
@@ -24314,52 +24335,52 @@
       <c r="A6" t="s">
         <v>259</v>
       </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+      <c r="C6" s="7">
         <v>-5.0000301997463072</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
+      <c r="D6" s="7">
+        <v>0</v>
+      </c>
+      <c r="E6" s="7">
         <v>4.8749837646976886</v>
       </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
+      <c r="F6" s="5">
+        <v>0</v>
+      </c>
+      <c r="G6" s="5">
+        <v>0</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0</v>
+      </c>
+      <c r="I6" s="5">
+        <v>0</v>
+      </c>
+      <c r="J6" s="5">
+        <v>0</v>
+      </c>
+      <c r="K6" s="5">
+        <v>0</v>
+      </c>
+      <c r="L6" s="5">
+        <v>0</v>
+      </c>
+      <c r="M6" s="5">
+        <v>0</v>
+      </c>
+      <c r="N6" s="5">
+        <v>0</v>
+      </c>
+      <c r="O6" s="5">
+        <v>0</v>
+      </c>
+      <c r="P6" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="5">
         <v>0</v>
       </c>
     </row>
@@ -24367,52 +24388,52 @@
       <c r="A7" t="s">
         <v>260</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="5">
         <v>24335.359356691049</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="7">
         <v>-7.585787127703818</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
+      <c r="D7" s="7">
+        <v>0</v>
+      </c>
+      <c r="E7" s="7">
         <v>5.1467577691935888</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="5">
         <v>17805.867176710381</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="5">
         <v>8902.9335883551885</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="5">
         <v>8902.9335883551885</v>
       </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
+      <c r="I7" s="5">
+        <v>0</v>
+      </c>
+      <c r="J7" s="5">
+        <v>0</v>
+      </c>
+      <c r="K7" s="5">
+        <v>0</v>
+      </c>
+      <c r="L7" s="5">
         <v>662330.73752616369</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="5">
         <v>2053883.0460989999</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="5">
         <v>1409358.1757495459</v>
       </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7">
+      <c r="O7" s="5">
+        <v>0</v>
+      </c>
+      <c r="P7" s="5">
         <v>949180.67008989316</v>
       </c>
-      <c r="Q7">
+      <c r="Q7" s="5">
         <v>0</v>
       </c>
     </row>
@@ -24420,52 +24441,52 @@
       <c r="A8" t="s">
         <v>261</v>
       </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
+      <c r="B8" s="5">
+        <v>0</v>
+      </c>
+      <c r="C8" s="7">
         <v>-5.0000301997463072</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
+      <c r="D8" s="7">
+        <v>0</v>
+      </c>
+      <c r="E8" s="7">
         <v>4.8749837646976886</v>
       </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-      <c r="Q8">
+      <c r="F8" s="5">
+        <v>0</v>
+      </c>
+      <c r="G8" s="5">
+        <v>0</v>
+      </c>
+      <c r="H8" s="5">
+        <v>0</v>
+      </c>
+      <c r="I8" s="5">
+        <v>0</v>
+      </c>
+      <c r="J8" s="5">
+        <v>0</v>
+      </c>
+      <c r="K8" s="5">
+        <v>0</v>
+      </c>
+      <c r="L8" s="5">
+        <v>0</v>
+      </c>
+      <c r="M8" s="5">
+        <v>0</v>
+      </c>
+      <c r="N8" s="5">
+        <v>0</v>
+      </c>
+      <c r="O8" s="5">
+        <v>0</v>
+      </c>
+      <c r="P8" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="5">
         <v>0</v>
       </c>
     </row>
@@ -24473,52 +24494,52 @@
       <c r="A9" t="s">
         <v>262</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="5">
         <v>130349.2496292837</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="7">
         <v>-6.5166760901829237</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
+      <c r="D9" s="7">
+        <v>0</v>
+      </c>
+      <c r="E9" s="7">
         <v>5.0343896711808611</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="5">
         <v>1836783.845600649</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="5">
         <v>972876.63394495833</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="5">
         <v>972876.63394495833</v>
       </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
+      <c r="I9" s="5">
+        <v>0</v>
+      </c>
+      <c r="J9" s="5">
+        <v>0</v>
+      </c>
+      <c r="K9" s="5">
+        <v>0</v>
+      </c>
+      <c r="L9" s="5">
         <v>5131056.6994807534</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="5">
         <v>9812139.0623499639</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="5">
         <v>6517866.2084698593</v>
       </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-      <c r="P9">
+      <c r="O9" s="5">
+        <v>0</v>
+      </c>
+      <c r="P9" s="5">
         <v>4186623.081909996</v>
       </c>
-      <c r="Q9">
+      <c r="Q9" s="5">
         <v>0</v>
       </c>
     </row>
@@ -24526,52 +24547,52 @@
       <c r="A10" t="s">
         <v>263</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="5">
         <v>238490.15752252701</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="7">
         <v>-6.5166760901829237</v>
       </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
+      <c r="D10" s="7">
+        <v>0</v>
+      </c>
+      <c r="E10" s="7">
         <v>5.0343896711808611</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="5">
         <v>3360624.3988206289</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="5">
         <v>1779998.752117051</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="5">
         <v>1779998.752117051</v>
       </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
+      <c r="I10" s="5">
+        <v>0</v>
+      </c>
+      <c r="J10" s="5">
+        <v>0</v>
+      </c>
+      <c r="K10" s="5">
+        <v>0</v>
+      </c>
+      <c r="L10" s="5">
         <v>9387906.1367551591</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="5">
         <v>17952528.282810051</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="5">
         <v>11925246.544875519</v>
       </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10">
+      <c r="O10" s="5">
+        <v>0</v>
+      </c>
+      <c r="P10" s="5">
         <v>7659947.4191975025</v>
       </c>
-      <c r="Q10">
+      <c r="Q10" s="5">
         <v>0</v>
       </c>
     </row>
@@ -24579,52 +24600,52 @@
       <c r="A11" t="s">
         <v>264</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="5">
         <v>368839.40715181082</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="7">
         <v>-6.5166760901829237</v>
       </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
+      <c r="D11" s="7">
+        <v>0</v>
+      </c>
+      <c r="E11" s="7">
         <v>5.0343896711808611</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="5">
         <v>5197408.2444212781</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="5">
         <v>2752875.3860620102</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="5">
         <v>2752875.3860620102</v>
       </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
+      <c r="I11" s="5">
+        <v>0</v>
+      </c>
+      <c r="J11" s="5">
+        <v>0</v>
+      </c>
+      <c r="K11" s="5">
+        <v>0</v>
+      </c>
+      <c r="L11" s="5">
         <v>14518962.836235911</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="5">
         <v>27764667.345160019</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="5">
         <v>18443112.753345389</v>
       </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-      <c r="P11">
+      <c r="O11" s="5">
+        <v>0</v>
+      </c>
+      <c r="P11" s="5">
         <v>11846570.501107501</v>
       </c>
-      <c r="Q11">
+      <c r="Q11" s="5">
         <v>0</v>
       </c>
     </row>
@@ -24632,52 +24653,52 @@
       <c r="A12" t="s">
         <v>265</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="5">
         <v>9381.2812260099963</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="7">
         <v>-6.5166760901829237</v>
       </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
+      <c r="D12" s="7">
+        <v>0</v>
+      </c>
+      <c r="E12" s="7">
         <v>5.0343896711808611</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="5">
         <v>148718.22498384581</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="5">
         <v>74359.112491922875</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="5">
         <v>74359.112491922875</v>
       </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
+      <c r="I12" s="5">
+        <v>0</v>
+      </c>
+      <c r="J12" s="5">
+        <v>0</v>
+      </c>
+      <c r="K12" s="5">
+        <v>0</v>
+      </c>
+      <c r="L12" s="5">
         <v>385675.07966004609</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="5">
         <v>710523.93052661105</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="5">
         <v>473567.07585041062</v>
       </c>
-      <c r="O12">
-        <v>0</v>
-      </c>
-      <c r="P12">
+      <c r="O12" s="5">
+        <v>0</v>
+      </c>
+      <c r="P12" s="5">
         <v>300046.19557565352</v>
       </c>
-      <c r="Q12">
+      <c r="Q12" s="5">
         <v>0</v>
       </c>
     </row>
@@ -24685,52 +24706,52 @@
       <c r="A13" t="s">
         <v>266</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="5">
         <v>10875.722527829839</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="7">
         <v>-6.044278189882994</v>
       </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
+      <c r="D13" s="7">
+        <v>0</v>
+      </c>
+      <c r="E13" s="7">
         <v>4.9847386511287253</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="5">
         <v>12017.673393251969</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="5">
         <v>10005.66472560345</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="5">
         <v>10005.66472560345</v>
       </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
+      <c r="I13" s="5">
+        <v>0</v>
+      </c>
+      <c r="J13" s="5">
+        <v>0</v>
+      </c>
+      <c r="K13" s="5">
+        <v>0</v>
+      </c>
+      <c r="L13" s="5">
         <v>282231.50407453772</v>
       </c>
-      <c r="M13">
+      <c r="M13" s="5">
         <v>677567.50018944137</v>
       </c>
-      <c r="N13">
+      <c r="N13" s="5">
         <v>407353.66950815573</v>
       </c>
-      <c r="O13">
-        <v>0</v>
-      </c>
-      <c r="P13">
+      <c r="O13" s="5">
+        <v>0</v>
+      </c>
+      <c r="P13" s="5">
         <v>327467.08392047661</v>
       </c>
-      <c r="Q13">
+      <c r="Q13" s="5">
         <v>0</v>
       </c>
     </row>
@@ -24738,52 +24759,52 @@
       <c r="A14" t="s">
         <v>267</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="5">
         <v>42274.274414881816</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="7">
         <v>-1.2807860584197921</v>
       </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
+      <c r="D14" s="7">
+        <v>0</v>
+      </c>
+      <c r="E14" s="7">
         <v>2.5860796726634172</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="5">
         <v>549069.84811508202</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="5">
         <v>664478.67296891147</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="5">
         <v>407774.31000719138</v>
       </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14">
+      <c r="I14" s="5">
+        <v>0</v>
+      </c>
+      <c r="J14" s="5">
         <v>176991.48534691479</v>
       </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
-      <c r="L14">
+      <c r="K14" s="5">
+        <v>0</v>
+      </c>
+      <c r="L14" s="5">
         <v>831792.08184248838</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="5">
         <v>1016548.172944742</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="5">
         <v>477121.57625561551</v>
       </c>
-      <c r="O14">
-        <v>0</v>
-      </c>
-      <c r="P14">
+      <c r="O14" s="5">
+        <v>0</v>
+      </c>
+      <c r="P14" s="5">
         <v>317012.96233042493</v>
       </c>
-      <c r="Q14">
+      <c r="Q14" s="5">
         <v>0</v>
       </c>
     </row>
@@ -24791,52 +24812,52 @@
       <c r="A15" t="s">
         <v>268</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="5">
         <v>48672</v>
       </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
+      <c r="C15" s="7">
+        <v>0</v>
+      </c>
+      <c r="D15" s="7">
+        <v>0</v>
+      </c>
+      <c r="E15" s="7">
+        <v>0</v>
+      </c>
+      <c r="F15" s="5">
         <v>685470.48959999997</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="5">
         <v>685470.48959999997</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="5">
         <v>1370928</v>
       </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15">
+      <c r="I15" s="5">
+        <v>0</v>
+      </c>
+      <c r="J15" s="5">
+        <v>0</v>
+      </c>
+      <c r="K15" s="5">
+        <v>0</v>
+      </c>
+      <c r="L15" s="5">
         <v>685470.48959999997</v>
       </c>
-      <c r="M15">
+      <c r="M15" s="5">
         <v>685470.48959999997</v>
       </c>
-      <c r="N15">
+      <c r="N15" s="5">
         <v>1370928</v>
       </c>
-      <c r="O15">
-        <v>0</v>
-      </c>
-      <c r="P15">
-        <v>0</v>
-      </c>
-      <c r="Q15">
+      <c r="O15" s="5">
+        <v>0</v>
+      </c>
+      <c r="P15" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="5">
         <v>0</v>
       </c>
     </row>
@@ -24844,52 +24865,52 @@
       <c r="A16" t="s">
         <v>269</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="5">
         <v>20554.306180410989</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="7">
         <v>-0.25000150998731557</v>
       </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
+      <c r="D16" s="7">
+        <v>0</v>
+      </c>
+      <c r="E16" s="7">
         <v>5.8395911382049999</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="5">
         <v>1599.012969228992</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="5">
         <v>1175.6525637437401</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="5">
         <v>1175.6525637437401</v>
       </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-      <c r="L16">
+      <c r="I16" s="5">
+        <v>0</v>
+      </c>
+      <c r="J16" s="5">
+        <v>0</v>
+      </c>
+      <c r="K16" s="5">
+        <v>0</v>
+      </c>
+      <c r="L16" s="5">
         <v>702517.80406420305</v>
       </c>
-      <c r="M16">
+      <c r="M16" s="5">
         <v>703379.10331341124</v>
       </c>
-      <c r="N16">
+      <c r="N16" s="5">
         <v>2460.3122184370968</v>
       </c>
-      <c r="O16">
-        <v>0</v>
-      </c>
-      <c r="P16">
+      <c r="O16" s="5">
+        <v>0</v>
+      </c>
+      <c r="P16" s="5">
         <v>30007.367297651359</v>
       </c>
-      <c r="Q16">
+      <c r="Q16" s="5">
         <v>0</v>
       </c>
     </row>
@@ -24897,52 +24918,52 @@
       <c r="A17" t="s">
         <v>270</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="5">
         <v>30635</v>
       </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
+      <c r="C17" s="7">
+        <v>0</v>
+      </c>
+      <c r="D17" s="7">
         <v>-5.0645499999999997</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="7">
         <v>1.8145500000000001</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="5">
         <v>67245.697870724995</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="5">
         <v>67245.697870724995</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="5">
         <v>67245.697870724995</v>
       </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-      <c r="L17">
+      <c r="I17" s="5">
+        <v>0</v>
+      </c>
+      <c r="J17" s="5">
+        <v>0</v>
+      </c>
+      <c r="K17" s="5">
+        <v>0</v>
+      </c>
+      <c r="L17" s="5">
         <v>953891.78410789988</v>
       </c>
-      <c r="M17">
+      <c r="M17" s="5">
         <v>168114.24467681249</v>
       </c>
-      <c r="N17">
+      <c r="N17" s="5">
         <v>853023.23730181227</v>
       </c>
-      <c r="O17">
-        <v>0</v>
-      </c>
-      <c r="P17">
-        <v>0</v>
-      </c>
-      <c r="Q17">
+      <c r="O17" s="5">
+        <v>0</v>
+      </c>
+      <c r="P17" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="5">
         <v>281531.94936858752</v>
       </c>
     </row>
@@ -24950,52 +24971,52 @@
       <c r="A18" t="s">
         <v>271</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="5">
         <v>11983.85</v>
       </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
+      <c r="C18" s="7">
+        <v>0</v>
+      </c>
+      <c r="D18" s="7">
         <v>5.0645499999999997</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="7">
         <v>1.8145500000000001</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="5">
         <v>26305.28338266975</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="5">
         <v>26305.28338266975</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="5">
         <v>26305.28338266975</v>
       </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="J18">
-        <v>0</v>
-      </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-      <c r="L18">
+      <c r="I18" s="5">
+        <v>0</v>
+      </c>
+      <c r="J18" s="5">
+        <v>0</v>
+      </c>
+      <c r="K18" s="5">
+        <v>0</v>
+      </c>
+      <c r="L18" s="5">
         <v>373144.96676942898</v>
       </c>
-      <c r="M18">
+      <c r="M18" s="5">
         <v>65763.208456674387</v>
       </c>
-      <c r="N18">
+      <c r="N18" s="5">
         <v>333687.0416954243</v>
       </c>
-      <c r="O18">
-        <v>0</v>
-      </c>
-      <c r="P18">
-        <v>0</v>
-      </c>
-      <c r="Q18">
+      <c r="O18" s="5">
+        <v>0</v>
+      </c>
+      <c r="P18" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="5">
         <v>-110130.1338808796</v>
       </c>
     </row>
@@ -25003,52 +25024,52 @@
       <c r="A19" t="s">
         <v>272</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="5">
         <v>644856.52500807797</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="7">
         <v>-5.1246947866635502</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="7">
         <v>-0.1464817026257379</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="7">
         <v>4.3145020943890202</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="5">
         <v>9474045.4037341513</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="5">
         <v>10608608.55845475</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="5">
         <v>10536262.431653479</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="5">
         <v>484077.03852444101</v>
       </c>
-      <c r="J19">
+      <c r="J19" s="5">
         <v>2197871.758895677</v>
       </c>
-      <c r="K19">
+      <c r="K19" s="5">
         <v>-236144.67918248361</v>
       </c>
-      <c r="L19">
+      <c r="L19" s="5">
         <v>21491840.01005739</v>
       </c>
-      <c r="M19">
+      <c r="M19" s="5">
         <v>39548108.881687172</v>
       </c>
-      <c r="N19">
+      <c r="N19" s="5">
         <v>27485641.37858199</v>
       </c>
-      <c r="O19">
+      <c r="O19" s="5">
         <v>5.8207660913467407E-11</v>
       </c>
-      <c r="P19">
+      <c r="P19" s="5">
         <v>16455976.07582598</v>
       </c>
-      <c r="Q19">
+      <c r="Q19" s="5">
         <v>171401.81548770779</v>
       </c>
     </row>
@@ -25056,52 +25077,52 @@
       <c r="A20" t="s">
         <v>273</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="5">
         <v>28248.90136716282</v>
       </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-      <c r="L20">
-        <v>0</v>
-      </c>
-      <c r="M20">
-        <v>0</v>
-      </c>
-      <c r="N20">
-        <v>0</v>
-      </c>
-      <c r="O20">
-        <v>0</v>
-      </c>
-      <c r="P20">
-        <v>0</v>
-      </c>
-      <c r="Q20">
+      <c r="C20" s="7">
+        <v>0</v>
+      </c>
+      <c r="D20" s="7">
+        <v>0</v>
+      </c>
+      <c r="E20" s="7">
+        <v>0</v>
+      </c>
+      <c r="F20" s="5">
+        <v>0</v>
+      </c>
+      <c r="G20" s="5">
+        <v>0</v>
+      </c>
+      <c r="H20" s="5">
+        <v>0</v>
+      </c>
+      <c r="I20" s="5">
+        <v>0</v>
+      </c>
+      <c r="J20" s="5">
+        <v>0</v>
+      </c>
+      <c r="K20" s="5">
+        <v>0</v>
+      </c>
+      <c r="L20" s="5">
+        <v>0</v>
+      </c>
+      <c r="M20" s="5">
+        <v>0</v>
+      </c>
+      <c r="N20" s="5">
+        <v>0</v>
+      </c>
+      <c r="O20" s="5">
+        <v>0</v>
+      </c>
+      <c r="P20" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="5">
         <v>0</v>
       </c>
     </row>
@@ -25109,52 +25130,52 @@
       <c r="A21" t="s">
         <v>274</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="5">
         <v>673105.42637524079</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="7">
         <v>-4.909621498152327</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="7">
         <v>-0.14033415573720379</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="7">
         <v>4.1334309882338491</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="5">
         <v>9957241.3195051178</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="5">
         <v>11772170.494625719</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="5">
         <v>11217741.101433801</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="5">
         <v>464613.89610973833</v>
       </c>
-      <c r="J21">
+      <c r="J21" s="5">
         <v>2771143.1450576759</v>
       </c>
-      <c r="K21">
+      <c r="K21" s="5">
         <v>-219758.57772524981</v>
       </c>
-      <c r="L21">
+      <c r="L21" s="5">
         <v>21470672.89266571</v>
       </c>
-      <c r="M21">
+      <c r="M21" s="5">
         <v>39497137.316548608</v>
       </c>
-      <c r="N21">
+      <c r="N21" s="5">
         <v>27455788.18957036</v>
       </c>
-      <c r="O21">
+      <c r="O21" s="5">
         <v>852.6119672296918</v>
       </c>
-      <c r="P21">
+      <c r="P21" s="5">
         <v>16430863.06817811</v>
       </c>
-      <c r="Q21">
+      <c r="Q21" s="5">
         <v>170683.9978865725</v>
       </c>
     </row>
@@ -25162,52 +25183,52 @@
       <c r="A22" t="s">
         <v>275</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="5">
         <v>204961.55078278569</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="7">
         <v>-11.42022628194767</v>
       </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
+      <c r="D22" s="7">
+        <v>0</v>
+      </c>
+      <c r="E22" s="7">
         <v>5.5497735641731554</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="5">
         <v>349225321.01329261</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="5">
         <v>174612660.50664631</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="5">
         <v>174612660.50664631</v>
       </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-      <c r="J22">
-        <v>0</v>
-      </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-      <c r="L22">
+      <c r="I22" s="5">
+        <v>0</v>
+      </c>
+      <c r="J22" s="5">
+        <v>0</v>
+      </c>
+      <c r="K22" s="5">
+        <v>0</v>
+      </c>
+      <c r="L22" s="5">
         <v>353630281.24654222</v>
       </c>
-      <c r="M22">
+      <c r="M22" s="5">
         <v>207656880.42767969</v>
       </c>
-      <c r="N22">
+      <c r="N22" s="5">
         <v>203251920.19442999</v>
       </c>
-      <c r="O22">
-        <v>0</v>
-      </c>
-      <c r="P22">
+      <c r="O22" s="5">
+        <v>0</v>
+      </c>
+      <c r="P22" s="5">
         <v>-5161611.3078898322</v>
       </c>
-      <c r="Q22">
+      <c r="Q22" s="5">
         <v>0</v>
       </c>
     </row>
@@ -25215,52 +25236,52 @@
       <c r="A23" t="s">
         <v>276</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="5">
         <v>69131.420672551787</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="7">
         <v>-11.42022628194767</v>
       </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
+      <c r="D23" s="7">
+        <v>0</v>
+      </c>
+      <c r="E23" s="7">
         <v>5.5497735641731554</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="5">
         <v>969951.70136243373</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="5">
         <v>618151.75307987188</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="5">
         <v>618151.75307987188</v>
       </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
-      <c r="J23">
-        <v>0</v>
-      </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-      <c r="L23">
+      <c r="I23" s="5">
+        <v>0</v>
+      </c>
+      <c r="J23" s="5">
+        <v>0</v>
+      </c>
+      <c r="K23" s="5">
+        <v>0</v>
+      </c>
+      <c r="L23" s="5">
         <v>3095354.696190001</v>
       </c>
-      <c r="M23">
+      <c r="M23" s="5">
         <v>11763626.88942988</v>
       </c>
-      <c r="N23">
+      <c r="N23" s="5">
         <v>9638223.8946023136</v>
       </c>
-      <c r="O23">
-        <v>0</v>
-      </c>
-      <c r="P23">
+      <c r="O23" s="5">
+        <v>0</v>
+      </c>
+      <c r="P23" s="5">
         <v>4344954.9620415894</v>
       </c>
-      <c r="Q23">
+      <c r="Q23" s="5">
         <v>0</v>
       </c>
     </row>
@@ -25268,52 +25289,52 @@
       <c r="A24" t="s">
         <v>277</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="5">
         <v>947198.39783057827</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="7">
         <v>-7.32757651493068</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="7">
         <v>-9.9725339431365481E-2</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="7">
         <v>4.5994034146528691</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="5">
         <v>500563636.70987213</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="5">
         <v>343236240.54460227</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="5">
         <v>344088802.06717718</v>
       </c>
-      <c r="I24">
+      <c r="I24" s="5">
         <v>693013.15743812313</v>
       </c>
-      <c r="J24">
+      <c r="J24" s="5">
         <v>-12763545.71155962</v>
       </c>
-      <c r="K24">
+      <c r="K24" s="5">
         <v>-263774.18482091109</v>
       </c>
-      <c r="L24">
+      <c r="L24" s="5">
         <v>378800134.5900588</v>
       </c>
-      <c r="M24">
+      <c r="M24" s="5">
         <v>272321599.62090337</v>
       </c>
-      <c r="N24">
+      <c r="N24" s="5">
         <v>253146061.51118699</v>
       </c>
-      <c r="O24">
+      <c r="O24" s="5">
         <v>852.6119672296918</v>
       </c>
-      <c r="P24">
+      <c r="P24" s="5">
         <v>19159389.76782107</v>
       </c>
-      <c r="Q24">
+      <c r="Q24" s="5">
         <v>170683.9978865725</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update OF and HAWC2 files with changes to drivetrain properties
</commit_message>
<xml_diff>
--- a/Documentation/IEA-15-240-RWT_tabular.xlsx
+++ b/Documentation/IEA-15-240-RWT_tabular.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gbarter/devel/IEA-15-240-RWT/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81D91865-4193-F240-A7A5-E6E76AB74416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3458DE0-F260-3B46-A514-4CF0BC11A23E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20340" yWindow="500" windowWidth="30720" windowHeight="25140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -919,7 +919,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -1001,8 +1001,8 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Heading 1" xfId="2" builtinId="16"/>
@@ -18025,10 +18025,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:K77"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18184,7 +18184,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B5">
-        <v>-27.5</v>
+        <v>-25</v>
       </c>
       <c r="C5">
         <v>10</v>
@@ -18216,2314 +18216,1162 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B6">
-        <v>-27.498999999999999</v>
+        <v>-24.998999999999999</v>
       </c>
       <c r="C6">
         <v>10</v>
       </c>
       <c r="D6">
-        <v>55.341000000000001</v>
+        <v>53.448999999999998</v>
       </c>
       <c r="E6">
-        <v>14429.960803688969</v>
+        <v>13939.280294147429</v>
       </c>
       <c r="F6">
-        <v>178389.13728831729</v>
+        <v>172388.3576143948</v>
       </c>
       <c r="G6">
-        <v>178389.13728831729</v>
+        <v>172388.3576143948</v>
       </c>
       <c r="H6">
-        <v>4274841535785.2231</v>
+        <v>4131041399817.752</v>
       </c>
       <c r="I6">
-        <v>4274841535785.2231</v>
+        <v>4131041399817.752</v>
       </c>
       <c r="J6">
-        <v>3389949337877.6821</v>
+        <v>3275915830055.478</v>
       </c>
       <c r="K6">
-        <v>345793453239.61108</v>
+        <v>334034993868.85773</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B7">
-        <v>-25</v>
+        <v>-20</v>
       </c>
       <c r="C7">
         <v>10</v>
       </c>
       <c r="D7">
-        <v>55.341000000000001</v>
+        <v>53.448999999999998</v>
       </c>
       <c r="E7">
-        <v>14429.960803688969</v>
+        <v>13939.280294147429</v>
       </c>
       <c r="F7">
-        <v>178389.13728831729</v>
+        <v>172388.3576143948</v>
       </c>
       <c r="G7">
-        <v>178389.13728831729</v>
+        <v>172388.3576143948</v>
       </c>
       <c r="H7">
-        <v>4274841535785.2231</v>
+        <v>4131041399817.752</v>
       </c>
       <c r="I7">
-        <v>4274841535785.2231</v>
+        <v>4131041399817.752</v>
       </c>
       <c r="J7">
-        <v>3389949337877.6821</v>
+        <v>3275915830055.478</v>
       </c>
       <c r="K7">
-        <v>345793453239.61108</v>
+        <v>334034993868.85773</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B8">
-        <v>-24.998999999999999</v>
+        <v>-19.998999999999999</v>
       </c>
       <c r="C8">
         <v>10</v>
       </c>
       <c r="D8">
-        <v>54.395000000000003</v>
+        <v>51.509</v>
       </c>
       <c r="E8">
-        <v>14184.64401337621</v>
+        <v>13435.95631086556</v>
       </c>
       <c r="F8">
-        <v>175389.60832743839</v>
+        <v>166228.18419461499</v>
       </c>
       <c r="G8">
-        <v>175389.60832743839</v>
+        <v>166228.18419461499</v>
       </c>
       <c r="H8">
-        <v>4202962097470.3682</v>
+        <v>3983421619808.6509</v>
       </c>
       <c r="I8">
-        <v>4202962097470.3682</v>
+        <v>3983421619808.6509</v>
       </c>
       <c r="J8">
-        <v>3332948943294.001</v>
+        <v>3158853344508.2598</v>
       </c>
       <c r="K8">
-        <v>339914785846.54242</v>
+        <v>321973551662.24689</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B9">
-        <v>-24.998999999999999</v>
+        <v>-15</v>
       </c>
       <c r="C9">
         <v>10</v>
       </c>
       <c r="D9">
-        <v>54.395000000000003</v>
+        <v>51.509</v>
       </c>
       <c r="E9">
-        <v>14184.64401337621</v>
+        <v>13435.95631086556</v>
       </c>
       <c r="F9">
-        <v>175389.60832743839</v>
+        <v>166228.18419461499</v>
       </c>
       <c r="G9">
-        <v>175389.60832743839</v>
+        <v>166228.18419461499</v>
       </c>
       <c r="H9">
-        <v>4202962097470.3682</v>
+        <v>3983421619808.6509</v>
       </c>
       <c r="I9">
-        <v>4202962097470.3682</v>
+        <v>3983421619808.6509</v>
       </c>
       <c r="J9">
-        <v>3332948943294.001</v>
+        <v>3158853344508.2598</v>
       </c>
       <c r="K9">
-        <v>339914785846.54242</v>
+        <v>321973551662.24689</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B10">
-        <v>-24.998000000000001</v>
+        <v>-14.999000000000001</v>
       </c>
       <c r="C10">
         <v>10</v>
       </c>
       <c r="D10">
-        <v>53.448999999999998</v>
+        <v>49.527000000000001</v>
       </c>
       <c r="E10">
-        <v>13939.280294147429</v>
+        <v>12921.531806218951</v>
       </c>
       <c r="F10">
-        <v>172388.3576143948</v>
+        <v>159927.1596963164</v>
       </c>
       <c r="G10">
-        <v>172388.3576143948</v>
+        <v>159927.1596963164</v>
       </c>
       <c r="H10">
-        <v>4131041399817.752</v>
+        <v>3832426544364.1611</v>
       </c>
       <c r="I10">
-        <v>4131041399817.752</v>
+        <v>3832426544364.1611</v>
       </c>
       <c r="J10">
-        <v>3275915830055.478</v>
+        <v>3039114249680.7788</v>
       </c>
       <c r="K10">
-        <v>334034993868.85773</v>
+        <v>309646101275.31641</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B11">
-        <v>-20</v>
+        <v>-10</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
       <c r="D11">
-        <v>53.448999999999998</v>
+        <v>49.527000000000001</v>
       </c>
       <c r="E11">
-        <v>13939.280294147429</v>
+        <v>12921.531806218951</v>
       </c>
       <c r="F11">
-        <v>172388.3576143948</v>
+        <v>159927.1596963164</v>
       </c>
       <c r="G11">
-        <v>172388.3576143948</v>
+        <v>159927.1596963164</v>
       </c>
       <c r="H11">
-        <v>4131041399817.752</v>
+        <v>3832426544364.1611</v>
       </c>
       <c r="I11">
-        <v>4131041399817.752</v>
+        <v>3832426544364.1611</v>
       </c>
       <c r="J11">
-        <v>3275915830055.478</v>
+        <v>3039114249680.7788</v>
       </c>
       <c r="K11">
-        <v>334034993868.85773</v>
+        <v>309646101275.31641</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B12">
-        <v>-19.998999999999999</v>
+        <v>-9.9990000000000006</v>
       </c>
       <c r="C12">
         <v>10</v>
       </c>
       <c r="D12">
-        <v>52.478999999999999</v>
+        <v>47.517000000000003</v>
       </c>
       <c r="E12">
-        <v>13687.642972652549</v>
+        <v>12399.629567330059</v>
       </c>
       <c r="F12">
-        <v>169309.17671693451</v>
+        <v>153529.38576954859</v>
       </c>
       <c r="G12">
-        <v>169309.17671693451</v>
+        <v>153529.38576954859</v>
       </c>
       <c r="H12">
-        <v>4057253216317.624</v>
+        <v>3679113006698.9839</v>
       </c>
       <c r="I12">
-        <v>4057253216317.624</v>
+        <v>3679113006698.9839</v>
       </c>
       <c r="J12">
-        <v>3217401800539.876</v>
+        <v>2917536614312.2939</v>
       </c>
       <c r="K12">
-        <v>328004863950.45648</v>
+        <v>297139457640.30811</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B13">
-        <v>-19.998999999999999</v>
+        <v>-5</v>
       </c>
       <c r="C13">
         <v>10</v>
       </c>
       <c r="D13">
-        <v>52.478999999999999</v>
+        <v>47.517000000000003</v>
       </c>
       <c r="E13">
-        <v>13687.642972652549</v>
+        <v>12399.629567330059</v>
       </c>
       <c r="F13">
-        <v>169309.17671693451</v>
+        <v>153529.38576954859</v>
       </c>
       <c r="G13">
-        <v>169309.17671693451</v>
+        <v>153529.38576954859</v>
       </c>
       <c r="H13">
-        <v>4057253216317.624</v>
+        <v>3679113006698.9839</v>
       </c>
       <c r="I13">
-        <v>4057253216317.624</v>
+        <v>3679113006698.9839</v>
       </c>
       <c r="J13">
-        <v>3217401800539.876</v>
+        <v>2917536614312.2939</v>
       </c>
       <c r="K13">
-        <v>328004863950.45648</v>
+        <v>297139457640.30811</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B14">
-        <v>-19.998000000000001</v>
+        <v>-4.9989999999999997</v>
       </c>
       <c r="C14">
         <v>10</v>
       </c>
       <c r="D14">
-        <v>51.509</v>
+        <v>45.517000000000003</v>
       </c>
       <c r="E14">
-        <v>13435.95631086556</v>
+        <v>11880.11357474014</v>
       </c>
       <c r="F14">
-        <v>166228.18419461499</v>
+        <v>147155.7051570719</v>
       </c>
       <c r="G14">
-        <v>166228.18419461499</v>
+        <v>147155.7051570719</v>
       </c>
       <c r="H14">
-        <v>3983421619808.6509</v>
+        <v>3526376830986.626</v>
       </c>
       <c r="I14">
-        <v>3983421619808.6509</v>
+        <v>3526376830986.626</v>
       </c>
       <c r="J14">
-        <v>3158853344508.2598</v>
+        <v>2796416826972.395</v>
       </c>
       <c r="K14">
-        <v>321973551662.24689</v>
+        <v>284689996998.32593</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>186</v>
+      </c>
       <c r="B15">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="C15">
         <v>10</v>
       </c>
       <c r="D15">
-        <v>51.509</v>
+        <v>45.517000000000003</v>
       </c>
       <c r="E15">
-        <v>13435.95631086556</v>
+        <v>11880.11357474014</v>
       </c>
       <c r="F15">
-        <v>166228.18419461499</v>
+        <v>147155.7051570719</v>
       </c>
       <c r="G15">
-        <v>166228.18419461499</v>
+        <v>147155.7051570719</v>
       </c>
       <c r="H15">
-        <v>3983421619808.6509</v>
+        <v>3526376830986.626</v>
       </c>
       <c r="I15">
-        <v>3983421619808.6509</v>
+        <v>3526376830986.626</v>
       </c>
       <c r="J15">
-        <v>3158853344508.2598</v>
+        <v>2796416826972.395</v>
       </c>
       <c r="K15">
-        <v>321973551662.24689</v>
+        <v>284689996998.32593</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B16">
-        <v>-14.999000000000001</v>
+        <v>1E-3</v>
       </c>
       <c r="C16">
         <v>10</v>
       </c>
       <c r="D16">
-        <v>50.518000000000001</v>
+        <v>43.527000000000001</v>
       </c>
       <c r="E16">
-        <v>13178.76980844315</v>
+        <v>11362.9869748166</v>
       </c>
       <c r="F16">
-        <v>163078.61815282659</v>
+        <v>140806.22742808619</v>
       </c>
       <c r="G16">
-        <v>163078.61815282659</v>
+        <v>140806.22742808619</v>
       </c>
       <c r="H16">
-        <v>3907946756597.8101</v>
+        <v>3374220642896.8662</v>
       </c>
       <c r="I16">
-        <v>3907946756597.8101</v>
+        <v>3374220642896.8662</v>
       </c>
       <c r="J16">
-        <v>3099001777982.063</v>
+        <v>2675756969817.2139</v>
       </c>
       <c r="K16">
-        <v>315810443528.47241</v>
+        <v>272297794747.58209</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B17">
-        <v>-14.999000000000001</v>
+        <v>5</v>
       </c>
       <c r="C17">
         <v>10</v>
       </c>
       <c r="D17">
-        <v>50.518000000000001</v>
+        <v>43.527000000000001</v>
       </c>
       <c r="E17">
-        <v>13178.76980844315</v>
+        <v>11362.9869748166</v>
       </c>
       <c r="F17">
-        <v>163078.61815282659</v>
+        <v>140806.22742808619</v>
       </c>
       <c r="G17">
-        <v>163078.61815282659</v>
+        <v>140806.22742808619</v>
       </c>
       <c r="H17">
-        <v>3907946756597.8101</v>
+        <v>3374220642896.8662</v>
       </c>
       <c r="I17">
-        <v>3907946756597.8101</v>
+        <v>3374220642896.8662</v>
       </c>
       <c r="J17">
-        <v>3099001777982.063</v>
+        <v>2675756969817.2139</v>
       </c>
       <c r="K17">
-        <v>315810443528.47241</v>
+        <v>272297794747.58209</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B18">
-        <v>-14.997999999999999</v>
+        <v>5.0010000000000003</v>
       </c>
       <c r="C18">
         <v>10</v>
       </c>
       <c r="D18">
-        <v>49.527000000000001</v>
+        <v>42.241999999999997</v>
       </c>
       <c r="E18">
-        <v>12921.531806218951</v>
+        <v>11028.95317461117</v>
       </c>
       <c r="F18">
-        <v>159927.1596963164</v>
+        <v>136702.1220616003</v>
       </c>
       <c r="G18">
-        <v>159927.1596963164</v>
+        <v>136702.1220616003</v>
       </c>
       <c r="H18">
-        <v>3832426544364.1611</v>
+        <v>3275871604639.355</v>
       </c>
       <c r="I18">
-        <v>3832426544364.1611</v>
+        <v>3275871604639.355</v>
       </c>
       <c r="J18">
-        <v>3039114249680.7788</v>
+        <v>2597766182479.0088</v>
       </c>
       <c r="K18">
-        <v>309646101275.31641</v>
+        <v>264293150601.75339</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B19">
-        <v>-10</v>
+        <v>10</v>
       </c>
       <c r="C19">
         <v>10</v>
       </c>
       <c r="D19">
-        <v>49.527000000000001</v>
+        <v>42.241999999999997</v>
       </c>
       <c r="E19">
-        <v>12921.531806218951</v>
+        <v>11028.95317461117</v>
       </c>
       <c r="F19">
-        <v>159927.1596963164</v>
+        <v>136702.1220616003</v>
       </c>
       <c r="G19">
-        <v>159927.1596963164</v>
+        <v>136702.1220616003</v>
       </c>
       <c r="H19">
-        <v>3832426544364.1611</v>
+        <v>3275871604639.355</v>
       </c>
       <c r="I19">
-        <v>3832426544364.1611</v>
+        <v>3275871604639.355</v>
       </c>
       <c r="J19">
-        <v>3039114249680.7788</v>
+        <v>2597766182479.0088</v>
       </c>
       <c r="K19">
-        <v>309646101275.31641</v>
+        <v>264293150601.75339</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B20">
-        <v>-9.9990000000000006</v>
+        <v>10.000999999999999</v>
       </c>
       <c r="C20">
         <v>10</v>
       </c>
       <c r="D20">
-        <v>48.521999999999998</v>
+        <v>41.058</v>
       </c>
       <c r="E20">
-        <v>12660.60716935962</v>
+        <v>10721.09752311486</v>
       </c>
       <c r="F20">
-        <v>156729.2466485856</v>
+        <v>132917.77028131139</v>
       </c>
       <c r="G20">
-        <v>156729.2466485856</v>
+        <v>132917.77028131139</v>
       </c>
       <c r="H20">
-        <v>3755793114032.7241</v>
+        <v>3185185005543.0488</v>
       </c>
       <c r="I20">
-        <v>3755793114032.7241</v>
+        <v>3185185005543.0488</v>
       </c>
       <c r="J20">
-        <v>2978343939427.9502</v>
+        <v>2525851709395.6382</v>
       </c>
       <c r="K20">
-        <v>303393414075.23657</v>
+        <v>256915828495.4436</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>187</v>
+      </c>
       <c r="B21">
-        <v>-9.9990000000000006</v>
+        <v>15</v>
       </c>
       <c r="C21">
         <v>10</v>
       </c>
       <c r="D21">
-        <v>48.521999999999998</v>
+        <v>41.058</v>
       </c>
       <c r="E21">
-        <v>12660.60716935962</v>
+        <v>10721.09752311486</v>
       </c>
       <c r="F21">
-        <v>156729.2466485856</v>
+        <v>132917.77028131139</v>
       </c>
       <c r="G21">
-        <v>156729.2466485856</v>
+        <v>132917.77028131139</v>
       </c>
       <c r="H21">
-        <v>3755793114032.7241</v>
+        <v>3185185005543.0488</v>
       </c>
       <c r="I21">
-        <v>3755793114032.7241</v>
+        <v>3185185005543.0488</v>
       </c>
       <c r="J21">
-        <v>2978343939427.9502</v>
+        <v>2525851709395.6382</v>
       </c>
       <c r="K21">
-        <v>303393414075.23657</v>
+        <v>256915828495.4436</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B22">
-        <v>-9.9979999999999993</v>
+        <v>15.000999999999999</v>
       </c>
       <c r="C22">
         <v>10</v>
       </c>
       <c r="D22">
-        <v>47.517000000000003</v>
+        <v>39.496000000000002</v>
       </c>
       <c r="E22">
-        <v>12399.629567330059</v>
+        <v>10314.844411733609</v>
       </c>
       <c r="F22">
-        <v>153529.38576954859</v>
+        <v>127921.09002862249</v>
       </c>
       <c r="G22">
-        <v>153529.38576954859</v>
+        <v>127921.09002862249</v>
       </c>
       <c r="H22">
-        <v>3679113006698.9839</v>
+        <v>3065446681730.708</v>
       </c>
       <c r="I22">
-        <v>3679113006698.9839</v>
+        <v>3065446681730.708</v>
       </c>
       <c r="J22">
-        <v>2917536614312.2939</v>
+        <v>2430899218612.4521</v>
       </c>
       <c r="K22">
-        <v>297139457640.30811</v>
+        <v>247180551443.41281</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B23">
-        <v>-5</v>
+        <v>28</v>
       </c>
       <c r="C23">
         <v>10</v>
       </c>
       <c r="D23">
-        <v>47.517000000000003</v>
+        <v>39.496000000000002</v>
       </c>
       <c r="E23">
-        <v>12399.629567330059</v>
+        <v>10314.844411733609</v>
       </c>
       <c r="F23">
-        <v>153529.38576954859</v>
+        <v>127921.09002862249</v>
       </c>
       <c r="G23">
-        <v>153529.38576954859</v>
+        <v>127921.09002862249</v>
       </c>
       <c r="H23">
-        <v>3679113006698.9839</v>
+        <v>3065446681730.708</v>
       </c>
       <c r="I23">
-        <v>3679113006698.9839</v>
+        <v>3065446681730.708</v>
       </c>
       <c r="J23">
-        <v>2917536614312.2939</v>
+        <v>2430899218612.4521</v>
       </c>
       <c r="K23">
-        <v>297139457640.30811</v>
+        <v>247180551443.41281</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B24">
-        <v>-4.9989999999999997</v>
+        <v>28.001000000000001</v>
       </c>
       <c r="C24">
         <v>10</v>
       </c>
       <c r="D24">
-        <v>46.517000000000003</v>
+        <v>36.456000000000003</v>
       </c>
       <c r="E24">
-        <v>12139.897790767271</v>
+        <v>9523.8185311774014</v>
       </c>
       <c r="F24">
-        <v>150343.51049342929</v>
+        <v>118182.8952025789</v>
       </c>
       <c r="G24">
-        <v>150343.51049342929</v>
+        <v>118182.8952025789</v>
       </c>
       <c r="H24">
-        <v>3602768044414.792</v>
+        <v>2832084716093.4321</v>
       </c>
       <c r="I24">
-        <v>3602768044414.792</v>
+        <v>2832084716093.4321</v>
       </c>
       <c r="J24">
-        <v>2856995059220.9312</v>
+        <v>2245843179862.0918</v>
       </c>
       <c r="K24">
-        <v>290915355637.84497</v>
+        <v>228224743138.6868</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B25">
-        <v>-4.9989999999999997</v>
+        <v>41</v>
       </c>
       <c r="C25">
-        <v>10</v>
+        <v>9.9260000000000002</v>
       </c>
       <c r="D25">
-        <v>46.517000000000003</v>
+        <v>36.456000000000003</v>
       </c>
       <c r="E25">
-        <v>12139.897790767271</v>
+        <v>9453.0844057189461</v>
       </c>
       <c r="F25">
-        <v>150343.51049342929</v>
+        <v>115569.1673620746</v>
       </c>
       <c r="G25">
-        <v>150343.51049342929</v>
+        <v>115569.1673620746</v>
       </c>
       <c r="H25">
-        <v>3602768044414.792</v>
+        <v>2769450452002.7461</v>
       </c>
       <c r="I25">
-        <v>3602768044414.792</v>
+        <v>2769450452002.7461</v>
       </c>
       <c r="J25">
-        <v>2856995059220.9312</v>
+        <v>2196174208438.178</v>
       </c>
       <c r="K25">
-        <v>290915355637.84497</v>
+        <v>226529700592.35431</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B26">
-        <v>-4.9980000000000002</v>
+        <v>41.000999999999998</v>
       </c>
       <c r="C26">
-        <v>10</v>
+        <v>9.9260000000000002</v>
       </c>
       <c r="D26">
-        <v>45.517000000000003</v>
+        <v>33.779000000000003</v>
       </c>
       <c r="E26">
-        <v>11880.11357474014</v>
+        <v>8761.3060592618385</v>
       </c>
       <c r="F26">
-        <v>147155.7051570719</v>
+        <v>107169.58508948211</v>
       </c>
       <c r="G26">
-        <v>147155.7051570719</v>
+        <v>107169.58508948211</v>
       </c>
       <c r="H26">
-        <v>3526376830986.626</v>
+        <v>2568166429175.2251</v>
       </c>
       <c r="I26">
-        <v>3526376830986.626</v>
+        <v>2568166429175.2251</v>
       </c>
       <c r="J26">
-        <v>2796416826972.395</v>
+        <v>2036555978335.9529</v>
       </c>
       <c r="K26">
-        <v>284689996998.32593</v>
+        <v>209952218050.84689</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>186</v>
-      </c>
       <c r="B27">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="C27">
-        <v>10</v>
+        <v>9.4429999999999996</v>
       </c>
       <c r="D27">
-        <v>45.517000000000003</v>
+        <v>33.779000000000003</v>
       </c>
       <c r="E27">
-        <v>11880.11357474014</v>
+        <v>8333.5243885306409</v>
       </c>
       <c r="F27">
-        <v>147155.7051570719</v>
+        <v>92225.636090311411</v>
       </c>
       <c r="G27">
-        <v>147155.7051570719</v>
+        <v>92225.636090311411</v>
       </c>
       <c r="H27">
-        <v>3526376830986.626</v>
+        <v>2210055981076.2378</v>
       </c>
       <c r="I27">
-        <v>3526376830986.626</v>
+        <v>2210055981076.2378</v>
       </c>
       <c r="J27">
-        <v>2796416826972.395</v>
+        <v>1752574392993.457</v>
       </c>
       <c r="K27">
-        <v>284689996998.32593</v>
+        <v>199701039744.32401</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B28">
-        <v>1E-3</v>
+        <v>54.000999999999998</v>
       </c>
       <c r="C28">
-        <v>10</v>
+        <v>9.4429999999999996</v>
       </c>
       <c r="D28">
-        <v>44.521999999999998</v>
+        <v>32.192</v>
       </c>
       <c r="E28">
-        <v>11621.5762329687</v>
+        <v>7943.339505959193</v>
       </c>
       <c r="F28">
-        <v>143981.92246624999</v>
+        <v>87937.081105321893</v>
       </c>
       <c r="G28">
-        <v>143981.92246624999</v>
+        <v>87937.081105321893</v>
       </c>
       <c r="H28">
-        <v>3450321650281.5718</v>
+        <v>2107286870484.5891</v>
       </c>
       <c r="I28">
-        <v>3450321650281.5718</v>
+        <v>2107286870484.5891</v>
       </c>
       <c r="J28">
-        <v>2736105068673.2871</v>
+        <v>1671078488294.2791</v>
       </c>
       <c r="K28">
-        <v>278494517924.00439</v>
+        <v>190350814904.366</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B29">
-        <v>1E-3</v>
+        <v>67</v>
       </c>
       <c r="C29">
-        <v>10</v>
+        <v>8.8330000000000002</v>
       </c>
       <c r="D29">
-        <v>44.521999999999998</v>
+        <v>32.192</v>
       </c>
       <c r="E29">
-        <v>11621.5762329687</v>
+        <v>7428.4594766741811</v>
       </c>
       <c r="F29">
-        <v>143981.92246624999</v>
+        <v>71921.655457150788</v>
       </c>
       <c r="G29">
-        <v>143981.92246624999</v>
+        <v>71921.655457150788</v>
       </c>
       <c r="H29">
-        <v>3450321650281.5718</v>
+        <v>1723500010954.967</v>
       </c>
       <c r="I29">
-        <v>3450321650281.5718</v>
+        <v>1723500010954.967</v>
       </c>
       <c r="J29">
-        <v>2736105068673.2871</v>
+        <v>1366735508687.2891</v>
       </c>
       <c r="K29">
-        <v>278494517924.00439</v>
+        <v>178012448518.43231</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B30">
-        <v>2E-3</v>
+        <v>67.001000000000005</v>
       </c>
       <c r="C30">
-        <v>10</v>
+        <v>8.8330000000000002</v>
       </c>
       <c r="D30">
-        <v>43.527000000000001</v>
+        <v>30.707999999999998</v>
       </c>
       <c r="E30">
-        <v>11362.9869748166</v>
+        <v>7087.214160266677</v>
       </c>
       <c r="F30">
-        <v>140806.22742808619</v>
+        <v>68640.809682709922</v>
       </c>
       <c r="G30">
-        <v>140806.22742808619</v>
+        <v>68640.809682709922</v>
       </c>
       <c r="H30">
-        <v>3374220642896.8662</v>
+        <v>1644879215976.7529</v>
       </c>
       <c r="I30">
-        <v>3374220642896.8662</v>
+        <v>1644879215976.7529</v>
       </c>
       <c r="J30">
-        <v>2675756969817.2139</v>
+        <v>1304389218269.5649</v>
       </c>
       <c r="K30">
-        <v>272297794747.58209</v>
+        <v>169834990660.59619</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B31">
-        <v>5</v>
+        <v>80</v>
       </c>
       <c r="C31">
-        <v>10</v>
+        <v>8.1509999999999998</v>
       </c>
       <c r="D31">
-        <v>43.527000000000001</v>
+        <v>30.707999999999998</v>
       </c>
       <c r="E31">
-        <v>11362.9869748166</v>
+        <v>6538.0980826244668</v>
       </c>
       <c r="F31">
-        <v>140806.22742808619</v>
+        <v>53890.34303307574</v>
       </c>
       <c r="G31">
-        <v>140806.22742808619</v>
+        <v>53890.34303307574</v>
       </c>
       <c r="H31">
-        <v>3374220642896.8662</v>
+        <v>1291405296742.769</v>
       </c>
       <c r="I31">
-        <v>3374220642896.8662</v>
+        <v>1291405296742.769</v>
       </c>
       <c r="J31">
-        <v>2675756969817.2139</v>
+        <v>1024084400317.016</v>
       </c>
       <c r="K31">
-        <v>272297794747.58209</v>
+        <v>156676206149.63971</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B32">
-        <v>5.0010000000000003</v>
+        <v>80.001000000000005</v>
       </c>
       <c r="C32">
-        <v>10</v>
+        <v>8.1509999999999998</v>
       </c>
       <c r="D32">
-        <v>42.884</v>
+        <v>29.100999999999999</v>
       </c>
       <c r="E32">
-        <v>11195.85092413538</v>
+        <v>6197.1748615481274</v>
       </c>
       <c r="F32">
-        <v>138752.97677141579</v>
+        <v>51100.424514406717</v>
       </c>
       <c r="G32">
-        <v>138752.97677141579</v>
+        <v>51100.424514406717</v>
       </c>
       <c r="H32">
-        <v>3325017416041.5952</v>
+        <v>1224548874057.1941</v>
       </c>
       <c r="I32">
-        <v>3325017416041.5952</v>
+        <v>1224548874057.1941</v>
       </c>
       <c r="J32">
-        <v>2636738810920.9849</v>
+        <v>971067257127.3551</v>
       </c>
       <c r="K32">
-        <v>268292617400.79999</v>
+        <v>148506466847.54681</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B33">
-        <v>5.0010000000000003</v>
+        <v>93</v>
       </c>
       <c r="C33">
-        <v>10</v>
+        <v>7.39</v>
       </c>
       <c r="D33">
-        <v>42.884</v>
+        <v>29.100999999999999</v>
       </c>
       <c r="E33">
-        <v>11195.85092413538</v>
+        <v>5616.5163148661431</v>
       </c>
       <c r="F33">
-        <v>138752.97677141579</v>
+        <v>38040.441011391602</v>
       </c>
       <c r="G33">
-        <v>138752.97677141579</v>
+        <v>38040.441011391602</v>
       </c>
       <c r="H33">
-        <v>3325017416041.5952</v>
+        <v>911584975111.22949</v>
       </c>
       <c r="I33">
-        <v>3325017416041.5952</v>
+        <v>911584975111.22949</v>
       </c>
       <c r="J33">
-        <v>2636738810920.9849</v>
+        <v>722886885263.20496</v>
       </c>
       <c r="K33">
-        <v>268292617400.79999</v>
+        <v>134591812002.54359</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B34">
-        <v>5.0019999999999998</v>
+        <v>93.001000000000005</v>
       </c>
       <c r="C34">
-        <v>10</v>
+        <v>7.39</v>
       </c>
       <c r="D34">
-        <v>42.241999999999997</v>
+        <v>27.213000000000001</v>
       </c>
       <c r="E34">
-        <v>11028.95317461117</v>
+        <v>5253.4779234371445</v>
       </c>
       <c r="F34">
-        <v>136702.1220616003</v>
+        <v>35599.7813771168</v>
       </c>
       <c r="G34">
-        <v>136702.1220616003</v>
+        <v>35599.7813771168</v>
       </c>
       <c r="H34">
-        <v>3275871604639.355</v>
+        <v>853098044023.88684</v>
       </c>
       <c r="I34">
-        <v>3275871604639.355</v>
+        <v>853098044023.88684</v>
       </c>
       <c r="J34">
-        <v>2597766182479.0088</v>
+        <v>676506748910.94226</v>
       </c>
       <c r="K34">
-        <v>264293150601.75339</v>
+        <v>125892114148.985</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B35">
-        <v>10</v>
+        <v>106</v>
       </c>
       <c r="C35">
-        <v>10</v>
+        <v>6.9089999999999998</v>
       </c>
       <c r="D35">
-        <v>42.241999999999997</v>
+        <v>27.213000000000001</v>
       </c>
       <c r="E35">
-        <v>11028.95317461117</v>
+        <v>4910.275969995676</v>
       </c>
       <c r="F35">
-        <v>136702.1220616003</v>
+        <v>29068.669776437349</v>
       </c>
       <c r="G35">
-        <v>136702.1220616003</v>
+        <v>29068.669776437349</v>
       </c>
       <c r="H35">
-        <v>3275871604639.355</v>
+        <v>696589258960.87573</v>
       </c>
       <c r="I35">
-        <v>3275871604639.355</v>
+        <v>696589258960.87573</v>
       </c>
       <c r="J35">
-        <v>2597766182479.0088</v>
+        <v>552395282355.97449</v>
       </c>
       <c r="K35">
-        <v>264293150601.75339</v>
+        <v>117667768272.1226</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B36">
-        <v>10.000999999999999</v>
+        <v>106.001</v>
       </c>
       <c r="C36">
-        <v>10</v>
+        <v>6.9089999999999998</v>
       </c>
       <c r="D36">
-        <v>41.65</v>
+        <v>24.009</v>
       </c>
       <c r="E36">
-        <v>10875.03453793534</v>
+        <v>4334.1676032059768</v>
       </c>
       <c r="F36">
-        <v>134810.28504470401</v>
+        <v>25681.93541283693</v>
       </c>
       <c r="G36">
-        <v>134810.28504470401</v>
+        <v>25681.93541283693</v>
       </c>
       <c r="H36">
-        <v>3230536425705.8242</v>
+        <v>615430994795.99658</v>
       </c>
       <c r="I36">
-        <v>3230536425705.8242</v>
+        <v>615430994795.99658</v>
       </c>
       <c r="J36">
-        <v>2561815385584.7192</v>
+        <v>488036778873.22522</v>
       </c>
       <c r="K36">
-        <v>260604709751.62579</v>
+        <v>103862152005.8945</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B37">
-        <v>10.000999999999999</v>
+        <v>119</v>
       </c>
       <c r="C37">
-        <v>10</v>
+        <v>6.7480000000000002</v>
       </c>
       <c r="D37">
-        <v>41.65</v>
+        <v>24.009</v>
       </c>
       <c r="E37">
-        <v>10875.03453793534</v>
+        <v>4232.8165652574853</v>
       </c>
       <c r="F37">
-        <v>134810.28504470401</v>
+        <v>23922.096893685812</v>
       </c>
       <c r="G37">
-        <v>134810.28504470401</v>
+        <v>23922.096893685812</v>
       </c>
       <c r="H37">
-        <v>3230536425705.8242</v>
+        <v>573258971811.30627</v>
       </c>
       <c r="I37">
-        <v>3230536425705.8242</v>
+        <v>573258971811.30627</v>
       </c>
       <c r="J37">
-        <v>2561815385584.7192</v>
+        <v>454594364646.36578</v>
       </c>
       <c r="K37">
-        <v>260604709751.62579</v>
+        <v>101433418769.6498</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B38">
-        <v>10.002000000000001</v>
+        <v>119.001</v>
       </c>
       <c r="C38">
-        <v>10</v>
+        <v>6.7480000000000002</v>
       </c>
       <c r="D38">
-        <v>41.058</v>
+        <v>20.826000000000001</v>
       </c>
       <c r="E38">
-        <v>10721.09752311486</v>
+        <v>3673.3877898387768</v>
       </c>
       <c r="F38">
-        <v>132917.77028131139</v>
+        <v>20780.03502692196</v>
       </c>
       <c r="G38">
-        <v>132917.77028131139</v>
+        <v>20780.03502692196</v>
       </c>
       <c r="H38">
-        <v>3185185005543.0488</v>
+        <v>497963935464.22137</v>
       </c>
       <c r="I38">
-        <v>3185185005543.0488</v>
+        <v>497963935464.22137</v>
       </c>
       <c r="J38">
-        <v>2525851709395.6382</v>
+        <v>394885400823.12762</v>
       </c>
       <c r="K38">
-        <v>256915828495.4436</v>
+        <v>88027505148.305237</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>187</v>
-      </c>
       <c r="B39">
-        <v>15</v>
+        <v>132</v>
       </c>
       <c r="C39">
-        <v>10</v>
+        <v>6.5720000000000001</v>
       </c>
       <c r="D39">
-        <v>41.058</v>
+        <v>20.826000000000001</v>
       </c>
       <c r="E39">
-        <v>10721.09752311486</v>
+        <v>3577.282612388075</v>
       </c>
       <c r="F39">
-        <v>132917.77028131139</v>
+        <v>19191.367526978469</v>
       </c>
       <c r="G39">
-        <v>132917.77028131139</v>
+        <v>19191.367526978469</v>
       </c>
       <c r="H39">
-        <v>3185185005543.0488</v>
+        <v>459893782098.69342</v>
       </c>
       <c r="I39">
-        <v>3185185005543.0488</v>
+        <v>459893782098.69342</v>
       </c>
       <c r="J39">
-        <v>2525851709395.6382</v>
+        <v>364695769204.26392</v>
       </c>
       <c r="K39">
-        <v>256915828495.4436</v>
+        <v>85724481485.455917</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B40">
-        <v>15.000999999999999</v>
+        <v>132.001</v>
       </c>
       <c r="C40">
-        <v>10</v>
+        <v>6.5720000000000001</v>
       </c>
       <c r="D40">
-        <v>39.496000000000002</v>
+        <v>23.998000000000001</v>
       </c>
       <c r="E40">
-        <v>10314.844411733609</v>
+        <v>4120.1412531729766</v>
       </c>
       <c r="F40">
-        <v>127921.09002862249</v>
+        <v>22082.363701823171</v>
       </c>
       <c r="G40">
-        <v>127921.09002862249</v>
+        <v>22082.363701823171</v>
       </c>
       <c r="H40">
-        <v>3065446681730.708</v>
+        <v>529172386815.79602</v>
       </c>
       <c r="I40">
-        <v>3065446681730.708</v>
+        <v>529172386815.79602</v>
       </c>
       <c r="J40">
-        <v>2430899218612.4521</v>
+        <v>419633702744.92621</v>
       </c>
       <c r="K40">
-        <v>247180551443.41281</v>
+        <v>98733315436.687683</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>188</v>
+      </c>
       <c r="B41">
-        <v>28</v>
+        <v>144.386</v>
       </c>
       <c r="C41">
-        <v>10</v>
+        <v>6.5</v>
       </c>
       <c r="D41">
-        <v>39.496000000000002</v>
+        <v>23.998000000000001</v>
       </c>
       <c r="E41">
-        <v>10314.844411733609</v>
+        <v>4074.8373314227201</v>
       </c>
       <c r="F41">
-        <v>127921.09002862249</v>
+        <v>21361.915922655739</v>
       </c>
       <c r="G41">
-        <v>127921.09002862249</v>
+        <v>21361.915922655739</v>
       </c>
       <c r="H41">
-        <v>3065446681730.708</v>
+        <v>511907882162.8501</v>
       </c>
       <c r="I41">
-        <v>3065446681730.708</v>
+        <v>511907882162.8501</v>
       </c>
       <c r="J41">
-        <v>2430899218612.4521</v>
+        <v>405942950555.14008</v>
       </c>
       <c r="K41">
-        <v>247180551443.41281</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B42">
-        <v>28.001000000000001</v>
-      </c>
-      <c r="C42">
-        <v>10</v>
-      </c>
-      <c r="D42">
-        <v>37.975999999999999</v>
-      </c>
-      <c r="E42">
-        <v>9919.3920495248731</v>
-      </c>
-      <c r="F42">
-        <v>123054.2299165951</v>
-      </c>
-      <c r="G42">
-        <v>123054.2299165951</v>
-      </c>
-      <c r="H42">
-        <v>2948819312643.0649</v>
-      </c>
-      <c r="I42">
-        <v>2948819312643.0649</v>
-      </c>
-      <c r="J42">
-        <v>2338413714925.9512</v>
-      </c>
-      <c r="K42">
-        <v>237704098958.18051</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B43">
-        <v>28.001000000000001</v>
-      </c>
-      <c r="C43">
-        <v>10</v>
-      </c>
-      <c r="D43">
-        <v>37.975999999999999</v>
-      </c>
-      <c r="E43">
-        <v>9919.3920495248731</v>
-      </c>
-      <c r="F43">
-        <v>123054.2299165951</v>
-      </c>
-      <c r="G43">
-        <v>123054.2299165951</v>
-      </c>
-      <c r="H43">
-        <v>2948819312643.0649</v>
-      </c>
-      <c r="I43">
-        <v>2948819312643.0649</v>
-      </c>
-      <c r="J43">
-        <v>2338413714925.9512</v>
-      </c>
-      <c r="K43">
-        <v>237704098958.18051</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B44">
-        <v>28.001999999999999</v>
-      </c>
-      <c r="C44">
-        <v>10</v>
-      </c>
-      <c r="D44">
-        <v>36.456000000000003</v>
-      </c>
-      <c r="E44">
-        <v>9523.8185311774014</v>
-      </c>
-      <c r="F44">
-        <v>118182.8952025789</v>
-      </c>
-      <c r="G44">
-        <v>118182.8952025789</v>
-      </c>
-      <c r="H44">
-        <v>2832084716093.4321</v>
-      </c>
-      <c r="I44">
-        <v>2832084716093.4321</v>
-      </c>
-      <c r="J44">
-        <v>2245843179862.0918</v>
-      </c>
-      <c r="K44">
-        <v>228224743138.6868</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B45">
-        <v>41</v>
-      </c>
-      <c r="C45">
-        <v>9.9260000000000002</v>
-      </c>
-      <c r="D45">
-        <v>36.456000000000003</v>
-      </c>
-      <c r="E45">
-        <v>9453.0844057189461</v>
-      </c>
-      <c r="F45">
-        <v>115569.1673620746</v>
-      </c>
-      <c r="G45">
-        <v>115569.1673620746</v>
-      </c>
-      <c r="H45">
-        <v>2769450452002.7461</v>
-      </c>
-      <c r="I45">
-        <v>2769450452002.7461</v>
-      </c>
-      <c r="J45">
-        <v>2196174208438.178</v>
-      </c>
-      <c r="K45">
-        <v>226529700592.35431</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B46">
-        <v>41.000999999999998</v>
-      </c>
-      <c r="C46">
-        <v>9.9260000000000002</v>
-      </c>
-      <c r="D46">
-        <v>35.118000000000002</v>
-      </c>
-      <c r="E46">
-        <v>9107.3714150505875</v>
-      </c>
-      <c r="F46">
-        <v>111372.6561740015</v>
-      </c>
-      <c r="G46">
-        <v>111372.6561740015</v>
-      </c>
-      <c r="H46">
-        <v>2668887039875.4248</v>
-      </c>
-      <c r="I46">
-        <v>2668887039875.4248</v>
-      </c>
-      <c r="J46">
-        <v>2116427422621.2119</v>
-      </c>
-      <c r="K46">
-        <v>218245181285.65991</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B47">
-        <v>41.000999999999998</v>
-      </c>
-      <c r="C47">
-        <v>9.9260000000000002</v>
-      </c>
-      <c r="D47">
-        <v>35.118000000000002</v>
-      </c>
-      <c r="E47">
-        <v>9107.3714150505875</v>
-      </c>
-      <c r="F47">
-        <v>111372.6561740015</v>
-      </c>
-      <c r="G47">
-        <v>111372.6561740015</v>
-      </c>
-      <c r="H47">
-        <v>2668887039875.4248</v>
-      </c>
-      <c r="I47">
-        <v>2668887039875.4248</v>
-      </c>
-      <c r="J47">
-        <v>2116427422621.2119</v>
-      </c>
-      <c r="K47">
-        <v>218245181285.65991</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B48">
-        <v>41.002000000000002</v>
-      </c>
-      <c r="C48">
-        <v>9.9260000000000002</v>
-      </c>
-      <c r="D48">
-        <v>33.779000000000003</v>
-      </c>
-      <c r="E48">
-        <v>8761.3060592618385</v>
-      </c>
-      <c r="F48">
-        <v>107169.58508948211</v>
-      </c>
-      <c r="G48">
-        <v>107169.58508948211</v>
-      </c>
-      <c r="H48">
-        <v>2568166429175.2251</v>
-      </c>
-      <c r="I48">
-        <v>2568166429175.2251</v>
-      </c>
-      <c r="J48">
-        <v>2036555978335.9529</v>
-      </c>
-      <c r="K48">
-        <v>209952218050.84689</v>
-      </c>
-    </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B49">
-        <v>54</v>
-      </c>
-      <c r="C49">
-        <v>9.4429999999999996</v>
-      </c>
-      <c r="D49">
-        <v>33.779000000000003</v>
-      </c>
-      <c r="E49">
-        <v>8333.5243885306409</v>
-      </c>
-      <c r="F49">
-        <v>92225.636090311411</v>
-      </c>
-      <c r="G49">
-        <v>92225.636090311411</v>
-      </c>
-      <c r="H49">
-        <v>2210055981076.2378</v>
-      </c>
-      <c r="I49">
-        <v>2210055981076.2378</v>
-      </c>
-      <c r="J49">
-        <v>1752574392993.457</v>
-      </c>
-      <c r="K49">
-        <v>199701039744.32401</v>
-      </c>
-    </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B50">
-        <v>54.000999999999998</v>
-      </c>
-      <c r="C50">
-        <v>9.4429999999999996</v>
-      </c>
-      <c r="D50">
-        <v>32.985999999999997</v>
-      </c>
-      <c r="E50">
-        <v>8138.5713878846082</v>
-      </c>
-      <c r="F50">
-        <v>90083.25410621558</v>
-      </c>
-      <c r="G50">
-        <v>90083.25410621558</v>
-      </c>
-      <c r="H50">
-        <v>2158716848938.7871</v>
-      </c>
-      <c r="I50">
-        <v>2158716848938.7871</v>
-      </c>
-      <c r="J50">
-        <v>1711862461208.458</v>
-      </c>
-      <c r="K50">
-        <v>195029268820.62329</v>
-      </c>
-    </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B51">
-        <v>54.000999999999998</v>
-      </c>
-      <c r="C51">
-        <v>9.4429999999999996</v>
-      </c>
-      <c r="D51">
-        <v>32.985999999999997</v>
-      </c>
-      <c r="E51">
-        <v>8138.5713878846082</v>
-      </c>
-      <c r="F51">
-        <v>90083.25410621558</v>
-      </c>
-      <c r="G51">
-        <v>90083.25410621558</v>
-      </c>
-      <c r="H51">
-        <v>2158716848938.7871</v>
-      </c>
-      <c r="I51">
-        <v>2158716848938.7871</v>
-      </c>
-      <c r="J51">
-        <v>1711862461208.458</v>
-      </c>
-      <c r="K51">
-        <v>195029268820.62329</v>
-      </c>
-    </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B52">
-        <v>54.002000000000002</v>
-      </c>
-      <c r="C52">
-        <v>9.4429999999999996</v>
-      </c>
-      <c r="D52">
-        <v>32.192</v>
-      </c>
-      <c r="E52">
-        <v>7943.339505959193</v>
-      </c>
-      <c r="F52">
-        <v>87937.081105321893</v>
-      </c>
-      <c r="G52">
-        <v>87937.081105321893</v>
-      </c>
-      <c r="H52">
-        <v>2107286870484.5891</v>
-      </c>
-      <c r="I52">
-        <v>2107286870484.5891</v>
-      </c>
-      <c r="J52">
-        <v>1671078488294.2791</v>
-      </c>
-      <c r="K52">
-        <v>190350814904.366</v>
-      </c>
-    </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B53">
-        <v>67</v>
-      </c>
-      <c r="C53">
-        <v>8.8330000000000002</v>
-      </c>
-      <c r="D53">
-        <v>32.192</v>
-      </c>
-      <c r="E53">
-        <v>7428.4594766741811</v>
-      </c>
-      <c r="F53">
-        <v>71921.655457150788</v>
-      </c>
-      <c r="G53">
-        <v>71921.655457150788</v>
-      </c>
-      <c r="H53">
-        <v>1723500010954.967</v>
-      </c>
-      <c r="I53">
-        <v>1723500010954.967</v>
-      </c>
-      <c r="J53">
-        <v>1366735508687.2891</v>
-      </c>
-      <c r="K53">
-        <v>178012448518.43231</v>
-      </c>
-    </row>
-    <row r="54" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B54">
-        <v>67.001000000000005</v>
-      </c>
-      <c r="C54">
-        <v>8.8330000000000002</v>
-      </c>
-      <c r="D54">
-        <v>31.45</v>
-      </c>
-      <c r="E54">
-        <v>7257.8512541112013</v>
-      </c>
-      <c r="F54">
-        <v>70281.648937049016</v>
-      </c>
-      <c r="G54">
-        <v>70281.648937049016</v>
-      </c>
-      <c r="H54">
-        <v>1684199591110.688</v>
-      </c>
-      <c r="I54">
-        <v>1684199591110.688</v>
-      </c>
-      <c r="J54">
-        <v>1335570275750.7759</v>
-      </c>
-      <c r="K54">
-        <v>173924065519.0798</v>
-      </c>
-    </row>
-    <row r="55" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B55">
-        <v>67.001000000000005</v>
-      </c>
-      <c r="C55">
-        <v>8.8330000000000002</v>
-      </c>
-      <c r="D55">
-        <v>31.45</v>
-      </c>
-      <c r="E55">
-        <v>7257.8512541112013</v>
-      </c>
-      <c r="F55">
-        <v>70281.648937049016</v>
-      </c>
-      <c r="G55">
-        <v>70281.648937049016</v>
-      </c>
-      <c r="H55">
-        <v>1684199591110.688</v>
-      </c>
-      <c r="I55">
-        <v>1684199591110.688</v>
-      </c>
-      <c r="J55">
-        <v>1335570275750.7759</v>
-      </c>
-      <c r="K55">
-        <v>173924065519.0798</v>
-      </c>
-    </row>
-    <row r="56" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B56">
-        <v>67.001999999999995</v>
-      </c>
-      <c r="C56">
-        <v>8.8330000000000002</v>
-      </c>
-      <c r="D56">
-        <v>30.707999999999998</v>
-      </c>
-      <c r="E56">
-        <v>7087.214160266677</v>
-      </c>
-      <c r="F56">
-        <v>68640.809682709922</v>
-      </c>
-      <c r="G56">
-        <v>68640.809682709922</v>
-      </c>
-      <c r="H56">
-        <v>1644879215976.7529</v>
-      </c>
-      <c r="I56">
-        <v>1644879215976.7529</v>
-      </c>
-      <c r="J56">
-        <v>1304389218269.5649</v>
-      </c>
-      <c r="K56">
-        <v>169834990660.59619</v>
-      </c>
-    </row>
-    <row r="57" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B57">
-        <v>80</v>
-      </c>
-      <c r="C57">
-        <v>8.1509999999999998</v>
-      </c>
-      <c r="D57">
-        <v>30.707999999999998</v>
-      </c>
-      <c r="E57">
-        <v>6538.0980826244668</v>
-      </c>
-      <c r="F57">
-        <v>53890.34303307574</v>
-      </c>
-      <c r="G57">
-        <v>53890.34303307574</v>
-      </c>
-      <c r="H57">
-        <v>1291405296742.769</v>
-      </c>
-      <c r="I57">
-        <v>1291405296742.769</v>
-      </c>
-      <c r="J57">
-        <v>1024084400317.016</v>
-      </c>
-      <c r="K57">
-        <v>156676206149.63971</v>
-      </c>
-    </row>
-    <row r="58" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B58">
-        <v>80.001000000000005</v>
-      </c>
-      <c r="C58">
-        <v>8.1509999999999998</v>
-      </c>
-      <c r="D58">
-        <v>29.904</v>
-      </c>
-      <c r="E58">
-        <v>6367.5473254292383</v>
-      </c>
-      <c r="F58">
-        <v>52494.931303291327</v>
-      </c>
-      <c r="G58">
-        <v>52494.931303291327</v>
-      </c>
-      <c r="H58">
-        <v>1257966242590.2549</v>
-      </c>
-      <c r="I58">
-        <v>1257966242590.2549</v>
-      </c>
-      <c r="J58">
-        <v>997567230374.0719</v>
-      </c>
-      <c r="K58">
-        <v>152589200225.95831</v>
-      </c>
-    </row>
-    <row r="59" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B59">
-        <v>80.001000000000005</v>
-      </c>
-      <c r="C59">
-        <v>8.1509999999999998</v>
-      </c>
-      <c r="D59">
-        <v>29.904</v>
-      </c>
-      <c r="E59">
-        <v>6367.5473254292383</v>
-      </c>
-      <c r="F59">
-        <v>52494.931303291327</v>
-      </c>
-      <c r="G59">
-        <v>52494.931303291327</v>
-      </c>
-      <c r="H59">
-        <v>1257966242590.2549</v>
-      </c>
-      <c r="I59">
-        <v>1257966242590.2549</v>
-      </c>
-      <c r="J59">
-        <v>997567230374.0719</v>
-      </c>
-      <c r="K59">
-        <v>152589200225.95831</v>
-      </c>
-    </row>
-    <row r="60" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B60">
-        <v>80.001999999999995</v>
-      </c>
-      <c r="C60">
-        <v>8.1509999999999998</v>
-      </c>
-      <c r="D60">
-        <v>29.100999999999999</v>
-      </c>
-      <c r="E60">
-        <v>6197.1748615481274</v>
-      </c>
-      <c r="F60">
-        <v>51100.424514406717</v>
-      </c>
-      <c r="G60">
-        <v>51100.424514406717</v>
-      </c>
-      <c r="H60">
-        <v>1224548874057.1941</v>
-      </c>
-      <c r="I60">
-        <v>1224548874057.1941</v>
-      </c>
-      <c r="J60">
-        <v>971067257127.3551</v>
-      </c>
-      <c r="K60">
-        <v>148506466847.54681</v>
-      </c>
-    </row>
-    <row r="61" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B61">
-        <v>93</v>
-      </c>
-      <c r="C61">
-        <v>7.39</v>
-      </c>
-      <c r="D61">
-        <v>29.100999999999999</v>
-      </c>
-      <c r="E61">
-        <v>5616.5163148661431</v>
-      </c>
-      <c r="F61">
-        <v>38040.441011391602</v>
-      </c>
-      <c r="G61">
-        <v>38040.441011391602</v>
-      </c>
-      <c r="H61">
-        <v>911584975111.22949</v>
-      </c>
-      <c r="I61">
-        <v>911584975111.22949</v>
-      </c>
-      <c r="J61">
-        <v>722886885263.20496</v>
-      </c>
-      <c r="K61">
-        <v>134591812002.54359</v>
-      </c>
-    </row>
-    <row r="62" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B62">
-        <v>93.001000000000005</v>
-      </c>
-      <c r="C62">
-        <v>7.39</v>
-      </c>
-      <c r="D62">
-        <v>28.157</v>
-      </c>
-      <c r="E62">
-        <v>5435.0204844990558</v>
-      </c>
-      <c r="F62">
-        <v>36820.582440753249</v>
-      </c>
-      <c r="G62">
-        <v>36820.582440753249</v>
-      </c>
-      <c r="H62">
-        <v>882352802318.55383</v>
-      </c>
-      <c r="I62">
-        <v>882352802318.55383</v>
-      </c>
-      <c r="J62">
-        <v>699705772238.61316</v>
-      </c>
-      <c r="K62">
-        <v>130242522993.02789</v>
-      </c>
-    </row>
-    <row r="63" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B63">
-        <v>93.001000000000005</v>
-      </c>
-      <c r="C63">
-        <v>7.39</v>
-      </c>
-      <c r="D63">
-        <v>28.157</v>
-      </c>
-      <c r="E63">
-        <v>5435.0204844990558</v>
-      </c>
-      <c r="F63">
-        <v>36820.582440753249</v>
-      </c>
-      <c r="G63">
-        <v>36820.582440753249</v>
-      </c>
-      <c r="H63">
-        <v>882352802318.55383</v>
-      </c>
-      <c r="I63">
-        <v>882352802318.55383</v>
-      </c>
-      <c r="J63">
-        <v>699705772238.61316</v>
-      </c>
-      <c r="K63">
-        <v>130242522993.02789</v>
-      </c>
-    </row>
-    <row r="64" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B64">
-        <v>93.001999999999995</v>
-      </c>
-      <c r="C64">
-        <v>7.39</v>
-      </c>
-      <c r="D64">
-        <v>27.213000000000001</v>
-      </c>
-      <c r="E64">
-        <v>5253.4779234371445</v>
-      </c>
-      <c r="F64">
-        <v>35599.7813771168</v>
-      </c>
-      <c r="G64">
-        <v>35599.7813771168</v>
-      </c>
-      <c r="H64">
-        <v>853098044023.88684</v>
-      </c>
-      <c r="I64">
-        <v>853098044023.88684</v>
-      </c>
-      <c r="J64">
-        <v>676506748910.94226</v>
-      </c>
-      <c r="K64">
-        <v>125892114148.985</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B65">
-        <v>106</v>
-      </c>
-      <c r="C65">
-        <v>6.9089999999999998</v>
-      </c>
-      <c r="D65">
-        <v>27.213000000000001</v>
-      </c>
-      <c r="E65">
-        <v>4910.275969995676</v>
-      </c>
-      <c r="F65">
-        <v>29068.669776437349</v>
-      </c>
-      <c r="G65">
-        <v>29068.669776437349</v>
-      </c>
-      <c r="H65">
-        <v>696589258960.87573</v>
-      </c>
-      <c r="I65">
-        <v>696589258960.87573</v>
-      </c>
-      <c r="J65">
-        <v>552395282355.97449</v>
-      </c>
-      <c r="K65">
-        <v>117667768272.1226</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B66">
-        <v>106.001</v>
-      </c>
-      <c r="C66">
-        <v>6.9089999999999998</v>
-      </c>
-      <c r="D66">
-        <v>25.611000000000001</v>
-      </c>
-      <c r="E66">
-        <v>4622.2890770266577</v>
-      </c>
-      <c r="F66">
-        <v>27376.48932322409</v>
-      </c>
-      <c r="G66">
-        <v>27376.48932322409</v>
-      </c>
-      <c r="H66">
-        <v>656038565138.36768</v>
-      </c>
-      <c r="I66">
-        <v>656038565138.36768</v>
-      </c>
-      <c r="J66">
-        <v>520238582154.72559</v>
-      </c>
-      <c r="K66">
-        <v>110766572658.1993</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B67">
-        <v>106.001</v>
-      </c>
-      <c r="C67">
-        <v>6.9089999999999998</v>
-      </c>
-      <c r="D67">
-        <v>25.611000000000001</v>
-      </c>
-      <c r="E67">
-        <v>4622.2890770266577</v>
-      </c>
-      <c r="F67">
-        <v>27376.48932322409</v>
-      </c>
-      <c r="G67">
-        <v>27376.48932322409</v>
-      </c>
-      <c r="H67">
-        <v>656038565138.36768</v>
-      </c>
-      <c r="I67">
-        <v>656038565138.36768</v>
-      </c>
-      <c r="J67">
-        <v>520238582154.72559</v>
-      </c>
-      <c r="K67">
-        <v>110766572658.1993</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B68">
-        <v>106.002</v>
-      </c>
-      <c r="C68">
-        <v>6.9089999999999998</v>
-      </c>
-      <c r="D68">
-        <v>24.009</v>
-      </c>
-      <c r="E68">
-        <v>4334.1676032059768</v>
-      </c>
-      <c r="F68">
-        <v>25681.93541283693</v>
-      </c>
-      <c r="G68">
-        <v>25681.93541283693</v>
-      </c>
-      <c r="H68">
-        <v>615430994795.99658</v>
-      </c>
-      <c r="I68">
-        <v>615430994795.99658</v>
-      </c>
-      <c r="J68">
-        <v>488036778873.22522</v>
-      </c>
-      <c r="K68">
-        <v>103862152005.8945</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B69">
-        <v>119</v>
-      </c>
-      <c r="C69">
-        <v>6.7480000000000002</v>
-      </c>
-      <c r="D69">
-        <v>24.009</v>
-      </c>
-      <c r="E69">
-        <v>4232.8165652574853</v>
-      </c>
-      <c r="F69">
-        <v>23922.096893685812</v>
-      </c>
-      <c r="G69">
-        <v>23922.096893685812</v>
-      </c>
-      <c r="H69">
-        <v>573258971811.30627</v>
-      </c>
-      <c r="I69">
-        <v>573258971811.30627</v>
-      </c>
-      <c r="J69">
-        <v>454594364646.36578</v>
-      </c>
-      <c r="K69">
-        <v>101433418769.6498</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B70">
-        <v>119.001</v>
-      </c>
-      <c r="C70">
-        <v>6.7480000000000002</v>
-      </c>
-      <c r="D70">
-        <v>22.417999999999999</v>
-      </c>
-      <c r="E70">
-        <v>3953.2564663697899</v>
-      </c>
-      <c r="F70">
-        <v>22352.678535921561</v>
-      </c>
-      <c r="G70">
-        <v>22352.678535921561</v>
-      </c>
-      <c r="H70">
-        <v>535650096715.11072</v>
-      </c>
-      <c r="I70">
-        <v>535650096715.11072</v>
-      </c>
-      <c r="J70">
-        <v>424770526695.08282</v>
-      </c>
-      <c r="K70">
-        <v>94734159270.783371</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B71">
-        <v>119.001</v>
-      </c>
-      <c r="C71">
-        <v>6.7480000000000002</v>
-      </c>
-      <c r="D71">
-        <v>22.417999999999999</v>
-      </c>
-      <c r="E71">
-        <v>3953.2564663697899</v>
-      </c>
-      <c r="F71">
-        <v>22352.678535921561</v>
-      </c>
-      <c r="G71">
-        <v>22352.678535921561</v>
-      </c>
-      <c r="H71">
-        <v>535650096715.11072</v>
-      </c>
-      <c r="I71">
-        <v>535650096715.11072</v>
-      </c>
-      <c r="J71">
-        <v>424770526695.08282</v>
-      </c>
-      <c r="K71">
-        <v>94734159270.783371</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B72">
-        <v>119.002</v>
-      </c>
-      <c r="C72">
-        <v>6.7480000000000002</v>
-      </c>
-      <c r="D72">
-        <v>20.826000000000001</v>
-      </c>
-      <c r="E72">
-        <v>3673.3877898387768</v>
-      </c>
-      <c r="F72">
-        <v>20780.03502692196</v>
-      </c>
-      <c r="G72">
-        <v>20780.03502692196</v>
-      </c>
-      <c r="H72">
-        <v>497963935464.22137</v>
-      </c>
-      <c r="I72">
-        <v>497963935464.22137</v>
-      </c>
-      <c r="J72">
-        <v>394885400823.12762</v>
-      </c>
-      <c r="K72">
-        <v>88027505148.305237</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B73">
-        <v>132</v>
-      </c>
-      <c r="C73">
-        <v>6.5720000000000001</v>
-      </c>
-      <c r="D73">
-        <v>20.826000000000001</v>
-      </c>
-      <c r="E73">
-        <v>3577.282612388075</v>
-      </c>
-      <c r="F73">
-        <v>19191.367526978469</v>
-      </c>
-      <c r="G73">
-        <v>19191.367526978469</v>
-      </c>
-      <c r="H73">
-        <v>459893782098.69342</v>
-      </c>
-      <c r="I73">
-        <v>459893782098.69342</v>
-      </c>
-      <c r="J73">
-        <v>364695769204.26392</v>
-      </c>
-      <c r="K73">
-        <v>85724481485.455917</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B74">
-        <v>132.001</v>
-      </c>
-      <c r="C74">
-        <v>6.5720000000000001</v>
-      </c>
-      <c r="D74">
-        <v>22.411999999999999</v>
-      </c>
-      <c r="E74">
-        <v>3848.7778857902158</v>
-      </c>
-      <c r="F74">
-        <v>20637.919313358329</v>
-      </c>
-      <c r="G74">
-        <v>20637.919313358329</v>
-      </c>
-      <c r="H74">
-        <v>494558334851.62543</v>
-      </c>
-      <c r="I74">
-        <v>494558334851.62543</v>
-      </c>
-      <c r="J74">
-        <v>392184759537.33893</v>
-      </c>
-      <c r="K74">
-        <v>92230478930.990097</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B75">
-        <v>132.001</v>
-      </c>
-      <c r="C75">
-        <v>6.5720000000000001</v>
-      </c>
-      <c r="D75">
-        <v>22.411999999999999</v>
-      </c>
-      <c r="E75">
-        <v>3848.7778857902158</v>
-      </c>
-      <c r="F75">
-        <v>20637.919313358329</v>
-      </c>
-      <c r="G75">
-        <v>20637.919313358329</v>
-      </c>
-      <c r="H75">
-        <v>494558334851.62543</v>
-      </c>
-      <c r="I75">
-        <v>494558334851.62543</v>
-      </c>
-      <c r="J75">
-        <v>392184759537.33893</v>
-      </c>
-      <c r="K75">
-        <v>92230478930.990097</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B76">
-        <v>132.00200000000001</v>
-      </c>
-      <c r="C76">
-        <v>6.5720000000000001</v>
-      </c>
-      <c r="D76">
-        <v>23.998000000000001</v>
-      </c>
-      <c r="E76">
-        <v>4120.1412531729766</v>
-      </c>
-      <c r="F76">
-        <v>22082.363701823171</v>
-      </c>
-      <c r="G76">
-        <v>22082.363701823171</v>
-      </c>
-      <c r="H76">
-        <v>529172386815.79602</v>
-      </c>
-      <c r="I76">
-        <v>529172386815.79602</v>
-      </c>
-      <c r="J76">
-        <v>419633702744.92621</v>
-      </c>
-      <c r="K76">
-        <v>98733315436.687683</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
-        <v>188</v>
-      </c>
-      <c r="B77">
-        <v>144.386</v>
-      </c>
-      <c r="C77">
-        <v>6.5</v>
-      </c>
-      <c r="D77">
-        <v>23.998000000000001</v>
-      </c>
-      <c r="E77">
-        <v>4074.8373314227201</v>
-      </c>
-      <c r="F77">
-        <v>21361.915922655739</v>
-      </c>
-      <c r="G77">
-        <v>21361.915922655739</v>
-      </c>
-      <c r="H77">
-        <v>511907882162.8501</v>
-      </c>
-      <c r="I77">
-        <v>511907882162.8501</v>
-      </c>
-      <c r="J77">
-        <v>405942950555.14008</v>
-      </c>
-      <c r="K77">
         <v>97647671493.475189</v>
       </c>
     </row>
@@ -24098,7 +22946,7 @@
   <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fix column labels for shear and poisson ratios
</commit_message>
<xml_diff>
--- a/Documentation/IEA-15-240-RWT_tabular.xlsx
+++ b/Documentation/IEA-15-240-RWT_tabular.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gbarter/devel/IEA-15-240-RWT/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3458DE0-F260-3B46-A514-4CF0BC11A23E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD2D05A-B2D2-DC47-9992-0B7B95D17207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20340" yWindow="500" windowWidth="30720" windowHeight="25140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -638,24 +638,6 @@
     <t>Young Modulus E_3 [MPa]</t>
   </si>
   <si>
-    <t>Shear Modulus G_1 [MPa]</t>
-  </si>
-  <si>
-    <t>Shear Modulus G_2 [MPa]</t>
-  </si>
-  <si>
-    <t>Shear Modulus G_3 [MPa]</t>
-  </si>
-  <si>
-    <t>Poisson ratio nu_1</t>
-  </si>
-  <si>
-    <t>Poisson ratio nu_2</t>
-  </si>
-  <si>
-    <t>Poisson ratio nu_3</t>
-  </si>
-  <si>
     <t>Tensile failure Xt_1 [MPa]</t>
   </si>
   <si>
@@ -912,6 +894,24 @@
   </si>
   <si>
     <t>Floating transition piece height [m]</t>
+  </si>
+  <si>
+    <t>Shear Modulus G_12 [MPa]</t>
+  </si>
+  <si>
+    <t>Shear Modulus G_13 [MPa]</t>
+  </si>
+  <si>
+    <t>Shear Modulus G_23 [MPa]</t>
+  </si>
+  <si>
+    <t>Poisson ratio nu_12</t>
+  </si>
+  <si>
+    <t>Poisson ratio nu_13</t>
+  </si>
+  <si>
+    <t>Poisson ratio nu_23</t>
   </si>
 </sst>
 </file>
@@ -1311,7 +1311,7 @@
   <dimension ref="A1:B45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1610,7 +1610,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="B37">
         <v>1483.073634074095</v>
@@ -1618,7 +1618,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="B38">
         <v>10</v>
@@ -1626,7 +1626,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="B39">
         <v>15</v>
@@ -1634,7 +1634,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="B40">
         <v>4014.227616744387</v>
@@ -1642,7 +1642,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="B41">
         <v>2539.9999950000001</v>
@@ -1650,7 +1650,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="B42">
         <v>6722.1391163596727</v>
@@ -1658,7 +1658,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="B43">
         <v>17755.490038649681</v>
@@ -1666,7 +1666,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="B44">
         <v>15</v>
@@ -1674,7 +1674,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="B45">
         <v>20</v>
@@ -20093,7 +20093,7 @@
   <dimension ref="A1:T12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20130,46 +20130,46 @@
         <v>194</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
@@ -20227,7 +20227,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="B3">
         <v>7800</v>
@@ -20278,15 +20278,15 @@
         <v>450</v>
       </c>
       <c r="S3" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="T3" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="B4">
         <v>7850</v>
@@ -20337,15 +20337,15 @@
         <v>814</v>
       </c>
       <c r="S4" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="T4" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B5">
         <v>7200</v>
@@ -20396,10 +20396,10 @@
         <v>310</v>
       </c>
       <c r="S5" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="T5" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
@@ -20458,10 +20458,10 @@
         <v>113.22</v>
       </c>
       <c r="S6" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="T6" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
@@ -20576,10 +20576,10 @@
         <v>113.2</v>
       </c>
       <c r="S8" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="T8" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
@@ -20638,10 +20638,10 @@
         <v>113.2</v>
       </c>
       <c r="S9" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="T9" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
@@ -20697,12 +20697,12 @@
         <v>1.5629999999999999</v>
       </c>
       <c r="S10" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="B11">
         <v>1150</v>
@@ -20753,12 +20753,12 @@
         <v>0</v>
       </c>
       <c r="S11" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="B12">
         <v>1100</v>
@@ -20809,10 +20809,10 @@
         <v>0.4</v>
       </c>
       <c r="S12" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="T12" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -20847,43 +20847,43 @@
   <sheetData>
     <row r="1" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>232</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -22967,62 +22967,62 @@
     <row r="1" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="I1" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="J1" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="K1" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>248</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="B3" s="5">
         <v>48092.001786537301</v>
@@ -23075,7 +23075,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="B4" s="5">
         <v>13479.28387693245</v>
@@ -23128,7 +23128,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="B5" s="5">
         <v>15734.038486973781</v>
@@ -23181,7 +23181,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="B6" s="5">
         <v>0</v>
@@ -23234,7 +23234,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="B7" s="5">
         <v>24335.359356691049</v>
@@ -23287,7 +23287,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="B8" s="5">
         <v>0</v>
@@ -23340,7 +23340,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="B9" s="5">
         <v>130349.2496292837</v>
@@ -23393,7 +23393,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="B10" s="5">
         <v>238490.15752252701</v>
@@ -23446,7 +23446,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="B11" s="5">
         <v>368839.40715181082</v>
@@ -23499,7 +23499,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="B12" s="5">
         <v>9381.2812260099963</v>
@@ -23552,7 +23552,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="B13" s="5">
         <v>10875.722527829839</v>
@@ -23605,7 +23605,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="B14" s="5">
         <v>42274.274414881816</v>
@@ -23658,7 +23658,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="B15" s="5">
         <v>48672</v>
@@ -23711,7 +23711,7 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="B16" s="5">
         <v>20554.306180410989</v>
@@ -23764,7 +23764,7 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="B17" s="5">
         <v>30635</v>
@@ -23817,7 +23817,7 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="B18" s="5">
         <v>11983.85</v>
@@ -23870,7 +23870,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="B19" s="5">
         <v>644856.52500807797</v>
@@ -23923,7 +23923,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="B20" s="5">
         <v>28248.90136716282</v>
@@ -23976,7 +23976,7 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="B21" s="5">
         <v>673105.42637524079</v>
@@ -24029,7 +24029,7 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="B22" s="5">
         <v>204961.55078278569</v>
@@ -24082,7 +24082,7 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="B23" s="5">
         <v>69131.420672551787</v>
@@ -24135,7 +24135,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="B24" s="5">
         <v>947198.39783057827</v>

</xml_diff>

<commit_message>
correct REgion I.5 performance table
</commit_message>
<xml_diff>
--- a/Documentation/IEA-15-240-RWT_tabular.xlsx
+++ b/Documentation/IEA-15-240-RWT_tabular.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gbarter/devel/IEA-15-240-RWT/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A821894E-7868-F848-A44E-356C8FAF24FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BC3C6D2-DDED-E443-B5EF-53257DC87BC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18420" yWindow="500" windowWidth="33940" windowHeight="26840" firstSheet="10" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17260" yWindow="500" windowWidth="33940" windowHeight="26840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -1297,7 +1297,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -20796,12 +20796,13 @@
   <dimension ref="A1:M51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.33203125" bestFit="1" customWidth="1"/>
@@ -20861,16 +20862,16 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>3.92029306636835</v>
       </c>
       <c r="C2">
-        <v>-0.14191928155236991</v>
+        <v>4.2500120550869221E-2</v>
       </c>
       <c r="D2">
-        <v>-0.1884496837038572</v>
+        <v>5.6434433627199833E-2</v>
       </c>
       <c r="E2">
-        <v>-0.19694763951621669</v>
+        <v>5.8979289706730963E-2</v>
       </c>
       <c r="F2">
         <v>4.9999999999999991</v>
@@ -20879,22 +20880,22 @@
         <v>63.339743884126193</v>
       </c>
       <c r="H2">
-        <v>0.38180426769270132</v>
+        <v>0.20290942472624551</v>
       </c>
       <c r="I2">
-        <v>1.5209538696175331</v>
+        <v>0.80830912808874877</v>
       </c>
       <c r="J2">
-        <v>-0.28326841256382579</v>
+        <v>8.4829499913818551E-2</v>
       </c>
       <c r="K2">
-        <v>-9.372604295720198E-3</v>
+        <v>2.8067843078582099E-3</v>
       </c>
       <c r="L2">
-        <v>11.05153318937017</v>
+        <v>5.9801855440195784</v>
       </c>
       <c r="M2">
-        <v>0.36566607094480141</v>
+        <v>0.1978685594054812</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -20902,16 +20903,16 @@
         <v>3.5495323704249011</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>3.9130169732285638</v>
       </c>
       <c r="C3">
-        <v>4.2344690318867659E-2</v>
+        <v>0.29227327318956359</v>
       </c>
       <c r="D3">
-        <v>3.3947149326210319E-2</v>
+        <v>0.23431141836938821</v>
       </c>
       <c r="E3">
-        <v>3.5477963118304791E-2</v>
+        <v>0.24487746465027979</v>
       </c>
       <c r="F3">
         <v>4.9999999999999991</v>
@@ -20920,22 +20921,22 @@
         <v>63.339743884126193</v>
       </c>
       <c r="H3">
-        <v>0.47829949826022611</v>
+        <v>0.27578404836830173</v>
       </c>
       <c r="I3">
-        <v>1.361054187646209</v>
+        <v>0.78477404906973836</v>
       </c>
       <c r="J3">
-        <v>8.4519263879631309E-2</v>
+        <v>0.58337235945413046</v>
       </c>
       <c r="K3">
-        <v>1.9976438663342872E-3</v>
+        <v>1.378822013064589E-2</v>
       </c>
       <c r="L3">
-        <v>13.693204393190809</v>
+        <v>7.8549725145303606</v>
       </c>
       <c r="M3">
-        <v>0.32364391868670239</v>
+        <v>0.18565516242809521</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -20943,16 +20944,16 @@
         <v>4.0679007709585147</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>3.7095354733188231</v>
       </c>
       <c r="C4">
-        <v>0.34837620445170031</v>
+        <v>0.60768342909059347</v>
       </c>
       <c r="D4">
-        <v>0.18554754163204809</v>
+        <v>0.32365633736596139</v>
       </c>
       <c r="E4">
-        <v>0.19391462816087951</v>
+        <v>0.33825130616223842</v>
       </c>
       <c r="F4">
         <v>4.9999999999999991</v>
@@ -20961,22 +20962,22 @@
         <v>63.339743884126193</v>
       </c>
       <c r="H4">
-        <v>0.559152135203276</v>
+        <v>0.36056865333706128</v>
       </c>
       <c r="I4">
-        <v>1.2114543665206809</v>
+        <v>0.78120504602359109</v>
       </c>
       <c r="J4">
-        <v>0.69535283247349577</v>
+        <v>1.2129255335633431</v>
       </c>
       <c r="K4">
-        <v>1.251322257310453E-2</v>
+        <v>2.1827202618978601E-2</v>
       </c>
       <c r="L4">
-        <v>15.76967751906132</v>
+        <v>10.045653229138329</v>
       </c>
       <c r="M4">
-        <v>0.28378324713248149</v>
+        <v>0.18077656245575949</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -20984,16 +20985,16 @@
         <v>4.5539068481037646</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>3.347852062761739</v>
       </c>
       <c r="C5">
-        <v>0.73397264799007067</v>
+        <v>0.98082446702192738</v>
       </c>
       <c r="D5">
-        <v>0.27864112883796083</v>
+        <v>0.37235452496940769</v>
       </c>
       <c r="E5">
-        <v>0.29120618044129498</v>
+        <v>0.38914549132992798</v>
       </c>
       <c r="F5">
         <v>4.9999999999999991</v>
@@ -21002,22 +21003,22 @@
         <v>63.339743884126193</v>
       </c>
       <c r="H5">
-        <v>0.63548108577412965</v>
+        <v>0.45400676159434139</v>
       </c>
       <c r="I5">
-        <v>1.098631676050978</v>
+        <v>0.78489544471847994</v>
       </c>
       <c r="J5">
-        <v>1.4649966134777339</v>
+        <v>1.957708542052736</v>
       </c>
       <c r="K5">
-        <v>2.1036475449975469E-2</v>
+        <v>2.811152415249291E-2</v>
       </c>
       <c r="L5">
-        <v>17.678986985960972</v>
+        <v>12.46569388678485</v>
       </c>
       <c r="M5">
-        <v>0.2538596828751345</v>
+        <v>0.17899991099211121</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -21025,16 +21026,16 @@
         <v>5.006427062922798</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>2.9052717433405961</v>
       </c>
       <c r="C6">
-        <v>1.179136122731224</v>
+        <v>1.4016043406211209</v>
       </c>
       <c r="D6">
-        <v>0.33689769288398502</v>
+        <v>0.40046035363388571</v>
       </c>
       <c r="E6">
-        <v>0.35208976777179962</v>
+        <v>0.41851872509356131</v>
       </c>
       <c r="F6">
         <v>4.9999999999999991</v>
@@ -21043,22 +21044,22 @@
         <v>63.339743884126193</v>
       </c>
       <c r="H6">
-        <v>0.71032941472938216</v>
+        <v>0.55074311155379152</v>
       </c>
       <c r="I6">
-        <v>1.0160656871747089</v>
+        <v>0.78779108184732971</v>
       </c>
       <c r="J6">
-        <v>2.353535150609424</v>
+        <v>2.7975778362702872</v>
       </c>
       <c r="K6">
-        <v>2.7962084550845739E-2</v>
+        <v>3.323770540461482E-2</v>
       </c>
       <c r="L6">
-        <v>19.543206814879049</v>
+        <v>14.974125763967081</v>
       </c>
       <c r="M6">
-        <v>0.2321906266030529</v>
+        <v>0.17790589215488231</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -21066,16 +21067,16 @@
         <v>5.4244152884114127</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>2.4107422824568121</v>
       </c>
       <c r="C7">
-        <v>1.673536946982765</v>
+        <v>1.8580975666127479</v>
       </c>
       <c r="D7">
-        <v>0.37591900619898688</v>
+        <v>0.41737602024331849</v>
       </c>
       <c r="E7">
-        <v>0.39287070938531449</v>
+        <v>0.43619718729149431</v>
       </c>
       <c r="F7">
         <v>4.9999999999999991</v>
@@ -21084,22 +21085,22 @@
         <v>63.339743884126193</v>
       </c>
       <c r="H7">
-        <v>0.7828571821818423</v>
+        <v>0.64809184666449615</v>
       </c>
       <c r="I7">
-        <v>0.95388155433695898</v>
+        <v>0.78967514397261196</v>
       </c>
       <c r="J7">
-        <v>3.3403505792395491</v>
+        <v>3.7087303594393881</v>
       </c>
       <c r="K7">
-        <v>3.3805769772856931E-2</v>
+        <v>3.7533929959338463E-2</v>
       </c>
       <c r="L7">
-        <v>21.34760720335311</v>
+        <v>17.502362857049551</v>
       </c>
       <c r="M7">
-        <v>0.21604687208677081</v>
+        <v>0.1771313624694805</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -21107,16 +21108,16 @@
         <v>5.8069052279141022</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>1.897891096273286</v>
       </c>
       <c r="C8">
-        <v>2.2038877744011391</v>
+        <v>2.3368183198846868</v>
       </c>
       <c r="D8">
-        <v>0.40352740483291683</v>
+        <v>0.42786671950449812</v>
       </c>
       <c r="E8">
-        <v>0.42172408199335742</v>
+        <v>0.44716095446666593</v>
       </c>
       <c r="F8">
         <v>4.9999999999999991</v>
@@ -21125,22 +21126,22 @@
         <v>63.339743884126193</v>
       </c>
       <c r="H8">
-        <v>0.85200481052217514</v>
+        <v>0.74309762695723236</v>
       </c>
       <c r="I8">
-        <v>0.90587931628739315</v>
+        <v>0.79008564497451472</v>
       </c>
       <c r="J8">
-        <v>4.3989215876424979</v>
+        <v>4.664248639671527</v>
       </c>
       <c r="K8">
-        <v>3.8847348957506453E-2</v>
+        <v>4.1190480648463028E-2</v>
       </c>
       <c r="L8">
-        <v>23.07088814769013</v>
+        <v>19.973384855066019</v>
       </c>
       <c r="M8">
-        <v>0.2037414909032827</v>
+        <v>0.17638710667337831</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -21148,16 +21149,16 @@
         <v>6.153012648988982</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>1.387090080369336</v>
       </c>
       <c r="C9">
-        <v>2.746443049629868</v>
+        <v>2.8232506655887502</v>
       </c>
       <c r="D9">
-        <v>0.42269289446468122</v>
+        <v>0.43451401469907569</v>
       </c>
       <c r="E9">
-        <v>0.44175382080194142</v>
+        <v>0.45410800299446752</v>
       </c>
       <c r="F9">
         <v>4.9999999999999991</v>
@@ -21166,22 +21167,22 @@
         <v>63.339743884126193</v>
       </c>
       <c r="H9">
-        <v>0.91600941977978156</v>
+        <v>0.83365363617854105</v>
       </c>
       <c r="I9">
-        <v>0.86744529761247224</v>
+        <v>0.78945577515400112</v>
       </c>
       <c r="J9">
-        <v>5.4818524611718891</v>
+        <v>5.6351591239980809</v>
       </c>
       <c r="K9">
-        <v>4.3117777734042073E-2</v>
+        <v>4.4323618763093472E-2</v>
       </c>
       <c r="L9">
-        <v>24.670504032280711</v>
+        <v>22.332833687577921</v>
       </c>
       <c r="M9">
-        <v>0.19404705197470171</v>
+        <v>0.17565999193390511</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
@@ -21189,16 +21190,16 @@
         <v>6.461937427558305</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>0.89171302362800164</v>
       </c>
       <c r="C10">
-        <v>3.2703733449329189</v>
+        <v>3.3022571375122158</v>
       </c>
       <c r="D10">
-        <v>0.43453710088049191</v>
+        <v>0.43877352569539829</v>
       </c>
       <c r="E10">
-        <v>0.45413213022485599</v>
+        <v>0.45855959251019962</v>
       </c>
       <c r="F10">
         <v>4.9999999999999991</v>
@@ -21207,22 +21208,22 @@
         <v>63.339743884126193</v>
       </c>
       <c r="H10">
-        <v>0.97300207500248759</v>
+        <v>0.91817523067797768</v>
       </c>
       <c r="I10">
-        <v>0.8354222598389881</v>
+        <v>0.78834778038805231</v>
       </c>
       <c r="J10">
-        <v>6.5276081993717474</v>
+        <v>6.5912476936790716</v>
       </c>
       <c r="K10">
-        <v>4.6551451289635587E-2</v>
+        <v>4.7005294524226422E-2</v>
       </c>
       <c r="L10">
-        <v>26.095859726010019</v>
+        <v>24.5401606480178</v>
       </c>
       <c r="M10">
-        <v>0.1861018777158589</v>
+        <v>0.17500745420902891</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
@@ -21230,16 +21231,16 @@
         <v>6.7329653976189894</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>0.4252073936548052</v>
       </c>
       <c r="C11">
-        <v>3.751815727502601</v>
+        <v>3.7587087232875418</v>
       </c>
       <c r="D11">
-        <v>0.44069703147689832</v>
+        <v>0.44150669884892257</v>
       </c>
       <c r="E11">
-        <v>0.46056983692036019</v>
+        <v>0.46141601545767241</v>
       </c>
       <c r="F11">
         <v>4.9999999999999991</v>
@@ -21248,22 +21249,22 @@
         <v>63.339743884126193</v>
       </c>
       <c r="H11">
-        <v>1.022075967313403</v>
+        <v>0.9951616025285136</v>
       </c>
       <c r="I11">
-        <v>0.80832904574420816</v>
+        <v>0.78704328666255474</v>
       </c>
       <c r="J11">
-        <v>7.4885588042487514</v>
+        <v>7.5023171037021568</v>
       </c>
       <c r="K11">
-        <v>4.9191506361455632E-2</v>
+        <v>4.9281883093851848E-2</v>
       </c>
       <c r="L11">
-        <v>27.320730150936111</v>
+        <v>26.55670159395137</v>
       </c>
       <c r="M11">
-        <v>0.17946682481238929</v>
+        <v>0.17444800655861201</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
@@ -21271,16 +21272,16 @@
         <v>6.965470002237022</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>4.6916183299056108E-4</v>
       </c>
       <c r="C12">
-        <v>4.1781435560526523</v>
+        <v>4.1781435686967399</v>
       </c>
       <c r="D12">
-        <v>0.44325113075989619</v>
+        <v>0.44325113210128292</v>
       </c>
       <c r="E12">
-        <v>0.4632391108347011</v>
+        <v>0.46323911223657632</v>
       </c>
       <c r="F12">
         <v>4.9999999999999991</v>
@@ -21289,22 +21290,22 @@
         <v>63.339743884126193</v>
       </c>
       <c r="H12">
-        <v>1.0633110712471501</v>
+        <v>1.0632807464234291</v>
       </c>
       <c r="I12">
-        <v>0.78573709425224547</v>
+        <v>0.78571468562741442</v>
       </c>
       <c r="J12">
-        <v>8.3395017198566759</v>
+        <v>8.3395017450940543</v>
       </c>
       <c r="K12">
-        <v>5.1185139664553923E-2</v>
+        <v>5.1185139819452712E-2</v>
       </c>
       <c r="L12">
-        <v>28.347767130297729</v>
+        <v>28.34690586761047</v>
       </c>
       <c r="M12">
-        <v>0.17398934234735991</v>
+        <v>0.1739840561980891</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -21927,16 +21928,16 @@
         <v>9.7800375142981277</v>
       </c>
       <c r="B28">
-        <v>0.9520380501267659</v>
+        <v>-0.13530100801320749</v>
       </c>
       <c r="C28">
-        <v>11.509097778118919</v>
+        <v>11.61840604573959</v>
       </c>
       <c r="D28">
-        <v>0.44110043984193242</v>
+        <v>0.44528981470479162</v>
       </c>
       <c r="E28">
-        <v>0.45933814267743289</v>
+        <v>0.46370073109193299</v>
       </c>
       <c r="F28">
         <v>6.9482707247528213</v>
@@ -21945,22 +21946,22 @@
         <v>88.020337628683137</v>
       </c>
       <c r="H28">
-        <v>1.9546910360395531</v>
+        <v>2.0948411147616262</v>
       </c>
       <c r="I28">
-        <v>0.73268087115230496</v>
+        <v>0.78521361411622925</v>
       </c>
       <c r="J28">
-        <v>16.471416517110178</v>
+        <v>16.627854670600112</v>
       </c>
       <c r="K28">
-        <v>5.1280771531633712E-2</v>
+        <v>5.1767813383778859E-2</v>
       </c>
       <c r="L28">
-        <v>51.870027503480209</v>
+        <v>55.834993819987382</v>
       </c>
       <c r="M28">
-        <v>0.16148793438514761</v>
+        <v>0.1738321387585976</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
@@ -21968,16 +21969,16 @@
         <v>10.20964775919068</v>
       </c>
       <c r="B29">
-        <v>2.103996053204447</v>
+        <v>-0.1352156790530952</v>
       </c>
       <c r="C29">
-        <v>12.66620928599834</v>
+        <v>13.195742132985281</v>
       </c>
       <c r="D29">
-        <v>0.42670934710235531</v>
+        <v>0.44454867142623389</v>
       </c>
       <c r="E29">
-        <v>0.44509285247604391</v>
+        <v>0.46370073112571347</v>
       </c>
       <c r="F29">
         <v>7.2534892153032686</v>
@@ -21986,22 +21987,22 @@
         <v>91.886829832716131</v>
       </c>
       <c r="H29">
-        <v>1.9578668202870011</v>
+        <v>2.2829129613145218</v>
       </c>
       <c r="I29">
-        <v>0.6734097528743217</v>
+        <v>0.7852096154768291</v>
       </c>
       <c r="J29">
-        <v>17.393602308449459</v>
+        <v>18.120772019748429</v>
       </c>
       <c r="K29">
-        <v>4.9690419230470143E-2</v>
+        <v>5.1767813387550127E-2</v>
       </c>
       <c r="L29">
-        <v>51.67639752270663</v>
+        <v>60.847759270752057</v>
       </c>
       <c r="M29">
-        <v>0.1476302500015379</v>
+        <v>0.17383119458409241</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
@@ -22009,16 +22010,16 @@
         <v>10.673450038768539</v>
       </c>
       <c r="B30">
-        <v>3.0696396365291818</v>
+        <v>3.0696370593862179</v>
       </c>
       <c r="C30">
-        <v>13.79893929822155</v>
+        <v>13.798941169832769</v>
       </c>
       <c r="D30">
-        <v>0.40686376408147829</v>
+        <v>0.40686381926621162</v>
       </c>
       <c r="E30">
-        <v>0.42489539400661902</v>
+        <v>0.42489545163706199</v>
       </c>
       <c r="F30">
         <v>7.4992409326593661</v>
@@ -22027,22 +22028,22 @@
         <v>95</v>
       </c>
       <c r="H30">
-        <v>1.957870854438956</v>
+        <v>1.957871297237179</v>
       </c>
       <c r="I30">
-        <v>0.61615811317972768</v>
+        <v>0.61615825253198231</v>
       </c>
       <c r="J30">
-        <v>18.349861478044691</v>
+        <v>18.349863966917621</v>
       </c>
       <c r="K30">
-        <v>4.7965368964219823E-2</v>
+        <v>4.7965375469975133E-2</v>
       </c>
       <c r="L30">
-        <v>51.348728956521192</v>
+        <v>51.348741380706812</v>
       </c>
       <c r="M30">
-        <v>0.1342223064294055</v>
+        <v>0.1342223389054352</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
@@ -22915,7 +22916,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
ensure that no peak thrust shaving is applied
</commit_message>
<xml_diff>
--- a/Documentation/IEA-15-240-RWT_tabular.xlsx
+++ b/Documentation/IEA-15-240-RWT_tabular.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gbarter/devel/IEA-15-240-RWT/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BC3C6D2-DDED-E443-B5EF-53257DC87BC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D41ECA8-11BF-D44F-8DD0-092068BF77D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17260" yWindow="500" windowWidth="33940" windowHeight="26840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20796,13 +20796,12 @@
   <dimension ref="A1:M51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.33203125" bestFit="1" customWidth="1"/>
@@ -20862,16 +20861,16 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>3.92029306636835</v>
+        <v>3.9202930663685378</v>
       </c>
       <c r="C2">
-        <v>4.2500120550869221E-2</v>
+        <v>4.2500120560404683E-2</v>
       </c>
       <c r="D2">
-        <v>5.6434433627199833E-2</v>
+        <v>5.6434433639861642E-2</v>
       </c>
       <c r="E2">
-        <v>5.8979289706730963E-2</v>
+        <v>5.8979289706730907E-2</v>
       </c>
       <c r="F2">
         <v>4.9999999999999991</v>
@@ -20880,22 +20879,22 @@
         <v>63.339743884126193</v>
       </c>
       <c r="H2">
-        <v>0.20290942472624551</v>
+        <v>0.20290942472623591</v>
       </c>
       <c r="I2">
-        <v>0.80830912808874877</v>
+        <v>0.80830912808871058</v>
       </c>
       <c r="J2">
-        <v>8.4829499913818551E-2</v>
+        <v>8.4829499913818482E-2</v>
       </c>
       <c r="K2">
-        <v>2.8067843078582099E-3</v>
+        <v>2.8067843078582082E-3</v>
       </c>
       <c r="L2">
-        <v>5.9801855440195784</v>
+        <v>5.9801855440193146</v>
       </c>
       <c r="M2">
-        <v>0.1978685594054812</v>
+        <v>0.19786855940547241</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -20903,16 +20902,16 @@
         <v>3.5495323704249011</v>
       </c>
       <c r="B3">
-        <v>3.9130169732285638</v>
+        <v>3.9130169732287619</v>
       </c>
       <c r="C3">
-        <v>0.29227327318956359</v>
+        <v>0.29227327325513919</v>
       </c>
       <c r="D3">
-        <v>0.23431141836938821</v>
+        <v>0.23431141842195921</v>
       </c>
       <c r="E3">
-        <v>0.24487746465027979</v>
+        <v>0.24487746465027971</v>
       </c>
       <c r="F3">
         <v>4.9999999999999991</v>
@@ -20921,22 +20920,22 @@
         <v>63.339743884126193</v>
       </c>
       <c r="H3">
-        <v>0.27578404836830173</v>
+        <v>0.27578404836829129</v>
       </c>
       <c r="I3">
-        <v>0.78477404906973836</v>
+        <v>0.78477404906970871</v>
       </c>
       <c r="J3">
-        <v>0.58337235945413046</v>
+        <v>0.58337235945413035</v>
       </c>
       <c r="K3">
         <v>1.378822013064589E-2</v>
       </c>
       <c r="L3">
-        <v>7.8549725145303606</v>
+        <v>7.8549725145300764</v>
       </c>
       <c r="M3">
-        <v>0.18565516242809521</v>
+        <v>0.18565516242808841</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -20944,13 +20943,13 @@
         <v>4.0679007709585147</v>
       </c>
       <c r="B4">
-        <v>3.7095354733188231</v>
+        <v>3.7095354733204511</v>
       </c>
       <c r="C4">
-        <v>0.60768342909059347</v>
+        <v>0.60768342922693575</v>
       </c>
       <c r="D4">
-        <v>0.32365633736596139</v>
+        <v>0.32365633743857819</v>
       </c>
       <c r="E4">
         <v>0.33825130616223842</v>
@@ -20962,10 +20961,10 @@
         <v>63.339743884126193</v>
       </c>
       <c r="H4">
-        <v>0.36056865333706128</v>
+        <v>0.36056865333697202</v>
       </c>
       <c r="I4">
-        <v>0.78120504602359109</v>
+        <v>0.7812050460233978</v>
       </c>
       <c r="J4">
         <v>1.2129255335633431</v>
@@ -20974,10 +20973,10 @@
         <v>2.1827202618978601E-2</v>
       </c>
       <c r="L4">
-        <v>10.045653229138329</v>
+        <v>10.04565322913589</v>
       </c>
       <c r="M4">
-        <v>0.18077656245575949</v>
+        <v>0.18077656245571541</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -20985,16 +20984,16 @@
         <v>4.5539068481037646</v>
       </c>
       <c r="B5">
-        <v>3.347852062761739</v>
+        <v>3.347852062762545</v>
       </c>
       <c r="C5">
-        <v>0.98082446702192738</v>
+        <v>0.98082446724198902</v>
       </c>
       <c r="D5">
-        <v>0.37235452496940769</v>
+        <v>0.37235452505295058</v>
       </c>
       <c r="E5">
-        <v>0.38914549132992798</v>
+        <v>0.38914549132992787</v>
       </c>
       <c r="F5">
         <v>4.9999999999999991</v>
@@ -21003,10 +21002,10 @@
         <v>63.339743884126193</v>
       </c>
       <c r="H5">
-        <v>0.45400676159434139</v>
+        <v>0.45400676159429543</v>
       </c>
       <c r="I5">
-        <v>0.78489544471847994</v>
+        <v>0.78489544471840045</v>
       </c>
       <c r="J5">
         <v>1.957708542052736</v>
@@ -21015,10 +21014,10 @@
         <v>2.811152415249291E-2</v>
       </c>
       <c r="L5">
-        <v>12.46569388678485</v>
+        <v>12.46569388678358</v>
       </c>
       <c r="M5">
-        <v>0.17899991099211121</v>
+        <v>0.17899991099209289</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -21026,16 +21025,16 @@
         <v>5.006427062922798</v>
       </c>
       <c r="B6">
-        <v>2.9052717433405961</v>
+        <v>2.905271743334926</v>
       </c>
       <c r="C6">
-        <v>1.4016043406211209</v>
+        <v>1.4016043409355901</v>
       </c>
       <c r="D6">
-        <v>0.40046035363388571</v>
+        <v>0.40046035372373451</v>
       </c>
       <c r="E6">
-        <v>0.41851872509356131</v>
+        <v>0.41851872509356108</v>
       </c>
       <c r="F6">
         <v>4.9999999999999991</v>
@@ -21044,22 +21043,22 @@
         <v>63.339743884126193</v>
       </c>
       <c r="H6">
-        <v>0.55074311155379152</v>
+        <v>0.55074311155412614</v>
       </c>
       <c r="I6">
-        <v>0.78779108184732971</v>
+        <v>0.78779108184780833</v>
       </c>
       <c r="J6">
-        <v>2.7975778362702872</v>
+        <v>2.7975778362702859</v>
       </c>
       <c r="K6">
-        <v>3.323770540461482E-2</v>
+        <v>3.3237705404614813E-2</v>
       </c>
       <c r="L6">
-        <v>14.974125763967081</v>
+        <v>14.974125763976399</v>
       </c>
       <c r="M6">
-        <v>0.17790589215488231</v>
+        <v>0.177905892154993</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -21067,16 +21066,16 @@
         <v>5.4244152884114127</v>
       </c>
       <c r="B7">
-        <v>2.4107422824568121</v>
+        <v>2.4107422824568658</v>
       </c>
       <c r="C7">
-        <v>1.8580975666127479</v>
+        <v>1.8580975670296369</v>
       </c>
       <c r="D7">
-        <v>0.41737602024331849</v>
+        <v>0.41737602033696253</v>
       </c>
       <c r="E7">
-        <v>0.43619718729149431</v>
+        <v>0.43619718729149409</v>
       </c>
       <c r="F7">
         <v>4.9999999999999991</v>
@@ -21085,22 +21084,22 @@
         <v>63.339743884126193</v>
       </c>
       <c r="H7">
-        <v>0.64809184666449615</v>
+        <v>0.64809184666449282</v>
       </c>
       <c r="I7">
-        <v>0.78967514397261196</v>
+        <v>0.78967514397260785</v>
       </c>
       <c r="J7">
-        <v>3.7087303594393881</v>
+        <v>3.7087303594393868</v>
       </c>
       <c r="K7">
-        <v>3.7533929959338463E-2</v>
+        <v>3.7533929959338443E-2</v>
       </c>
       <c r="L7">
-        <v>17.502362857049551</v>
+        <v>17.502362857049459</v>
       </c>
       <c r="M7">
-        <v>0.1771313624694805</v>
+        <v>0.1771313624694795</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -21108,16 +21107,16 @@
         <v>5.8069052279141022</v>
       </c>
       <c r="B8">
-        <v>1.897891096273286</v>
+        <v>1.8978910962722211</v>
       </c>
       <c r="C8">
-        <v>2.3368183198846868</v>
+        <v>2.3368183204089861</v>
       </c>
       <c r="D8">
-        <v>0.42786671950449812</v>
+        <v>0.4278667196004961</v>
       </c>
       <c r="E8">
-        <v>0.44716095446666593</v>
+        <v>0.44716095446666609</v>
       </c>
       <c r="F8">
         <v>4.9999999999999991</v>
@@ -21126,22 +21125,22 @@
         <v>63.339743884126193</v>
       </c>
       <c r="H8">
-        <v>0.74309762695723236</v>
+        <v>0.74309762695729842</v>
       </c>
       <c r="I8">
-        <v>0.79008564497451472</v>
+        <v>0.790085644974585</v>
       </c>
       <c r="J8">
-        <v>4.664248639671527</v>
+        <v>4.6642486396715288</v>
       </c>
       <c r="K8">
-        <v>4.1190480648463028E-2</v>
+        <v>4.1190480648463042E-2</v>
       </c>
       <c r="L8">
-        <v>19.973384855066019</v>
+        <v>19.97338485506787</v>
       </c>
       <c r="M8">
-        <v>0.17638710667337831</v>
+        <v>0.17638710667339469</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -21149,13 +21148,13 @@
         <v>6.153012648988982</v>
       </c>
       <c r="B9">
-        <v>1.387090080369336</v>
+        <v>1.387090080368143</v>
       </c>
       <c r="C9">
-        <v>2.8232506655887502</v>
+        <v>2.8232506662221861</v>
       </c>
       <c r="D9">
-        <v>0.43451401469907569</v>
+        <v>0.43451401479656498</v>
       </c>
       <c r="E9">
         <v>0.45410800299446752</v>
@@ -21167,10 +21166,10 @@
         <v>63.339743884126193</v>
       </c>
       <c r="H9">
-        <v>0.83365363617854105</v>
+        <v>0.83365363617861621</v>
       </c>
       <c r="I9">
-        <v>0.78945577515400112</v>
+        <v>0.78945577515407228</v>
       </c>
       <c r="J9">
         <v>5.6351591239980809</v>
@@ -21179,10 +21178,10 @@
         <v>4.4323618763093472E-2</v>
       </c>
       <c r="L9">
-        <v>22.332833687577921</v>
+        <v>22.332833687580042</v>
       </c>
       <c r="M9">
-        <v>0.17565999193390511</v>
+        <v>0.17565999193392171</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
@@ -21190,13 +21189,13 @@
         <v>6.461937427558305</v>
       </c>
       <c r="B10">
-        <v>0.89171302362800164</v>
+        <v>0.8917130236284514</v>
       </c>
       <c r="C10">
-        <v>3.3022571375122158</v>
+        <v>3.3022571382531241</v>
       </c>
       <c r="D10">
-        <v>0.43877352569539829</v>
+        <v>0.43877352579384332</v>
       </c>
       <c r="E10">
         <v>0.45855959251019962</v>
@@ -21208,10 +21207,10 @@
         <v>63.339743884126193</v>
       </c>
       <c r="H10">
-        <v>0.91817523067797768</v>
+        <v>0.91817523067794926</v>
       </c>
       <c r="I10">
-        <v>0.78834778038805231</v>
+        <v>0.78834778038802789</v>
       </c>
       <c r="J10">
         <v>6.5912476936790716</v>
@@ -21220,10 +21219,10 @@
         <v>4.7005294524226422E-2</v>
       </c>
       <c r="L10">
-        <v>24.5401606480178</v>
+        <v>24.54016064801699</v>
       </c>
       <c r="M10">
-        <v>0.17500745420902891</v>
+        <v>0.17500745420902311</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
@@ -21231,13 +21230,13 @@
         <v>6.7329653976189894</v>
       </c>
       <c r="B11">
-        <v>0.4252073936548052</v>
+        <v>0.42520739365487531</v>
       </c>
       <c r="C11">
-        <v>3.7587087232875418</v>
+        <v>3.758708724130861</v>
       </c>
       <c r="D11">
-        <v>0.44150669884892257</v>
+        <v>0.44150669894798078</v>
       </c>
       <c r="E11">
         <v>0.46141601545767241</v>
@@ -21249,10 +21248,10 @@
         <v>63.339743884126193</v>
       </c>
       <c r="H11">
-        <v>0.9951616025285136</v>
+        <v>0.99516160252850927</v>
       </c>
       <c r="I11">
-        <v>0.78704328666255474</v>
+        <v>0.7870432866625513</v>
       </c>
       <c r="J11">
         <v>7.5023171037021568</v>
@@ -21261,10 +21260,10 @@
         <v>4.9281883093851848E-2</v>
       </c>
       <c r="L11">
-        <v>26.55670159395137</v>
+        <v>26.556701593951239</v>
       </c>
       <c r="M11">
-        <v>0.17444800655861201</v>
+        <v>0.17444800655861109</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
@@ -21272,13 +21271,13 @@
         <v>6.965470002237022</v>
       </c>
       <c r="B12">
-        <v>4.6916183299056108E-4</v>
+        <v>4.6916182858695171E-4</v>
       </c>
       <c r="C12">
-        <v>4.1781435686967399</v>
+        <v>4.1781435696341642</v>
       </c>
       <c r="D12">
-        <v>0.44325113210128292</v>
+        <v>0.44325113220073242</v>
       </c>
       <c r="E12">
         <v>0.46323911223657632</v>
@@ -21290,10 +21289,10 @@
         <v>63.339743884126193</v>
       </c>
       <c r="H12">
-        <v>1.0632807464234291</v>
+        <v>1.0632807464237131</v>
       </c>
       <c r="I12">
-        <v>0.78571468562741442</v>
+        <v>0.78571468562762481</v>
       </c>
       <c r="J12">
         <v>8.3395017450940543</v>
@@ -21302,10 +21301,10 @@
         <v>5.1185139819452712E-2</v>
       </c>
       <c r="L12">
-        <v>28.34690586761047</v>
+        <v>28.346905867618549</v>
       </c>
       <c r="M12">
-        <v>0.1739840561980891</v>
+        <v>0.1739840561981387</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -21316,10 +21315,10 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <v>4.5469595802022624</v>
+        <v>4.5469595811615813</v>
       </c>
       <c r="D13">
-        <v>0.44432165271148588</v>
+        <v>0.44432165280522912</v>
       </c>
       <c r="E13">
         <v>0.46363055021664751</v>
@@ -21357,10 +21356,10 @@
         <v>0</v>
       </c>
       <c r="C14">
-        <v>4.855095715233567</v>
+        <v>4.8550957161853212</v>
       </c>
       <c r="D14">
-        <v>0.44509803502533618</v>
+        <v>0.44509803511258972</v>
       </c>
       <c r="E14">
         <v>0.46363055021664762</v>
@@ -21398,10 +21397,10 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <v>5.0912784127956803</v>
+        <v>5.0912784137470233</v>
       </c>
       <c r="D15">
-        <v>0.44557229376258972</v>
+        <v>0.44557229384584829</v>
       </c>
       <c r="E15">
         <v>0.4636305502166474</v>
@@ -21439,10 +21438,10 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <v>5.248186601663674</v>
+        <v>5.2481866026156334</v>
       </c>
       <c r="D16">
-        <v>0.44585428682050238</v>
+        <v>0.44585428690137507</v>
       </c>
       <c r="E16">
         <v>0.4636305502166474</v>
@@ -21480,10 +21479,10 @@
         <v>0</v>
       </c>
       <c r="C17">
-        <v>5.3205230547082252</v>
+        <v>5.3205230556611873</v>
       </c>
       <c r="D17">
-        <v>0.4459713127475381</v>
+        <v>0.44597131282741631</v>
       </c>
       <c r="E17">
         <v>0.46363055021664762</v>
@@ -21521,10 +21520,10 @@
         <v>0</v>
       </c>
       <c r="C18">
-        <v>5.3350746198482719</v>
+        <v>5.3350746208014117</v>
       </c>
       <c r="D18">
-        <v>0.44599470403549718</v>
+        <v>0.44599470411517661</v>
       </c>
       <c r="E18">
         <v>0.46363055021664751</v>
@@ -21562,10 +21561,10 @@
         <v>0</v>
       </c>
       <c r="C19">
-        <v>5.4376296268088469</v>
+        <v>5.4376296277630694</v>
       </c>
       <c r="D19">
-        <v>0.44615750972272988</v>
+        <v>0.44615750980102381</v>
       </c>
       <c r="E19">
         <v>0.4636305502166474</v>
@@ -21603,10 +21602,10 @@
         <v>0</v>
       </c>
       <c r="C20">
-        <v>5.6309673740720614</v>
+        <v>5.6309673750304778</v>
       </c>
       <c r="D20">
-        <v>0.44642729328031061</v>
+        <v>0.44642729335629461</v>
       </c>
       <c r="E20">
         <v>0.4636305502166474</v>
@@ -21644,10 +21643,10 @@
         <v>0</v>
       </c>
       <c r="C21">
-        <v>5.9206804975500544</v>
+        <v>5.9206804985167514</v>
       </c>
       <c r="D21">
-        <v>0.44677906809992018</v>
+        <v>0.44677906817286789</v>
       </c>
       <c r="E21">
         <v>0.46363055021664751</v>
@@ -21685,10 +21684,10 @@
         <v>0</v>
       </c>
       <c r="C22">
-        <v>6.3147957481196606</v>
+        <v>6.3147957491022897</v>
       </c>
       <c r="D22">
-        <v>0.44716337952706492</v>
+        <v>0.4471633795966467</v>
       </c>
       <c r="E22">
         <v>0.46363055021664767</v>
@@ -21726,10 +21725,10 @@
         <v>0</v>
       </c>
       <c r="C23">
-        <v>6.8241246915178877</v>
+        <v>6.8241246925283496</v>
       </c>
       <c r="D23">
-        <v>0.44753244180855539</v>
+        <v>0.44753244187482261</v>
       </c>
       <c r="E23">
         <v>0.46363055021664762</v>
@@ -21767,10 +21766,10 @@
         <v>0</v>
       </c>
       <c r="C24">
-        <v>7.4624689822597787</v>
+        <v>7.4624689833144862</v>
       </c>
       <c r="D24">
-        <v>0.44784916271052527</v>
+        <v>0.44784916277382192</v>
       </c>
       <c r="E24">
         <v>0.46363055021664751</v>
@@ -21808,10 +21807,10 @@
         <v>0</v>
       </c>
       <c r="C25">
-        <v>8.2379430843291424</v>
+        <v>8.2379430855212128</v>
       </c>
       <c r="D25">
-        <v>0.44760843077999801</v>
+        <v>0.44760843084476909</v>
       </c>
       <c r="E25">
         <v>0.4636305502166474</v>
@@ -21849,10 +21848,10 @@
         <v>0</v>
       </c>
       <c r="C26">
-        <v>9.1675030553241346</v>
+        <v>9.1675030567788287</v>
       </c>
       <c r="D26">
-        <v>0.44678383876763061</v>
+        <v>0.44678383883852613</v>
       </c>
       <c r="E26">
         <v>0.46363055021664762</v>
@@ -21890,10 +21889,10 @@
         <v>0</v>
       </c>
       <c r="C27">
-        <v>10.28468981121207</v>
+        <v>10.28468981298067</v>
       </c>
       <c r="D27">
-        <v>0.44598588727911959</v>
+        <v>0.44598588735581363</v>
       </c>
       <c r="E27">
         <v>0.4636305502166474</v>
@@ -21928,16 +21927,16 @@
         <v>9.7800375142981277</v>
       </c>
       <c r="B28">
-        <v>-0.13530100801320749</v>
+        <v>0</v>
       </c>
       <c r="C28">
-        <v>11.61840604573959</v>
+        <v>11.61664760789853</v>
       </c>
       <c r="D28">
-        <v>0.44528981470479162</v>
+        <v>0.44522242039464832</v>
       </c>
       <c r="E28">
-        <v>0.46370073109193299</v>
+        <v>0.46363055021664762</v>
       </c>
       <c r="F28">
         <v>6.9482707247528213</v>
@@ -21946,22 +21945,22 @@
         <v>88.020337628683137</v>
       </c>
       <c r="H28">
-        <v>2.0948411147616262</v>
+        <v>2.0778572792330792</v>
       </c>
       <c r="I28">
-        <v>0.78521361411622925</v>
+        <v>0.77884752802838619</v>
       </c>
       <c r="J28">
-        <v>16.627854670600112</v>
+        <v>16.625338053056389</v>
       </c>
       <c r="K28">
-        <v>5.1767813383778859E-2</v>
+        <v>5.1759978350941351E-2</v>
       </c>
       <c r="L28">
-        <v>55.834993819987382</v>
+        <v>55.352481403095773</v>
       </c>
       <c r="M28">
-        <v>0.1738321387585976</v>
+        <v>0.17232992375565029</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
@@ -21969,16 +21968,16 @@
         <v>10.20964775919068</v>
       </c>
       <c r="B29">
-        <v>-0.1352156790530952</v>
+        <v>0</v>
       </c>
       <c r="C29">
-        <v>13.195742132985281</v>
+        <v>13.193744965595791</v>
       </c>
       <c r="D29">
-        <v>0.44454867142623389</v>
+        <v>0.44448138926046682</v>
       </c>
       <c r="E29">
-        <v>0.46370073112571347</v>
+        <v>0.46363055021664751</v>
       </c>
       <c r="F29">
         <v>7.2534892153032686</v>
@@ -21987,39 +21986,39 @@
         <v>91.886829832716131</v>
       </c>
       <c r="H29">
-        <v>2.2829129613145218</v>
+        <v>2.2644158726253489</v>
       </c>
       <c r="I29">
-        <v>0.7852096154768291</v>
+        <v>0.77884752802838642</v>
       </c>
       <c r="J29">
-        <v>18.120772019748429</v>
+        <v>18.118029448585698</v>
       </c>
       <c r="K29">
-        <v>5.1767813387550127E-2</v>
+        <v>5.175997835094133E-2</v>
       </c>
       <c r="L29">
-        <v>60.847759270752057</v>
+        <v>60.32225539794144</v>
       </c>
       <c r="M29">
-        <v>0.17383119458409241</v>
+        <v>0.1723299237556504</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>10.673450038768539</v>
+        <v>10.65843263308146</v>
       </c>
       <c r="B30">
-        <v>3.0696370593862179</v>
+        <v>0</v>
       </c>
       <c r="C30">
-        <v>13.798941169832769</v>
+        <v>15</v>
       </c>
       <c r="D30">
-        <v>0.40686381926621162</v>
+        <v>0.44414932053348638</v>
       </c>
       <c r="E30">
-        <v>0.42489545163706199</v>
+        <v>0.46383339379791422</v>
       </c>
       <c r="F30">
         <v>7.4992409326593661</v>
@@ -22028,39 +22027,39 @@
         <v>95</v>
       </c>
       <c r="H30">
-        <v>1.957871297237179</v>
+        <v>2.44733984880892</v>
       </c>
       <c r="I30">
-        <v>0.61615825253198231</v>
+        <v>0.77236994452391527</v>
       </c>
       <c r="J30">
-        <v>18.349863966917621</v>
+        <v>19.94703494729313</v>
       </c>
       <c r="K30">
-        <v>4.7965375469975133E-2</v>
+        <v>5.2287310293663583E-2</v>
       </c>
       <c r="L30">
-        <v>51.348741380706812</v>
+        <v>65.148695985257845</v>
       </c>
       <c r="M30">
-        <v>0.1342223389054352</v>
+        <v>0.17077475881552001</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>11.168230921342939</v>
+        <v>10.673450038768539</v>
       </c>
       <c r="B31">
-        <v>3.715557720461502</v>
+        <v>0.5119743916727435</v>
       </c>
       <c r="C31">
-        <v>15</v>
+        <v>15.00000264755824</v>
       </c>
       <c r="D31">
-        <v>0.38606095156337478</v>
+        <v>0.44227729440075542</v>
       </c>
       <c r="E31">
-        <v>0.40317063008894721</v>
+        <v>0.46187840209967168</v>
       </c>
       <c r="F31">
         <v>7.4992409326593661</v>
@@ -22069,22 +22068,22 @@
         <v>95</v>
       </c>
       <c r="H31">
-        <v>1.957871879191831</v>
+        <v>2.3743110520855568</v>
       </c>
       <c r="I31">
-        <v>0.56277302370654214</v>
+        <v>0.74721527961762924</v>
       </c>
       <c r="J31">
-        <v>19.94703478448703</v>
+        <v>19.94703830114377</v>
       </c>
       <c r="K31">
-        <v>4.7622722248790383E-2</v>
+        <v>5.2140287435005539E-2</v>
       </c>
       <c r="L31">
-        <v>50.93441324085552</v>
+        <v>63.067410540110799</v>
       </c>
       <c r="M31">
-        <v>0.1216038093321424</v>
+        <v>0.1648541935749088</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
@@ -22092,16 +22091,16 @@
         <v>11.17037214438025</v>
       </c>
       <c r="B32">
-        <v>3.7237057847124899</v>
+        <v>3.7237332633991098</v>
       </c>
       <c r="C32">
-        <v>14.99999776662168</v>
+        <v>14.99997214828125</v>
       </c>
       <c r="D32">
-        <v>0.3858389272516467</v>
+        <v>0.38583826828134937</v>
       </c>
       <c r="E32">
-        <v>0.40293876597191591</v>
+        <v>0.40293807771468942</v>
       </c>
       <c r="F32">
         <v>7.4992409326593661</v>
@@ -22110,22 +22109,22 @@
         <v>95</v>
       </c>
       <c r="H32">
-        <v>1.956906638335602</v>
+        <v>1.9569017482867681</v>
       </c>
       <c r="I32">
-        <v>0.56227994741926968</v>
+        <v>0.56227854235663277</v>
       </c>
       <c r="J32">
-        <v>19.9470318145368</v>
+        <v>19.94699774313451</v>
       </c>
       <c r="K32">
-        <v>4.7604459529750051E-2</v>
+        <v>4.7604378216865667E-2</v>
       </c>
       <c r="L32">
-        <v>50.905569529375093</v>
+        <v>50.90543244011603</v>
       </c>
       <c r="M32">
-        <v>0.1214883571165692</v>
+        <v>0.1214880299470863</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
@@ -22133,16 +22132,16 @@
         <v>11.699265301635981</v>
       </c>
       <c r="B33">
-        <v>5.3964863650756216</v>
+        <v>5.3964863681084276</v>
       </c>
       <c r="C33">
-        <v>15.00000887891548</v>
+        <v>15.00000887812565</v>
       </c>
       <c r="D33">
-        <v>0.33584085026080451</v>
+        <v>0.33584085024312083</v>
       </c>
       <c r="E33">
-        <v>0.35072484451209562</v>
+        <v>0.35072484442199942</v>
       </c>
       <c r="F33">
         <v>7.4992409326593661</v>
@@ -22151,22 +22150,22 @@
         <v>95</v>
       </c>
       <c r="H33">
-        <v>1.769139016927969</v>
+        <v>1.76913901636086</v>
       </c>
       <c r="I33">
-        <v>0.46340696264216452</v>
+        <v>0.46340696249361651</v>
       </c>
       <c r="J33">
-        <v>19.947046591690871</v>
+        <v>19.94704658656676</v>
       </c>
       <c r="K33">
-        <v>4.3397635278644028E-2</v>
+        <v>4.33976352674958E-2</v>
       </c>
       <c r="L33">
-        <v>45.214243287748111</v>
+        <v>45.214243271898248</v>
       </c>
       <c r="M33">
-        <v>9.8370013354204575E-2</v>
+        <v>9.837001331972095E-2</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
@@ -22174,16 +22173,16 @@
         <v>12.2589068261207</v>
       </c>
       <c r="B34">
-        <v>6.7666944445678929</v>
+        <v>6.7666944465539336</v>
       </c>
       <c r="C34">
         <v>15.000000594158781</v>
       </c>
       <c r="D34">
-        <v>0.29191325577917121</v>
+        <v>0.29191325577917099</v>
       </c>
       <c r="E34">
-        <v>0.3048504408104703</v>
+        <v>0.30485044074821038</v>
       </c>
       <c r="F34">
         <v>7.4992409326593661</v>
@@ -22192,22 +22191,22 @@
         <v>95</v>
       </c>
       <c r="H34">
-        <v>1.630599159655282</v>
+        <v>1.6305991592715059</v>
       </c>
       <c r="I34">
-        <v>0.38901065683137809</v>
+        <v>0.38901065673982099</v>
       </c>
       <c r="J34">
-        <v>19.9470355746022</v>
+        <v>19.947035570528399</v>
       </c>
       <c r="K34">
-        <v>3.9525695111274288E-2</v>
+        <v>3.9525695103201919E-2</v>
       </c>
       <c r="L34">
-        <v>40.894632425681678</v>
+        <v>40.89463241497895</v>
       </c>
       <c r="M34">
-        <v>8.103403470153786E-2</v>
+        <v>8.1034034680330061E-2</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
@@ -22215,16 +22214,16 @@
         <v>12.84800294997107</v>
       </c>
       <c r="B35">
-        <v>7.9895900077556758</v>
+        <v>7.9895900094700147</v>
       </c>
       <c r="C35">
-        <v>15.000000101786091</v>
+        <v>15.0000001017861</v>
       </c>
       <c r="D35">
         <v>0.25357249983373609</v>
       </c>
       <c r="E35">
-        <v>0.2648104764732066</v>
+        <v>0.26481047641912431</v>
       </c>
       <c r="F35">
         <v>7.4992409326593661</v>
@@ -22233,22 +22232,22 @@
         <v>95</v>
       </c>
       <c r="H35">
-        <v>1.518234459274207</v>
+        <v>1.518234458934443</v>
       </c>
       <c r="I35">
-        <v>0.32975042361783879</v>
+        <v>0.32975042354404421</v>
       </c>
       <c r="J35">
-        <v>19.947034919843858</v>
+        <v>19.947034915770072</v>
       </c>
       <c r="K35">
-        <v>3.5984190326227627E-2</v>
+        <v>3.5984190318878569E-2</v>
       </c>
       <c r="L35">
-        <v>37.295728575121572</v>
+        <v>37.29572856566152</v>
       </c>
       <c r="M35">
-        <v>6.7281006966473308E-2</v>
+        <v>6.7281006949407501E-2</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
@@ -22256,16 +22255,16 @@
         <v>13.465191812781629</v>
       </c>
       <c r="B36">
-        <v>9.1242926738852752</v>
+        <v>9.1242926754036215</v>
       </c>
       <c r="C36">
-        <v>14.9999463245573</v>
+        <v>14.99994632455714</v>
       </c>
       <c r="D36">
-        <v>0.22027735094548401</v>
+        <v>0.22027735094548159</v>
       </c>
       <c r="E36">
-        <v>0.23003973340317541</v>
+        <v>0.23003973335619171</v>
       </c>
       <c r="F36">
         <v>7.4992409326593661</v>
@@ -22274,22 +22273,22 @@
         <v>95</v>
       </c>
       <c r="H36">
-        <v>1.42306735278828</v>
+        <v>1.4230673524810069</v>
       </c>
       <c r="I36">
-        <v>0.28139614260604701</v>
+        <v>0.28139614254528711</v>
       </c>
       <c r="J36">
-        <v>19.946963406760311</v>
+        <v>19.946963402686301</v>
       </c>
       <c r="K36">
-        <v>3.2760939274644719E-2</v>
+        <v>3.2760939267953558E-2</v>
       </c>
       <c r="L36">
-        <v>34.164972218352709</v>
+        <v>34.164972209807523</v>
       </c>
       <c r="M36">
-        <v>5.6112630145300137E-2</v>
+        <v>5.6112630131265481E-2</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
@@ -22297,16 +22296,16 @@
         <v>14.10904660992588</v>
       </c>
       <c r="B37">
-        <v>10.20005087631286</v>
+        <v>10.20005087767966</v>
       </c>
       <c r="C37">
-        <v>15.000081038243261</v>
+        <v>15.00008103824322</v>
       </c>
       <c r="D37">
-        <v>0.1914777757122921</v>
+        <v>0.1914777757122916</v>
       </c>
       <c r="E37">
-        <v>0.19996380149128401</v>
+        <v>0.19996380145044479</v>
       </c>
       <c r="F37">
         <v>7.4992409326593661</v>
@@ -22315,22 +22314,22 @@
         <v>95</v>
       </c>
       <c r="H37">
-        <v>1.3405031021925911</v>
+        <v>1.3405031019109841</v>
       </c>
       <c r="I37">
-        <v>0.24142945837780161</v>
+        <v>0.2414294583270831</v>
       </c>
       <c r="J37">
-        <v>19.947142549332291</v>
+        <v>19.947142545258419</v>
       </c>
       <c r="K37">
-        <v>2.9839393897744031E-2</v>
+        <v>2.983939389164984E-2</v>
       </c>
       <c r="L37">
-        <v>31.374101396643301</v>
+        <v>31.374101388818211</v>
       </c>
       <c r="M37">
-        <v>4.6933247077714318E-2</v>
+        <v>4.6933247066008578E-2</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
@@ -22338,16 +22337,16 @@
         <v>14.77807889101415</v>
       </c>
       <c r="B38">
-        <v>11.233709872066919</v>
+        <v>11.233709873311369</v>
       </c>
       <c r="C38">
-        <v>15.00005146443911</v>
+        <v>15.0000514644391</v>
       </c>
       <c r="D38">
-        <v>0.1666312991036781</v>
+        <v>0.16663129910367799</v>
       </c>
       <c r="E38">
-        <v>0.17401616397648409</v>
+        <v>0.17401616394094449</v>
       </c>
       <c r="F38">
         <v>7.4992409326593661</v>
@@ -22356,22 +22355,22 @@
         <v>95</v>
       </c>
       <c r="H38">
-        <v>1.26774475439473</v>
+        <v>1.267744754134241</v>
       </c>
       <c r="I38">
-        <v>0.2081199121929288</v>
+        <v>0.20811991215016551</v>
       </c>
       <c r="J38">
-        <v>19.947103222018949</v>
+        <v>19.94710321794512</v>
       </c>
       <c r="K38">
-        <v>2.7198723135732999E-2</v>
+        <v>2.7198723130178171E-2</v>
       </c>
       <c r="L38">
-        <v>28.845911417204611</v>
+        <v>28.845911409970132</v>
       </c>
       <c r="M38">
-        <v>3.9332626371951833E-2</v>
+        <v>3.9332626362087307E-2</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
@@ -22379,16 +22378,16 @@
         <v>15.470742000862851</v>
       </c>
       <c r="B39">
-        <v>12.235488524365429</v>
+        <v>12.23548852550794</v>
       </c>
       <c r="C39">
-        <v>15.00003481275845</v>
+        <v>15.00003481275844</v>
       </c>
       <c r="D39">
-        <v>0.14523677913726091</v>
+        <v>0.1452367791372608</v>
       </c>
       <c r="E39">
-        <v>0.1516734689684005</v>
+        <v>0.15167346893742409</v>
       </c>
       <c r="F39">
         <v>7.4992409326593661</v>
@@ -22397,22 +22396,22 @@
         <v>95</v>
       </c>
       <c r="H39">
-        <v>1.2029903600092799</v>
+        <v>1.2029903597666629</v>
       </c>
       <c r="I39">
-        <v>0.18020118103363869</v>
+        <v>0.1802011809972961</v>
       </c>
       <c r="J39">
-        <v>19.94708107857539</v>
+        <v>19.947081074501568</v>
       </c>
       <c r="K39">
-        <v>2.4817710155743251E-2</v>
+        <v>2.4817710150674709E-2</v>
       </c>
       <c r="L39">
-        <v>26.531022586106729</v>
+        <v>26.531022579371271</v>
       </c>
       <c r="M39">
-        <v>3.300930226752255E-2</v>
+        <v>3.3009302259142448E-2</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
@@ -22420,7 +22419,7 @@
         <v>16.185434655020341</v>
       </c>
       <c r="B40">
-        <v>13.2120723326722</v>
+        <v>13.212072333727919</v>
       </c>
       <c r="C40">
         <v>15.00002476086066</v>
@@ -22429,7 +22428,7 @@
         <v>0.12683428026856211</v>
       </c>
       <c r="E40">
-        <v>0.1324553972259481</v>
+        <v>0.1324553971988966</v>
       </c>
       <c r="F40">
         <v>7.4992409326593661</v>
@@ -22438,22 +22437,22 @@
         <v>95</v>
       </c>
       <c r="H40">
-        <v>1.1449533132837459</v>
+        <v>1.1449533130565619</v>
       </c>
       <c r="I40">
-        <v>0.15669560581603559</v>
+        <v>0.15669560578494379</v>
       </c>
       <c r="J40">
-        <v>19.947067711538399</v>
+        <v>19.947067707464601</v>
       </c>
       <c r="K40">
-        <v>2.267435651684124E-2</v>
+        <v>2.267435651221044E-2</v>
       </c>
       <c r="L40">
-        <v>24.394443661543772</v>
+        <v>24.394443655238671</v>
       </c>
       <c r="M40">
-        <v>2.7729805734397931E-2</v>
+        <v>2.7729805727230761E-2</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
@@ -22461,7 +22460,7 @@
         <v>16.92050464158374</v>
       </c>
       <c r="B41">
-        <v>14.167854713193689</v>
+        <v>14.167854714174419</v>
       </c>
       <c r="C41">
         <v>15.00001806410026</v>
@@ -22470,7 +22469,7 @@
         <v>0.1110119217613116</v>
       </c>
       <c r="E41">
-        <v>0.1159318140377783</v>
+        <v>0.11593181401410139</v>
       </c>
       <c r="F41">
         <v>7.4992409326593661</v>
@@ -22479,22 +22478,22 @@
         <v>95</v>
       </c>
       <c r="H41">
-        <v>1.0926750344444009</v>
+        <v>1.0926750342307421</v>
       </c>
       <c r="I41">
-        <v>0.13683026581560001</v>
+        <v>0.13683026578884461</v>
       </c>
       <c r="J41">
-        <v>19.94705880617089</v>
+        <v>19.9470588020971</v>
       </c>
       <c r="K41">
-        <v>2.0747075515419121E-2</v>
+        <v>2.074707551118193E-2</v>
       </c>
       <c r="L41">
-        <v>22.41059375551141</v>
+        <v>22.410593749582631</v>
       </c>
       <c r="M41">
-        <v>2.330941546365399E-2</v>
+        <v>2.3309415457487419E-2</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
@@ -22502,16 +22501,16 @@
         <v>17.674252640748659</v>
       </c>
       <c r="B42">
-        <v>15.105699726808091</v>
+        <v>15.105699727723261</v>
       </c>
       <c r="C42">
-        <v>15.000013149598161</v>
+        <v>15.000013149598169</v>
       </c>
       <c r="D42">
-        <v>9.7406118347547477E-2</v>
+        <v>9.7406118347547518E-2</v>
       </c>
       <c r="E42">
-        <v>0.10172302054809761</v>
+        <v>0.1017230205273226</v>
       </c>
       <c r="F42">
         <v>7.4992409326593661</v>
@@ -22520,22 +22519,22 @@
         <v>95</v>
       </c>
       <c r="H42">
-        <v>1.045410488371306</v>
+        <v>1.045410488169632</v>
       </c>
       <c r="I42">
-        <v>0.11998377139345399</v>
+        <v>0.1199837713703075</v>
       </c>
       <c r="J42">
-        <v>19.947052270854609</v>
+        <v>19.947052266780819</v>
       </c>
       <c r="K42">
-        <v>1.9015215470206012E-2</v>
+        <v>1.9015215466322531E-2</v>
       </c>
       <c r="L42">
-        <v>20.560163029984651</v>
+        <v>20.56016302438848</v>
       </c>
       <c r="M42">
-        <v>1.9599684445052681E-2</v>
+        <v>1.9599684439717938E-2</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
@@ -22543,16 +22542,16 @@
         <v>18.44493615326207</v>
       </c>
       <c r="B43">
-        <v>16.027446219282439</v>
+        <v>16.027446220139769</v>
       </c>
       <c r="C43">
-        <v>15.00000922553669</v>
+        <v>15.000009225536671</v>
       </c>
       <c r="D43">
-        <v>8.5699409690751072E-2</v>
+        <v>8.5699409690750947E-2</v>
       </c>
       <c r="E43">
-        <v>8.9497487024659747E-2</v>
+        <v>8.9497487006381493E-2</v>
       </c>
       <c r="F43">
         <v>7.4992409326593661</v>
@@ -22561,22 +22560,22 @@
         <v>95</v>
       </c>
       <c r="H43">
-        <v>1.0025613467142489</v>
+        <v>1.0025613465232861</v>
       </c>
       <c r="I43">
-        <v>0.1056511958510805</v>
+        <v>0.1056511958309565</v>
       </c>
       <c r="J43">
-        <v>19.947047052628559</v>
+        <v>19.94704704855473</v>
       </c>
       <c r="K43">
-        <v>1.7459385011976549E-2</v>
+        <v>1.745938500841078E-2</v>
       </c>
       <c r="L43">
-        <v>18.82803369135268</v>
+        <v>18.828033686052841</v>
       </c>
       <c r="M43">
-        <v>1.6479927498465191E-2</v>
+        <v>1.6479927493826318E-2</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
@@ -22584,16 +22583,16 @@
         <v>19.230773528696592</v>
       </c>
       <c r="B44">
-        <v>16.934227657476249</v>
+        <v>16.93422765828214</v>
       </c>
       <c r="C44">
-        <v>15.000005999146349</v>
+        <v>15.00000599914636</v>
       </c>
       <c r="D44">
-        <v>7.5616913329235619E-2</v>
+        <v>7.5616913329235688E-2</v>
       </c>
       <c r="E44">
-        <v>7.8968148601593652E-2</v>
+        <v>7.8968148585466011E-2</v>
       </c>
       <c r="F44">
         <v>7.4992409326593661</v>
@@ -22602,22 +22601,22 @@
         <v>95</v>
       </c>
       <c r="H44">
-        <v>0.96363490767920457</v>
+        <v>0.96363490749788072</v>
       </c>
       <c r="I44">
-        <v>9.3419339022496176E-2</v>
+        <v>9.3419339004917779E-2</v>
       </c>
       <c r="J44">
-        <v>19.9470427621672</v>
+        <v>19.947042758093421</v>
       </c>
       <c r="K44">
-        <v>1.6061631375198591E-2</v>
+        <v>1.6061631371918329E-2</v>
       </c>
       <c r="L44">
-        <v>17.20197892728374</v>
+        <v>17.201978922250049</v>
       </c>
       <c r="M44">
-        <v>1.3851268468627239E-2</v>
+        <v>1.385126846457403E-2</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
@@ -22625,16 +22624,16 @@
         <v>20.029948084233538</v>
       </c>
       <c r="B45">
-        <v>17.826682046869589</v>
+        <v>17.82668204762939</v>
       </c>
       <c r="C45">
-        <v>15.00000340862116</v>
+        <v>15.000003408621151</v>
       </c>
       <c r="D45">
-        <v>6.6922115306813426E-2</v>
+        <v>6.6922115306813384E-2</v>
       </c>
       <c r="E45">
-        <v>6.9888009356740152E-2</v>
+        <v>6.9888009342466834E-2</v>
       </c>
       <c r="F45">
         <v>7.4992409326593661</v>
@@ -22643,22 +22642,22 @@
         <v>95</v>
       </c>
       <c r="H45">
-        <v>0.92821751087275106</v>
+        <v>0.92821751070014535</v>
       </c>
       <c r="I45">
-        <v>8.2948375104646491E-2</v>
+        <v>8.2948375089221912E-2</v>
       </c>
       <c r="J45">
-        <v>19.947039317280801</v>
+        <v>19.947039313207</v>
       </c>
       <c r="K45">
-        <v>1.48055122821068E-2</v>
+        <v>1.480551227908306E-2</v>
       </c>
       <c r="L45">
-        <v>15.67182090319651</v>
+        <v>15.67182089840319</v>
       </c>
       <c r="M45">
-        <v>1.163226948995078E-2</v>
+        <v>1.163226948639298E-2</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
@@ -22666,16 +22665,16 @@
         <v>20.8406123044333</v>
       </c>
       <c r="B46">
-        <v>18.70508212857678</v>
+        <v>18.705082129295029</v>
       </c>
       <c r="C46">
-        <v>15.00000149044844</v>
+        <v>15.00000149044843</v>
       </c>
       <c r="D46">
-        <v>5.9412475974512727E-2</v>
+        <v>5.9412475974512699E-2</v>
       </c>
       <c r="E46">
-        <v>6.2045553368679937E-2</v>
+        <v>6.2045553356008303E-2</v>
       </c>
       <c r="F46">
         <v>7.4992409326593661</v>
@@ -22684,22 +22683,22 @@
         <v>95</v>
       </c>
       <c r="H46">
-        <v>0.89595601825221005</v>
+        <v>0.89595601808752534</v>
       </c>
       <c r="I46">
-        <v>7.3957720162785262E-2</v>
+        <v>7.3957720149191178E-2</v>
       </c>
       <c r="J46">
-        <v>19.947036766490271</v>
+        <v>19.94703676241646</v>
       </c>
       <c r="K46">
-        <v>1.3676094138862021E-2</v>
+        <v>1.3676094136068941E-2</v>
       </c>
       <c r="L46">
-        <v>14.22892793557954</v>
+        <v>14.2289279310046</v>
       </c>
       <c r="M46">
-        <v>9.7556424154678668E-3</v>
+        <v>9.7556424123311954E-3</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
@@ -22707,16 +22706,16 @@
         <v>21.660892112283761</v>
       </c>
       <c r="B47">
-        <v>19.56943767886381</v>
+        <v>19.569437679544389</v>
       </c>
       <c r="C47">
-        <v>15.000000329816</v>
+        <v>15.000000329815981</v>
       </c>
       <c r="D47">
-        <v>5.2915149072103318E-2</v>
+        <v>5.2915149072103262E-2</v>
       </c>
       <c r="E47">
-        <v>5.5260274073971848E-2</v>
+        <v>5.5260274062685938E-2</v>
       </c>
       <c r="F47">
         <v>7.4992409326593661</v>
@@ -22725,22 +22724,22 @@
         <v>95</v>
       </c>
       <c r="H47">
-        <v>0.86654489405268631</v>
+        <v>0.86654489389522416</v>
       </c>
       <c r="I47">
-        <v>6.6214966277235304E-2</v>
+        <v>6.6214966265203207E-2</v>
       </c>
       <c r="J47">
-        <v>19.947035223078551</v>
+        <v>19.947035219004739</v>
       </c>
       <c r="K47">
-        <v>1.26599012634953E-2</v>
+        <v>1.265990126090975E-2</v>
       </c>
       <c r="L47">
-        <v>12.86583720230151</v>
+        <v>12.865837197925909</v>
       </c>
       <c r="M47">
-        <v>8.1656359870909846E-3</v>
+        <v>8.1656359843138952E-3</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
@@ -22748,16 +22747,16 @@
         <v>22.48889120165342</v>
       </c>
       <c r="B48">
-        <v>20.4195090525361</v>
+        <v>20.419509053181802</v>
       </c>
       <c r="C48">
-        <v>15.000182163757639</v>
+        <v>15.000182163760419</v>
       </c>
       <c r="D48">
-        <v>4.7283560956950077E-2</v>
+        <v>4.7283560956958862E-2</v>
       </c>
       <c r="E48">
-        <v>4.9379101892239187E-2</v>
+        <v>4.9379101882163642E-2</v>
       </c>
       <c r="F48">
         <v>7.4992409326593661</v>
@@ -22766,22 +22765,22 @@
         <v>95</v>
       </c>
       <c r="H48">
-        <v>0.83972535375295065</v>
+        <v>0.83972535360223077</v>
       </c>
       <c r="I48">
-        <v>5.9527679366853131E-2</v>
+        <v>5.9527679356168678E-2</v>
       </c>
       <c r="J48">
-        <v>19.94727702627582</v>
+        <v>19.947277022205679</v>
       </c>
       <c r="K48">
-        <v>1.1744977114401429E-2</v>
+        <v>1.1744977112004919E-2</v>
       </c>
       <c r="L48">
-        <v>11.57634071085012</v>
+        <v>11.57634070666092</v>
       </c>
       <c r="M48">
-        <v>6.8161612503976352E-3</v>
+        <v>6.8161612479310301E-3</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.2">
@@ -22789,16 +22788,16 @@
         <v>23.32269542113314</v>
       </c>
       <c r="B49">
-        <v>21.255044545607571</v>
+        <v>21.255044546222539</v>
       </c>
       <c r="C49">
-        <v>15.00000053757749</v>
+        <v>15.00000053757752</v>
       </c>
       <c r="D49">
-        <v>4.2390918387633009E-2</v>
+        <v>4.2390918387633113E-2</v>
       </c>
       <c r="E49">
-        <v>4.4269624283888649E-2</v>
+        <v>4.4269624274847527E-2</v>
       </c>
       <c r="F49">
         <v>7.4992409326593661</v>
@@ -22807,22 +22806,22 @@
         <v>95</v>
       </c>
       <c r="H49">
-        <v>0.81523326246602013</v>
+        <v>0.81523326232122839</v>
       </c>
       <c r="I49">
-        <v>5.3733135369483452E-2</v>
+        <v>5.3733135359940017E-2</v>
       </c>
       <c r="J49">
-        <v>19.947035499360268</v>
+        <v>19.947035495286521</v>
       </c>
       <c r="K49">
-        <v>1.092007249757369E-2</v>
+        <v>1.09200724953435E-2</v>
       </c>
       <c r="L49">
-        <v>10.354113230884581</v>
+        <v>10.35411322685956</v>
       </c>
       <c r="M49">
-        <v>5.6683945407814016E-3</v>
+        <v>5.6683945385778874E-3</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.2">
@@ -22830,7 +22829,7 @@
         <v>24.160377199132409</v>
       </c>
       <c r="B50">
-        <v>22.075446991592649</v>
+        <v>22.075446992178989</v>
       </c>
       <c r="C50">
         <v>15.000001767071931</v>
@@ -22839,7 +22838,7 @@
         <v>3.8132734730036089E-2</v>
       </c>
       <c r="E50">
-        <v>3.9822723914100827E-2</v>
+        <v>3.9822723905967812E-2</v>
       </c>
       <c r="F50">
         <v>7.4992409326593661</v>
@@ -22848,22 +22847,22 @@
         <v>95</v>
       </c>
       <c r="H50">
-        <v>0.79288418988468379</v>
+        <v>0.7928841897454646</v>
       </c>
       <c r="I50">
-        <v>4.8699007528501301E-2</v>
+        <v>4.8699007519950453E-2</v>
       </c>
       <c r="J50">
-        <v>19.947037134344821</v>
+        <v>19.947037130271031</v>
       </c>
       <c r="K50">
-        <v>1.0175965314665889E-2</v>
+        <v>1.0175965312587651E-2</v>
       </c>
       <c r="L50">
-        <v>9.1951300371327402</v>
+        <v>9.1951300332624477</v>
       </c>
       <c r="M50">
-        <v>4.6908883605875241E-3</v>
+        <v>4.6908883586130974E-3</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.2">
@@ -22871,16 +22870,16 @@
         <v>25</v>
       </c>
       <c r="B51">
-        <v>22.880181345473659</v>
+        <v>22.88018134603378</v>
       </c>
       <c r="C51">
-        <v>15.0000034984956</v>
+        <v>15.000003498495611</v>
       </c>
       <c r="D51">
-        <v>3.4418275567828963E-2</v>
+        <v>3.4418275567828983E-2</v>
       </c>
       <c r="E51">
-        <v>3.5943645144797018E-2</v>
+        <v>3.5943645137456251E-2</v>
       </c>
       <c r="F51">
         <v>7.4992409326593661</v>
@@ -22889,22 +22888,22 @@
         <v>95</v>
       </c>
       <c r="H51">
-        <v>0.77248028934950941</v>
+        <v>0.77248028921542633</v>
       </c>
       <c r="I51">
-        <v>4.4312388780799621E-2</v>
+        <v>4.4312388773108113E-2</v>
       </c>
       <c r="J51">
-        <v>19.94703943679604</v>
+        <v>19.94703943272226</v>
       </c>
       <c r="K51">
-        <v>9.5039265543569763E-3</v>
+        <v>9.5039265524159908E-3</v>
       </c>
       <c r="L51">
-        <v>8.0950781270078576</v>
+        <v>8.0950781232805724</v>
       </c>
       <c r="M51">
-        <v>3.856964749813614E-3</v>
+        <v>3.8569647480377191E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding rotor performance caveat per discussion
</commit_message>
<xml_diff>
--- a/Documentation/IEA-15-240-RWT_tabular.xlsx
+++ b/Documentation/IEA-15-240-RWT_tabular.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gbarter/devel/IEA-15-240-RWT/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D41ECA8-11BF-D44F-8DD0-092068BF77D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67344A13-61F3-EA43-B984-FF6C76BB440D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17260" yWindow="500" windowWidth="33940" windowHeight="26840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="286">
   <si>
     <t>Parameter</t>
   </si>
@@ -907,6 +907,9 @@
   <si>
     <t>Floating Tower mass [t]</t>
   </si>
+  <si>
+    <t>NOTE: This data is auto-generated from WISDEM, which uses idealized steady-state conditions and maximizes the power production at each velocity subject to constraints on min or max rpm, torque, etc.  See the GitHub FAQ for additional comments</t>
+  </si>
 </sst>
 </file>
 
@@ -20793,10 +20796,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <dimension ref="A1:M51"/>
+  <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H55" sqref="H55"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -22904,6 +22907,11 @@
       </c>
       <c r="M51">
         <v>3.8569647480377191E-3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>285</v>
       </c>
     </row>
   </sheetData>

</xml_diff>